<commit_message>
guest user checkout tetscase for drybar emea
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="278">
   <si>
     <t>UserName</t>
   </si>
@@ -1246,7 +1246,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1256,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -1450,6 +1450,9 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
+      <c r="AJ2" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="3" spans="1:39">
       <c r="A3" t="s">
@@ -1459,6 +1462,9 @@
       <c r="E3" s="2"/>
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
+      <c r="AJ3" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="4" spans="1:39">
       <c r="A4" t="s">
@@ -1468,6 +1474,9 @@
       <c r="E4" s="2"/>
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
+      <c r="AJ4" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="5" spans="1:39">
       <c r="A5" t="s">
@@ -1480,6 +1489,9 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
+      <c r="AJ5" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="6" spans="1:39">
       <c r="A6" t="s">
@@ -1513,6 +1525,9 @@
         <v>161</v>
       </c>
       <c r="Z7" s="5"/>
+      <c r="AJ7" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="8" spans="1:39">
       <c r="A8" t="s">
@@ -1586,6 +1601,9 @@
       <c r="W10">
         <v>123</v>
       </c>
+      <c r="AJ10" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="11" spans="1:39">
       <c r="A11" t="s">
@@ -1602,6 +1620,9 @@
       <c r="W11">
         <v>123</v>
       </c>
+      <c r="AJ11" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="12" spans="1:39">
       <c r="A12" t="s">
@@ -1616,6 +1637,9 @@
       <c r="W12">
         <v>123</v>
       </c>
+      <c r="AJ12" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="13" spans="1:39">
       <c r="A13" t="s">
@@ -1624,6 +1648,9 @@
       <c r="U13" s="5"/>
       <c r="V13" s="6"/>
       <c r="W13" s="5"/>
+      <c r="AJ13" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="14" spans="1:39">
       <c r="A14" t="s">
@@ -1631,6 +1658,9 @@
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
+      <c r="AJ14" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="15" spans="1:39">
       <c r="A15" t="s">
@@ -1651,6 +1681,9 @@
       <c r="W15">
         <v>123</v>
       </c>
+      <c r="AJ15" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="16" spans="1:39">
       <c r="A16" t="s">
@@ -1658,6 +1691,9 @@
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
+      <c r="AJ16" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="17" spans="1:38">
       <c r="A17" t="s">
@@ -1690,6 +1726,9 @@
       <c r="S17">
         <v>9898989898</v>
       </c>
+      <c r="AJ17" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="18" spans="1:38">
       <c r="A18" t="s">
@@ -1722,6 +1761,9 @@
       <c r="S18">
         <v>9898989898</v>
       </c>
+      <c r="AJ18" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="19" spans="1:38">
       <c r="A19" t="s">
@@ -1754,6 +1796,9 @@
       <c r="S19">
         <v>9898989898</v>
       </c>
+      <c r="AJ19" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="20" spans="1:38">
       <c r="A20" t="s">
@@ -1785,6 +1830,9 @@
       </c>
       <c r="S20">
         <v>9898986598</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -1808,6 +1856,9 @@
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
+      <c r="AJ21" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="22" spans="1:38">
       <c r="A22" t="s">
@@ -1855,6 +1906,9 @@
       <c r="S23">
         <v>9898989898</v>
       </c>
+      <c r="AJ23" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="24" spans="1:38">
       <c r="A24" t="s">
@@ -1883,6 +1937,9 @@
       </c>
       <c r="S24">
         <v>9898989898</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:38">
@@ -1910,6 +1967,9 @@
       <c r="W25" s="2"/>
       <c r="AE25" s="5"/>
       <c r="AF25" s="5"/>
+      <c r="AJ25" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="26" spans="1:38">
       <c r="A26" t="s">
@@ -1960,6 +2020,9 @@
       <c r="S27" s="9">
         <v>9898989898</v>
       </c>
+      <c r="AJ27" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="28" spans="1:38">
       <c r="A28" t="s">
@@ -1970,6 +2033,9 @@
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
+      <c r="AJ28" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="29" spans="1:38">
       <c r="A29" t="s">
@@ -1978,6 +2044,9 @@
       <c r="M29" t="s">
         <v>107</v>
       </c>
+      <c r="AJ29" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="30" spans="1:38">
       <c r="A30" t="s">
@@ -1992,6 +2061,9 @@
       <c r="W30" s="5" t="s">
         <v>113</v>
       </c>
+      <c r="AJ30" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="31" spans="1:38">
       <c r="A31" t="s">
@@ -2000,6 +2072,9 @@
       <c r="M31" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="AJ31" t="s">
+        <v>269</v>
+      </c>
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
@@ -2021,6 +2096,9 @@
       <c r="A33" t="s">
         <v>159</v>
       </c>
+      <c r="AJ33" t="s">
+        <v>269</v>
+      </c>
       <c r="AK33" s="7" t="s">
         <v>157</v>
       </c>
@@ -2034,6 +2112,9 @@
       </c>
       <c r="M34" t="s">
         <v>163</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:39">

</xml_diff>

<commit_message>
Drybay uk testcases changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1256,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -3479,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI18"/>
+  <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3625,19 +3625,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>270</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>271</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>273</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>60</v>
+        <v>272</v>
+      </c>
+      <c r="R2" t="s">
+        <v>274</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -3659,7 +3659,7 @@
         <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>277</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="4"/>
@@ -3724,19 +3724,19 @@
         <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>81</v>
+        <v>214</v>
       </c>
       <c r="O9" t="s">
-        <v>82</v>
+        <v>215</v>
       </c>
       <c r="P9" t="s">
         <v>52</v>
       </c>
       <c r="Q9" t="s">
-        <v>83</v>
+        <v>216</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
       <c r="S9">
         <v>9898989898</v>
@@ -3756,19 +3756,19 @@
         <v>46</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>270</v>
       </c>
       <c r="O10" t="s">
-        <v>58</v>
+        <v>271</v>
       </c>
       <c r="P10" t="s">
-        <v>52</v>
+        <v>273</v>
       </c>
       <c r="Q10" t="s">
-        <v>59</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>60</v>
+        <v>272</v>
+      </c>
+      <c r="R10" t="s">
+        <v>274</v>
       </c>
       <c r="S10">
         <v>9898989898</v>
@@ -3817,19 +3817,19 @@
         <v>80</v>
       </c>
       <c r="N13" t="s">
-        <v>81</v>
+        <v>214</v>
       </c>
       <c r="O13" t="s">
-        <v>82</v>
+        <v>215</v>
       </c>
       <c r="P13" t="s">
         <v>52</v>
       </c>
       <c r="Q13" t="s">
-        <v>83</v>
+        <v>216</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
       <c r="S13">
         <v>9898989898</v>
@@ -3899,6 +3899,10 @@
       <c r="AI18" t="s">
         <v>201</v>
       </c>
+    </row>
+    <row r="22" spans="1:35">
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Drybar uk testcases changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F84614-7FF3-4EFA-B3C5-F694E7CE0BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -19,8 +18,8 @@
     <sheet name="Outofstock" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="272">
   <si>
     <t>UserName</t>
   </si>
@@ -639,21 +638,6 @@
     <t>Account Links</t>
   </si>
   <si>
-    <t>Non-Po_Box_Hawai</t>
-  </si>
-  <si>
-    <t>46008</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>2, dream Valley</t>
-  </si>
-  <si>
     <t>Notifyme</t>
   </si>
   <si>
@@ -723,12 +707,6 @@
     <t>The Double Shot Oval Blow-Dryer Brush</t>
   </si>
   <si>
-    <t>Non_POBox_Alaska</t>
-  </si>
-  <si>
-    <t>vnarra@helenoftroy.com</t>
-  </si>
-  <si>
     <t>Travel_SizeProduct</t>
   </si>
   <si>
@@ -862,16 +840,19 @@
   </si>
   <si>
     <t>Delivery</t>
+  </si>
+  <si>
+    <t>SUPER LEMON DROP BRUSH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1247,47 +1228,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:U48"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="16" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>97</v>
@@ -1402,11 +1383,11 @@
       <c r="AL1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AM1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM1" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1432,19 +1413,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="O2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Q2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -1452,10 +1433,10 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AJ2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1464,10 +1445,10 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AJ3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1476,25 +1457,25 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AJ4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AJ5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1510,10 +1491,10 @@
         <v>4</v>
       </c>
       <c r="AJ6" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1527,10 +1508,10 @@
       </c>
       <c r="Z7" s="5"/>
       <c r="AJ7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1547,23 +1528,23 @@
         <v>153</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="L8" s="2"/>
       <c r="N8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="O8" t="s">
         <v>58</v>
       </c>
       <c r="P8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Q8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R8" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>154</v>
@@ -1572,10 +1553,10 @@
         <v>166</v>
       </c>
       <c r="AJ8" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1586,10 +1567,10 @@
       </c>
       <c r="Z9" s="5"/>
       <c r="AJ9" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1603,10 +1584,10 @@
         <v>123</v>
       </c>
       <c r="AJ10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1622,10 +1603,10 @@
         <v>123</v>
       </c>
       <c r="AJ11" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1639,10 +1620,10 @@
         <v>123</v>
       </c>
       <c r="AJ12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1650,20 +1631,20 @@
       <c r="V13" s="6"/>
       <c r="W13" s="5"/>
       <c r="AJ13" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="AJ14" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1683,20 +1664,20 @@
         <v>123</v>
       </c>
       <c r="AJ15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="AJ16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1728,10 +1709,10 @@
         <v>9898989898</v>
       </c>
       <c r="AJ17" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1745,511 +1726,475 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="O18" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P18" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Q18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R18" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="S18">
         <v>9898989898</v>
       </c>
       <c r="AJ18" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="F19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AJ19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z20" s="5"/>
+      <c r="AJ20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="G21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N19" t="s">
-        <v>151</v>
-      </c>
-      <c r="O19" t="s">
-        <v>150</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="N21" t="s">
+        <v>74</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21" t="s">
         <v>52</v>
       </c>
-      <c r="Q19" t="s">
-        <v>148</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="S19">
+      <c r="Q21" t="s">
+        <v>76</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="S21">
         <v>9898989898</v>
       </c>
-      <c r="V19" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF19" s="8" t="s">
+      <c r="AJ21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="N22" t="s">
+        <v>81</v>
+      </c>
+      <c r="O22" t="s">
+        <v>82</v>
+      </c>
+      <c r="P22" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>83</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S22">
+        <v>9898989898</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="K23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M23" t="s">
+        <v>88</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="2"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AJ23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="X24" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z24" s="5"/>
+      <c r="AA24" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AI19" t="s">
-        <v>207</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>205</v>
-      </c>
-      <c r="AK19" t="s">
+      <c r="N25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P25" t="s">
         <v>52</v>
       </c>
-      <c r="AL19" t="s">
-        <v>206</v>
-      </c>
-      <c r="AM19" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="AN19">
+      <c r="Q25" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="S25" s="9">
         <v>9898989898</v>
       </c>
-      <c r="BE19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>231</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="N20" t="s">
-        <v>207</v>
-      </c>
-      <c r="O20" t="s">
-        <v>205</v>
-      </c>
-      <c r="P20" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>205</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="S20">
-        <v>9898986598</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" t="s">
-        <v>65</v>
-      </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AJ21" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y22" s="5" t="s">
+      <c r="AJ25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="M26" t="s">
+        <v>270</v>
+      </c>
+      <c r="R26" s="10"/>
+      <c r="S26" s="9"/>
+      <c r="AJ26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="M27" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK29" s="7"/>
+      <c r="AL29" s="7"/>
+    </row>
+    <row r="30" spans="1:38">
+      <c r="A30" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38">
+      <c r="A31" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK31" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL31" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38">
+      <c r="A32" t="s">
+        <v>162</v>
+      </c>
+      <c r="M32" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="X33" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y33" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z22" s="5"/>
-      <c r="AJ22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" t="s">
-        <v>78</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N23" t="s">
-        <v>74</v>
-      </c>
-      <c r="O23" t="s">
-        <v>75</v>
-      </c>
-      <c r="P23" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>76</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="S23">
-        <v>9898989898</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="1:39">
+      <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" t="s">
         <v>79</v>
       </c>
-      <c r="G24" t="s">
-        <v>80</v>
-      </c>
-      <c r="N24" t="s">
-        <v>81</v>
-      </c>
-      <c r="O24" t="s">
-        <v>82</v>
-      </c>
-      <c r="P24" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>83</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S24">
-        <v>9898989898</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="7"/>
-      <c r="K25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M25" t="s">
-        <v>88</v>
-      </c>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="2"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AJ25" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>95</v>
-      </c>
-      <c r="X26" t="s">
+      <c r="G34" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" t="s">
+        <v>175</v>
+      </c>
+      <c r="X35" t="s">
         <v>96</v>
-      </c>
-      <c r="Y26" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z26" s="5"/>
-      <c r="AA26" t="s">
-        <v>98</v>
-      </c>
-      <c r="AJ26" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" t="s">
-        <v>80</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N27" t="s">
-        <v>100</v>
-      </c>
-      <c r="O27" t="s">
-        <v>101</v>
-      </c>
-      <c r="P27" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>102</v>
-      </c>
-      <c r="R27" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="S27" s="9">
-        <v>9898989898</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>105</v>
-      </c>
-      <c r="M28" t="s">
-        <v>277</v>
-      </c>
-      <c r="R28" s="10"/>
-      <c r="S28" s="9"/>
-      <c r="AJ28" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>106</v>
-      </c>
-      <c r="M29" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ29" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>110</v>
-      </c>
-      <c r="U30" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V30" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="W30" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ30" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>114</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ31" t="s">
-        <v>269</v>
-      </c>
-      <c r="AK31" s="7"/>
-      <c r="AL31" s="7"/>
-    </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>145</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>145</v>
-      </c>
-      <c r="AJ32" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>159</v>
-      </c>
-      <c r="AJ33" t="s">
-        <v>269</v>
-      </c>
-      <c r="AK33" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AL33" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>162</v>
-      </c>
-      <c r="M34" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ34" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>164</v>
-      </c>
-      <c r="X35" t="s">
-        <v>165</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z35" s="5"/>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AA35" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
-        <v>167</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F36" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36" t="s">
+        <v>177</v>
+      </c>
+      <c r="I36" t="s">
+        <v>178</v>
+      </c>
+      <c r="X36" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" t="s">
         <v>79</v>
       </c>
-      <c r="G36" t="s">
-        <v>170</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>175</v>
-      </c>
-      <c r="X37" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AK37" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL37" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
-        <v>176</v>
-      </c>
-      <c r="H38" t="s">
-        <v>177</v>
-      </c>
-      <c r="I38" t="s">
-        <v>178</v>
-      </c>
-      <c r="X38" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y38" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z38" s="5"/>
-      <c r="AA38" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="AK39" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL39" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O39" t="s">
+        <v>82</v>
+      </c>
+      <c r="P39" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>83</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S39">
+        <v>9898989898</v>
+      </c>
+      <c r="T39">
+        <v>888888</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V39" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="W39" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" t="s">
-        <v>184</v>
-      </c>
-      <c r="D40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F41" t="s">
         <v>79</v>
@@ -2257,52 +2202,34 @@
       <c r="G41" t="s">
         <v>80</v>
       </c>
-      <c r="K41" s="8" t="s">
-        <v>187</v>
-      </c>
       <c r="N41" t="s">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="O41" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="P41" t="s">
-        <v>52</v>
+        <v>195</v>
       </c>
       <c r="Q41" t="s">
-        <v>83</v>
-      </c>
-      <c r="R41" s="5" t="s">
-        <v>84</v>
+        <v>196</v>
+      </c>
+      <c r="R41" t="s">
+        <v>197</v>
       </c>
       <c r="S41">
         <v>9898989898</v>
       </c>
-      <c r="T41">
-        <v>888888</v>
-      </c>
-      <c r="U41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V41" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="W41" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="AJ41" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>190</v>
+    </row>
+    <row r="42" spans="1:39">
+      <c r="A42" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>169</v>
@@ -2310,204 +2237,155 @@
       <c r="E42" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>192</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="F42" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G43" t="s">
-        <v>80</v>
-      </c>
-      <c r="N43" t="s">
-        <v>193</v>
-      </c>
-      <c r="O43" t="s">
-        <v>194</v>
-      </c>
-      <c r="P43" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>196</v>
-      </c>
-      <c r="R43" t="s">
-        <v>197</v>
-      </c>
-      <c r="S43">
-        <v>9898989898</v>
-      </c>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="G42" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+    </row>
+    <row r="43" spans="1:39">
+      <c r="A43" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="M43" s="9"/>
+    </row>
+    <row r="44" spans="1:39">
       <c r="A44" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-    </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="X44" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="AM45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
+      </c>
+      <c r="K46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L45" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="M45" s="9"/>
-    </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="X46" t="s">
-        <v>234</v>
-      </c>
-      <c r="Y46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="AM47" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>147</v>
-      </c>
-      <c r="F48" t="s">
-        <v>47</v>
-      </c>
-      <c r="G48" t="s">
-        <v>48</v>
-      </c>
-      <c r="K48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N48" t="s">
+      <c r="N46" t="s">
         <v>151</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O46" t="s">
         <v>150</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P46" t="s">
         <v>52</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="Q46" t="s">
         <v>148</v>
       </c>
-      <c r="R48" s="10" t="s">
+      <c r="R46" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="S48">
+      <c r="S46">
         <v>9898989898</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K23" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K27" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D36" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E36" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B42" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D42" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E42" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C42" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="AF19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E8" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B44" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C44" r:id="rId24" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D44" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E44" r:id="rId26" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="K44" r:id="rId27" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B45" r:id="rId28" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D45" r:id="rId29" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E45" r:id="rId30" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="K45" r:id="rId31" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L45" r:id="rId32" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K20" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="K19" r:id="rId34" xr:uid="{D69C7625-C6FC-4B84-81E9-F39D295D118B}"/>
-    <hyperlink ref="K48" r:id="rId35" xr:uid="{EA022D61-B415-41F8-A2EB-CE12BFC7D6CE}"/>
+    <hyperlink ref="K17" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K25" r:id="rId9"/>
+    <hyperlink ref="B34" r:id="rId10"/>
+    <hyperlink ref="D34" r:id="rId11"/>
+    <hyperlink ref="E34" r:id="rId12"/>
+    <hyperlink ref="K34" r:id="rId13"/>
+    <hyperlink ref="K39" r:id="rId14"/>
+    <hyperlink ref="B40" r:id="rId15"/>
+    <hyperlink ref="D40" r:id="rId16"/>
+    <hyperlink ref="E40" r:id="rId17"/>
+    <hyperlink ref="C40" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="E8" r:id="rId21"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K46" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="25" max="25" width="20.7109375" customWidth="1"/>
-    <col min="26" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.6640625" customWidth="1"/>
+    <col min="26" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2548,10 +2426,10 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>18</v>
@@ -2560,7 +2438,7 @@
         <v>124</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>21</v>
@@ -2569,13 +2447,13 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>11</v>
@@ -2587,16 +2465,16 @@
         <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2622,66 +2500,66 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
         <v>214</v>
-      </c>
-      <c r="J2" t="s">
-        <v>215</v>
-      </c>
-      <c r="K2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>219</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="Q3" t="s">
         <v>98</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AB5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AC5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -2692,39 +2570,39 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2750,25 +2628,25 @@
         <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>65</v>
@@ -2855,7 +2733,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2896,12 +2774,12 @@
         <v>60</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -2909,7 +2787,7 @@
         <v>177</v>
       </c>
       <c r="I3" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="P3" s="2"/>
       <c r="S3" s="2"/>
@@ -2922,68 +2800,68 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="H5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="K5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="AF5" s="3"/>
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H6" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L6" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="M7" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
@@ -2993,22 +2871,22 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H9" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="O9" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3018,39 +2896,39 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3154,7 +3032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3170,27 +3048,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3198,7 +3076,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3212,33 +3090,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3312,7 +3190,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3363,7 +3241,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3415,7 +3293,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3469,7 +3347,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3496,7 +3374,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3511,7 +3389,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3524,38 +3402,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3662,7 +3540,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3690,19 +3568,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="O2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Q2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -3710,7 +3588,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3719,18 +3597,18 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3743,7 +3621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3751,14 +3629,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3778,7 +3656,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -3789,25 +3667,25 @@
         <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="P9" t="s">
         <v>52</v>
       </c>
       <c r="Q9" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="S9">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -3821,25 +3699,25 @@
         <v>46</v>
       </c>
       <c r="N10" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="O10" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Q10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R10" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="S10">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3860,7 +3738,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -3871,7 +3749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -3882,25 +3760,25 @@
         <v>80</v>
       </c>
       <c r="N13" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O13" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="P13" t="s">
         <v>52</v>
       </c>
       <c r="Q13" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="S13">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -3927,7 +3805,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -3941,7 +3819,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -3949,7 +3827,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -3957,7 +3835,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -3965,39 +3843,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4110,7 +3988,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4156,7 +4034,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4165,7 +4043,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4174,7 +4052,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4185,7 +4063,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4198,7 +4076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4211,7 +4089,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4224,7 +4102,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4238,7 +4116,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4254,7 +4132,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4268,14 +4146,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4295,14 +4173,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4334,7 +4212,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4366,7 +4244,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4387,7 +4265,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4398,7 +4276,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4430,7 +4308,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4459,7 +4337,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4485,7 +4363,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4502,7 +4380,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4534,7 +4412,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4544,7 +4422,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4552,7 +4430,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4566,7 +4444,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4576,7 +4454,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4587,7 +4465,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4598,7 +4476,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4606,7 +4484,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4614,7 +4492,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -4625,7 +4503,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -4672,23 +4550,23 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="X34" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Y34" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="X35" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>68</v>
@@ -4696,32 +4574,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K33" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4762,10 +4640,10 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>18</v>
@@ -4774,7 +4652,7 @@
         <v>124</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>21</v>
@@ -4783,19 +4661,19 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4821,39 +4699,39 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
         <v>214</v>
-      </c>
-      <c r="J2" t="s">
-        <v>215</v>
-      </c>
-      <c r="K2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>219</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="Q3" t="s">
         <v>98</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -4861,11 +4739,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
37 testcase for the drybar UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="273">
   <si>
     <t>UserName</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t>SUPER LEMON DROP BRUSH</t>
+  </si>
+  <si>
+    <t>Baby Buttercup Travel Blow-Dryer</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -1482,7 +1485,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>44</v>
+        <v>272</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
135 testcase for drybar emea
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1231,7 +1231,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -3096,8 +3096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3107,6 +3107,8 @@
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -3216,11 +3218,11 @@
       <c r="I2" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>59</v>
+      <c r="J2" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>143</v>
+        <v>262</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>144</v>
@@ -3267,11 +3269,11 @@
       <c r="I3" t="s">
         <v>132</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>59</v>
+      <c r="J3" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>143</v>
+        <v>262</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>144</v>
@@ -3320,10 +3322,10 @@
         <v>135</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>143</v>
+        <v>265</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>262</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>68</v>
@@ -3370,25 +3372,25 @@
         <v>141</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="K5" t="s">
-        <v>143</v>
+      <c r="K5" s="13" t="s">
+        <v>262</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>60</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="K6" t="s">
-        <v>143</v>
+      <c r="K6" s="13" t="s">
+        <v>262</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>68</v>
       </c>
       <c r="V6" t="s">
-        <v>44</v>
+        <v>272</v>
       </c>
       <c r="X6" s="7"/>
     </row>
@@ -3396,8 +3398,8 @@
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="K7" t="s">
-        <v>143</v>
+      <c r="K7" s="13" t="s">
+        <v>262</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Drybar UK 42 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BCC1C7-803C-45EB-A58F-027227BF6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2488E4BF-41F1-4846-B20E-73D890E6319C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="277">
   <si>
     <t>UserName</t>
   </si>
@@ -847,6 +847,18 @@
   </si>
   <si>
     <t>Baby Buttercup Travel Blow-Dryer</t>
+  </si>
+  <si>
+    <t>8 Sillerton House</t>
+  </si>
+  <si>
+    <t>Aberdeen</t>
+  </si>
+  <si>
+    <t>Aberdeenshire</t>
+  </si>
+  <si>
+    <t>AB101YP</t>
   </si>
 </sst>
 </file>
@@ -1242,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1837,19 +1849,19 @@
         <v>80</v>
       </c>
       <c r="N22" t="s">
-        <v>81</v>
+        <v>273</v>
       </c>
       <c r="O22" t="s">
-        <v>82</v>
+        <v>274</v>
       </c>
       <c r="P22" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
       <c r="Q22" t="s">
-        <v>83</v>
+        <v>275</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>84</v>
+        <v>276</v>
       </c>
       <c r="S22">
         <v>9898989898</v>

</xml_diff>

<commit_message>
Drybar UK Commited 60 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2488E4BF-41F1-4846-B20E-73D890E6319C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4980CBBF-2B8F-4D8D-BAA6-C02C96C6E64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="278">
   <si>
     <t>UserName</t>
   </si>
@@ -859,6 +859,9 @@
   </si>
   <si>
     <t>AB101YP</t>
+  </si>
+  <si>
+    <t>QATEST25</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2011,7 +2014,7 @@
         <v>146</v>
       </c>
       <c r="AD30" t="s">
-        <v>145</v>
+        <v>277</v>
       </c>
       <c r="AE30" t="s">
         <v>145</v>
@@ -2188,7 +2191,7 @@
         <v>189</v>
       </c>
       <c r="AJ39" t="s">
-        <v>143</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Drybar UK 57 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C755325-A64B-42C0-82FE-CF3C349AF1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D508C225-AC5D-43C9-82F9-CC05179693EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -849,22 +849,22 @@
     <t>Baby Buttercup Travel Blow-Dryer</t>
   </si>
   <si>
-    <t>8 Sillerton House</t>
-  </si>
-  <si>
-    <t>Aberdeen</t>
-  </si>
-  <si>
-    <t>Aberdeenshire</t>
-  </si>
-  <si>
-    <t>AB101YP</t>
-  </si>
-  <si>
     <t>QATEST25</t>
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>84 High Point</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>West Midlands</t>
+  </si>
+  <si>
+    <t>B153RT</t>
   </si>
 </sst>
 </file>
@@ -1260,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1855,25 +1855,25 @@
         <v>80</v>
       </c>
       <c r="N22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="O22" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="P22" t="s">
         <v>266</v>
       </c>
       <c r="Q22" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
       </c>
       <c r="AB22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AJ22" t="s">
         <v>262</v>
@@ -2020,7 +2020,7 @@
         <v>146</v>
       </c>
       <c r="AD30" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="AE30" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
Guest user 3d for drybar UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D508C225-AC5D-43C9-82F9-CC05179693EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -19,8 +18,8 @@
     <sheet name="Outofstock" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="281">
   <si>
     <t>UserName</t>
   </si>
@@ -865,16 +864,22 @@
   </si>
   <si>
     <t>B153RT</t>
+  </si>
+  <si>
+    <t>3d_Secure</t>
+  </si>
+  <si>
+    <t>4000000000003220</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,21 +1255,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ17" sqref="AJ17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1290,7 +1295,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1409,7 +1414,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1458,7 +1463,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1470,7 +1475,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1497,7 +1502,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1516,7 +1521,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1533,7 +1538,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1592,7 +1597,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1609,7 +1614,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1628,7 +1633,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1645,98 +1650,80 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U13" s="5"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="5"/>
+        <v>279</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="W13">
+        <v>123</v>
+      </c>
       <c r="AJ13" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39">
       <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="5"/>
       <c r="AJ14" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+        <v>32</v>
+      </c>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
-      <c r="U15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="W15">
-        <v>123</v>
-      </c>
       <c r="AJ15" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
+      <c r="U16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="W16">
+        <v>123</v>
+      </c>
       <c r="AJ16" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" t="s">
-        <v>50</v>
-      </c>
-      <c r="P17" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>51</v>
-      </c>
-      <c r="R17">
-        <v>81504</v>
-      </c>
-      <c r="S17">
-        <v>9898989898</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
       <c r="AJ17" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
         <v>47</v>
@@ -1748,19 +1735,19 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>263</v>
+        <v>49</v>
       </c>
       <c r="O18" t="s">
-        <v>264</v>
+        <v>50</v>
       </c>
       <c r="P18" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="Q18" t="s">
-        <v>265</v>
-      </c>
-      <c r="R18" t="s">
-        <v>267</v>
+        <v>51</v>
+      </c>
+      <c r="R18">
+        <v>81504</v>
       </c>
       <c r="S18">
         <v>9898989898</v>
@@ -1769,626 +1756,661 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" t="s">
+        <v>263</v>
+      </c>
+      <c r="O19" t="s">
+        <v>264</v>
+      </c>
+      <c r="P19" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>265</v>
+      </c>
+      <c r="R19" t="s">
+        <v>267</v>
+      </c>
+      <c r="S19">
+        <v>9898989898</v>
+      </c>
       <c r="AJ19" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
-        <v>66</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z20" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
       <c r="AJ20" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N21" t="s">
-        <v>74</v>
-      </c>
-      <c r="O21" t="s">
-        <v>75</v>
-      </c>
-      <c r="P21" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>76</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="S21">
-        <v>9898989898</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="X21" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z21" s="5"/>
       <c r="AJ21" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="N22" t="s">
-        <v>275</v>
+        <v>74</v>
       </c>
       <c r="O22" t="s">
-        <v>276</v>
+        <v>75</v>
       </c>
       <c r="P22" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="Q22" t="s">
-        <v>277</v>
+        <v>76</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>278</v>
+        <v>77</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
       </c>
-      <c r="AB22" t="s">
-        <v>274</v>
-      </c>
       <c r="AJ22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="7"/>
-      <c r="K23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M23" t="s">
-        <v>88</v>
-      </c>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="2"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+      <c r="N23" t="s">
+        <v>275</v>
+      </c>
+      <c r="O23" t="s">
+        <v>276</v>
+      </c>
+      <c r="P23" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>277</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="S23">
+        <v>9898989898</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>274</v>
+      </c>
       <c r="AJ23" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="X24" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z24" s="5"/>
-      <c r="AA24" t="s">
-        <v>98</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="7"/>
+      <c r="K24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M24" t="s">
+        <v>88</v>
+      </c>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="2"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
       <c r="AJ24" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O25" t="s">
-        <v>101</v>
-      </c>
-      <c r="P25" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>102</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="S25" s="9">
-        <v>9898989898</v>
+        <v>95</v>
+      </c>
+      <c r="X25" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z25" s="5"/>
+      <c r="AA25" t="s">
+        <v>98</v>
       </c>
       <c r="AJ25" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
-        <v>105</v>
-      </c>
-      <c r="M26" t="s">
-        <v>270</v>
-      </c>
-      <c r="R26" s="10"/>
-      <c r="S26" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" t="s">
+        <v>80</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N26" t="s">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>101</v>
+      </c>
+      <c r="P26" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>102</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="S26" s="9">
+        <v>9898989898</v>
+      </c>
       <c r="AJ26" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M27" t="s">
-        <v>107</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="R27" s="10"/>
+      <c r="S27" s="9"/>
       <c r="AJ27" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="U28" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V28" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="W28" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="M28" t="s">
+        <v>107</v>
       </c>
       <c r="AJ28" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>88</v>
+        <v>110</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="V29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="AJ29" t="s">
         <v>262</v>
       </c>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="7"/>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>273</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>145</v>
+        <v>114</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="AJ30" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AK30" s="7"/>
+      <c r="AL30" s="7"/>
+    </row>
+    <row r="31" spans="1:38">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>146</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>273</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>145</v>
       </c>
       <c r="AJ31" t="s">
         <v>262</v>
       </c>
-      <c r="AK31" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AL31" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
-        <v>162</v>
-      </c>
-      <c r="M32" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AJ32" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AK32" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL32" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
+        <v>162</v>
+      </c>
+      <c r="M33" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39">
+      <c r="A34" t="s">
         <v>164</v>
       </c>
-      <c r="X33" t="s">
+      <c r="X34" t="s">
         <v>165</v>
       </c>
-      <c r="Y33" s="5" t="s">
+      <c r="Y34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z33" s="5"/>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="Z34" s="5"/>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" t="s">
         <v>167</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>79</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>170</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K35" s="8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:39">
+      <c r="A36" t="s">
         <v>175</v>
       </c>
-      <c r="X35" t="s">
+      <c r="X36" t="s">
         <v>96</v>
-      </c>
-      <c r="Y35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z35" s="5"/>
-      <c r="AA35" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" t="s">
-        <v>177</v>
-      </c>
-      <c r="I36" t="s">
-        <v>178</v>
-      </c>
-      <c r="X36" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z36" s="5"/>
       <c r="AA36" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" t="s">
+        <v>177</v>
+      </c>
+      <c r="I37" t="s">
+        <v>178</v>
+      </c>
+      <c r="X37" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:39">
+      <c r="A38" t="s">
         <v>181</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>79</v>
       </c>
-      <c r="AK37" t="s">
+      <c r="AK38" t="s">
         <v>182</v>
       </c>
-      <c r="AL37" s="7" t="s">
+      <c r="AL38" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:39">
+      <c r="A39" t="s">
         <v>183</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>184</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>184</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:39">
+      <c r="A40" t="s">
         <v>186</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>79</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>80</v>
       </c>
-      <c r="K39" s="8" t="s">
+      <c r="K40" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N40" t="s">
         <v>81</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O40" t="s">
         <v>82</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P40" t="s">
         <v>52</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="Q40" t="s">
         <v>83</v>
       </c>
-      <c r="R39" s="5" t="s">
+      <c r="R40" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="S39">
+      <c r="S40">
         <v>9898989898</v>
       </c>
-      <c r="T39">
+      <c r="T40">
         <v>888888</v>
       </c>
-      <c r="U39" s="5" t="s">
+      <c r="U40" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V39" s="5" t="s">
+      <c r="V40" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="W39" s="5" t="s">
+      <c r="W40" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="AJ39" t="s">
+      <c r="AJ40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:39">
+      <c r="A41" t="s">
         <v>190</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:39">
+      <c r="A42" t="s">
         <v>192</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>79</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G42" t="s">
         <v>80</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N42" t="s">
         <v>193</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O42" t="s">
         <v>194</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P42" t="s">
         <v>195</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="Q42" t="s">
         <v>196</v>
       </c>
-      <c r="R41" t="s">
+      <c r="R42" t="s">
         <v>197</v>
       </c>
-      <c r="S41">
+      <c r="S42">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+    <row r="43" spans="1:39">
+      <c r="A43" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C43" s="9"/>
       <c r="D43" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+    </row>
+    <row r="44" spans="1:39">
+      <c r="A44" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L43" s="8" t="s">
+      <c r="L44" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="M43" s="9"/>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
+      <c r="M44" s="9"/>
+    </row>
+    <row r="45" spans="1:39">
+      <c r="A45" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="X44" t="s">
+      <c r="X45" t="s">
         <v>227</v>
       </c>
-      <c r="Y44">
+      <c r="Y45">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+    <row r="46" spans="1:39">
+      <c r="A46" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="AM45" t="s">
+      <c r="AM46" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:39">
+      <c r="A47" t="s">
         <v>147</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>47</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>48</v>
       </c>
-      <c r="K46" s="8" t="s">
+      <c r="K47" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N47" t="s">
         <v>151</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O47" t="s">
         <v>150</v>
       </c>
-      <c r="P46" t="s">
+      <c r="P47" t="s">
         <v>52</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="Q47" t="s">
         <v>148</v>
       </c>
-      <c r="R46" s="10" t="s">
+      <c r="R47" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="S46">
+      <c r="S47">
         <v>9898989898</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K19" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K22" r:id="rId7"/>
+    <hyperlink ref="K24" r:id="rId8"/>
+    <hyperlink ref="K26" r:id="rId9"/>
+    <hyperlink ref="B35" r:id="rId10"/>
+    <hyperlink ref="D35" r:id="rId11"/>
+    <hyperlink ref="E35" r:id="rId12"/>
+    <hyperlink ref="K35" r:id="rId13"/>
+    <hyperlink ref="K40" r:id="rId14"/>
+    <hyperlink ref="B41" r:id="rId15"/>
+    <hyperlink ref="D41" r:id="rId16"/>
+    <hyperlink ref="E41" r:id="rId17"/>
+    <hyperlink ref="C41" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="E8" r:id="rId21"/>
+    <hyperlink ref="B43" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C43" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E43" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K43" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B44" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D44" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E44" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K44" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L44" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K47" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>
@@ -2396,21 +2418,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="25" max="25" width="20.6640625" customWidth="1"/>
     <col min="26" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2499,7 +2521,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2540,7 +2562,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2563,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2571,7 +2593,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -2582,7 +2604,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -2595,39 +2617,39 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2758,7 +2780,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2804,7 +2826,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -2825,7 +2847,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2839,7 +2861,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -2853,7 +2875,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -2866,7 +2888,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -2881,7 +2903,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -2896,7 +2918,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -2911,7 +2933,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -2921,30 +2943,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -2953,7 +2975,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3057,7 +3079,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3073,27 +3095,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3101,7 +3123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3115,14 +3137,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -3143,7 +3165,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3217,7 +3239,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3268,7 +3290,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3320,7 +3342,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3374,7 +3396,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3401,7 +3423,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3416,7 +3438,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3429,38 +3451,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3567,7 +3589,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3615,7 +3637,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3624,7 +3646,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3635,7 +3657,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3648,7 +3670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3656,14 +3678,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3683,7 +3705,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -3712,7 +3734,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -3744,7 +3766,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3765,7 +3787,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -3776,7 +3798,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -3805,7 +3827,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -3832,7 +3854,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -3846,7 +3868,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -3854,7 +3876,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -3862,7 +3884,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -3870,39 +3892,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4015,7 +4037,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4061,7 +4083,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4070,7 +4092,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4079,7 +4101,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4090,7 +4112,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4103,7 +4125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4116,7 +4138,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4129,7 +4151,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4143,7 +4165,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4159,7 +4181,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4173,14 +4195,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4200,14 +4222,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4239,7 +4261,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4271,7 +4293,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4292,7 +4314,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4303,7 +4325,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4335,7 +4357,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4364,7 +4386,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4390,7 +4412,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4407,7 +4429,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4439,7 +4461,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4449,7 +4471,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4457,7 +4479,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4471,7 +4493,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4481,7 +4503,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4492,7 +4514,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4503,7 +4525,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4511,7 +4533,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4519,7 +4541,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -4530,7 +4552,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -4577,7 +4599,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -4588,7 +4610,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -4601,32 +4623,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K33" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4700,7 +4722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4741,7 +4763,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -4766,11 +4788,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Drybar UK 20 testcase updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063EE81-08A3-465A-B770-B856B55837EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="Search" sheetId="8" r:id="rId2"/>
-    <sheet name="Header" sheetId="9" r:id="rId3"/>
-    <sheet name="Track_My_Order" sheetId="2" r:id="rId4"/>
-    <sheet name="Artical Links" sheetId="3" r:id="rId5"/>
-    <sheet name="GiftRegistry" sheetId="4" r:id="rId6"/>
-    <sheet name="My AccountPage" sheetId="5" r:id="rId7"/>
-    <sheet name="Bundles" sheetId="6" r:id="rId8"/>
-    <sheet name="Outofstock" sheetId="7" r:id="rId9"/>
+    <sheet name="ShareWhisList" sheetId="10" r:id="rId3"/>
+    <sheet name="Header" sheetId="9" r:id="rId4"/>
+    <sheet name="Track_My_Order" sheetId="2" r:id="rId5"/>
+    <sheet name="Artical Links" sheetId="3" r:id="rId6"/>
+    <sheet name="GiftRegistry" sheetId="4" r:id="rId7"/>
+    <sheet name="My AccountPage" sheetId="5" r:id="rId8"/>
+    <sheet name="Bundles" sheetId="6" r:id="rId9"/>
+    <sheet name="Outofstock" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="285">
   <si>
     <t>UserName</t>
   </si>
@@ -848,38 +850,50 @@
     <t>Baby Buttercup Travel Blow-Dryer</t>
   </si>
   <si>
-    <t>QATEST25</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>84 High Point</t>
-  </si>
-  <si>
-    <t>Birmingham</t>
-  </si>
-  <si>
-    <t>West Midlands</t>
-  </si>
-  <si>
-    <t>B153RT</t>
-  </si>
-  <si>
-    <t>3d_Secure</t>
-  </si>
-  <si>
-    <t>4000000000003220</t>
+    <t>8 Sillerton House</t>
+  </si>
+  <si>
+    <t>Aberdeen</t>
+  </si>
+  <si>
+    <t>Aberdeenshire</t>
+  </si>
+  <si>
+    <t>AB101YP</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Account validation</t>
+  </si>
+  <si>
+    <t>share whishlist</t>
+  </si>
+  <si>
+    <t>qatesting.lotuswave+1@gmail.com,qatesting.lotuswave+2@gmail.com</t>
+  </si>
+  <si>
+    <t>Best product and low price</t>
+  </si>
+  <si>
+    <t>WishListEmail</t>
+  </si>
+  <si>
+    <t>rthoutireddy@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>good product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,6 +950,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -964,7 +993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -982,6 +1011,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1255,47 +1289,49 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ17" sqref="AJ17"/>
+    <sheetView tabSelected="1" topLeftCell="AG34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI47" sqref="AI47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="16" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1414,7 +1450,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1463,7 +1499,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1475,7 +1511,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1487,7 +1523,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1502,7 +1538,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1521,7 +1557,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1538,7 +1574,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1583,7 +1619,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1597,7 +1633,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1614,7 +1650,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1633,7 +1669,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1650,80 +1686,98 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>279</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="W13">
-        <v>123</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="5"/>
       <c r="AJ13" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="U14" s="5"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
       <c r="AJ14" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
+      <c r="U15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="W15">
+        <v>123</v>
+      </c>
       <c r="AJ15" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+        <v>34</v>
+      </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="U16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="W16">
-        <v>123</v>
-      </c>
       <c r="AJ16" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" t="s">
+        <v>50</v>
+      </c>
+      <c r="P17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>51</v>
+      </c>
+      <c r="R17">
+        <v>81504</v>
+      </c>
+      <c r="S17">
+        <v>9898989898</v>
+      </c>
       <c r="AJ17" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>47</v>
@@ -1735,19 +1789,19 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>49</v>
+        <v>263</v>
       </c>
       <c r="O18" t="s">
-        <v>50</v>
+        <v>264</v>
       </c>
       <c r="P18" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
       <c r="Q18" t="s">
-        <v>51</v>
-      </c>
-      <c r="R18">
-        <v>81504</v>
+        <v>265</v>
+      </c>
+      <c r="R18" t="s">
+        <v>267</v>
       </c>
       <c r="S18">
         <v>9898989898</v>
@@ -1756,108 +1810,105 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N19" t="s">
-        <v>263</v>
-      </c>
-      <c r="O19" t="s">
-        <v>264</v>
-      </c>
-      <c r="P19" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>265</v>
-      </c>
-      <c r="R19" t="s">
-        <v>267</v>
-      </c>
-      <c r="S19">
-        <v>9898989898</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
       <c r="AJ19" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" t="s">
-        <v>65</v>
-      </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z20" s="5"/>
       <c r="AJ20" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
-      </c>
-      <c r="X21" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z21" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21" t="s">
+        <v>74</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>76</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="S21">
+        <v>9898989898</v>
+      </c>
       <c r="AJ21" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="N22" t="s">
-        <v>74</v>
+        <v>273</v>
       </c>
       <c r="O22" t="s">
-        <v>75</v>
+        <v>274</v>
       </c>
       <c r="P22" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
       <c r="Q22" t="s">
-        <v>76</v>
+        <v>275</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>77</v>
+        <v>276</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
@@ -1866,573 +1917,713 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
-      <c r="N23" t="s">
-        <v>275</v>
-      </c>
-      <c r="O23" t="s">
-        <v>276</v>
-      </c>
-      <c r="P23" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>277</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="S23">
-        <v>9898989898</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>274</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="K23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M23" t="s">
+        <v>88</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="2"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
       <c r="AJ23" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="7"/>
-      <c r="K24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M24" t="s">
-        <v>88</v>
-      </c>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="2"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="X24" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z24" s="5"/>
+      <c r="AA24" t="s">
+        <v>98</v>
+      </c>
       <c r="AJ24" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="X25" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z25" s="5"/>
-      <c r="AA25" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P25" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="S25" s="9">
+        <v>9898989898</v>
       </c>
       <c r="AJ25" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" t="s">
-        <v>80</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N26" t="s">
-        <v>100</v>
-      </c>
-      <c r="O26" t="s">
-        <v>101</v>
-      </c>
-      <c r="P26" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>102</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="S26" s="9">
-        <v>9898989898</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="M26" t="s">
+        <v>270</v>
+      </c>
+      <c r="R26" s="10"/>
+      <c r="S26" s="9"/>
       <c r="AJ26" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M27" t="s">
-        <v>270</v>
-      </c>
-      <c r="R27" s="10"/>
-      <c r="S27" s="9"/>
+        <v>107</v>
+      </c>
       <c r="AJ27" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
-      </c>
-      <c r="M28" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W28" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="AJ28" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="U29" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V29" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="AJ29" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="30" spans="1:38">
+      <c r="AK29" s="7"/>
+      <c r="AL29" s="7"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>88</v>
+        <v>146</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>145</v>
       </c>
       <c r="AJ30" t="s">
         <v>262</v>
       </c>
-      <c r="AK30" s="7"/>
-      <c r="AL30" s="7"/>
-    </row>
-    <row r="31" spans="1:38">
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>273</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="AJ31" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="32" spans="1:38">
+      <c r="AK31" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL31" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="M32" t="s">
+        <v>163</v>
       </c>
       <c r="AJ32" t="s">
         <v>262</v>
       </c>
-      <c r="AK32" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AL32" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:39">
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>162</v>
-      </c>
-      <c r="M33" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ33" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="1:39">
+        <v>164</v>
+      </c>
+      <c r="X33" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>164</v>
-      </c>
-      <c r="X34" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y34" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>175</v>
+      </c>
+      <c r="X35" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y35" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z34" s="5"/>
-    </row>
-    <row r="35" spans="1:39">
-      <c r="A35" t="s">
-        <v>167</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" t="s">
-        <v>170</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:39">
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>175</v>
-      </c>
-      <c r="X36" t="s">
-        <v>96</v>
+        <v>176</v>
+      </c>
+      <c r="H36" t="s">
+        <v>177</v>
+      </c>
+      <c r="I36" t="s">
+        <v>178</v>
+      </c>
+      <c r="X36" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z36" s="5"/>
       <c r="AA36" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:39">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>176</v>
-      </c>
-      <c r="H37" t="s">
-        <v>177</v>
-      </c>
-      <c r="I37" t="s">
-        <v>178</v>
-      </c>
-      <c r="X37" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" spans="1:39">
+        <v>181</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL37" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>181</v>
-      </c>
-      <c r="F38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="AK38" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL38" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:39">
-      <c r="A39" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39">
+      <c r="G39" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O39" t="s">
+        <v>82</v>
+      </c>
+      <c r="P39" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>83</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S39">
+        <v>9898989898</v>
+      </c>
+      <c r="T39">
+        <v>888888</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V39" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="W39" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>186</v>
-      </c>
-      <c r="F40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>192</v>
+      </c>
+      <c r="F41" t="s">
         <v>79</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
         <v>80</v>
       </c>
-      <c r="K40" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="N40" t="s">
-        <v>81</v>
-      </c>
-      <c r="O40" t="s">
-        <v>82</v>
-      </c>
-      <c r="P40" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>83</v>
-      </c>
-      <c r="R40" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S40">
+      <c r="N41" t="s">
+        <v>193</v>
+      </c>
+      <c r="O41" t="s">
+        <v>194</v>
+      </c>
+      <c r="P41" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>196</v>
+      </c>
+      <c r="R41" t="s">
+        <v>197</v>
+      </c>
+      <c r="S41">
         <v>9898989898</v>
       </c>
-      <c r="T40">
-        <v>888888</v>
-      </c>
-      <c r="U40" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V40" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="W40" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="AJ40" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="41" spans="1:39">
-      <c r="A41" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D41" s="8" t="s">
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="42" spans="1:39">
-      <c r="A42" t="s">
-        <v>192</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="F42" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G42" t="s">
-        <v>80</v>
-      </c>
-      <c r="N42" t="s">
-        <v>193</v>
-      </c>
-      <c r="O42" t="s">
-        <v>194</v>
-      </c>
-      <c r="P42" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>196</v>
-      </c>
-      <c r="R42" t="s">
-        <v>197</v>
-      </c>
-      <c r="S42">
-        <v>9898989898</v>
-      </c>
-    </row>
-    <row r="43" spans="1:39">
+      <c r="G42" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>167</v>
+        <v>218</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>216</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C43" s="9"/>
       <c r="D43" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>170</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L43" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>221</v>
+      </c>
       <c r="M43" s="9"/>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="X44" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AM45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
+      </c>
+      <c r="K46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L44" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="M44" s="9"/>
-    </row>
-    <row r="45" spans="1:39">
-      <c r="A45" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="X45" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39">
-      <c r="A46" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="AM46" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:39">
-      <c r="A47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F47" t="s">
-        <v>47</v>
-      </c>
-      <c r="G47" t="s">
-        <v>48</v>
+      <c r="N46" t="s">
+        <v>151</v>
+      </c>
+      <c r="O46" t="s">
+        <v>150</v>
+      </c>
+      <c r="P46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>148</v>
+      </c>
+      <c r="R46" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="S46">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>282</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N47" t="s">
-        <v>151</v>
-      </c>
-      <c r="O47" t="s">
-        <v>150</v>
-      </c>
-      <c r="P47" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>148</v>
-      </c>
-      <c r="R47" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="S47">
-        <v>9898989898</v>
+        <v>283</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
-    <hyperlink ref="K19" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K22" r:id="rId7"/>
-    <hyperlink ref="K24" r:id="rId8"/>
-    <hyperlink ref="K26" r:id="rId9"/>
-    <hyperlink ref="B35" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="E35" r:id="rId12"/>
-    <hyperlink ref="K35" r:id="rId13"/>
-    <hyperlink ref="K40" r:id="rId14"/>
-    <hyperlink ref="B41" r:id="rId15"/>
-    <hyperlink ref="D41" r:id="rId16"/>
-    <hyperlink ref="E41" r:id="rId17"/>
-    <hyperlink ref="C41" r:id="rId18"/>
-    <hyperlink ref="F8" r:id="rId19"/>
-    <hyperlink ref="D8" r:id="rId20"/>
-    <hyperlink ref="E8" r:id="rId21"/>
-    <hyperlink ref="B43" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C43" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D43" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E43" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K43" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B44" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D44" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E44" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K44" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L44" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K47" r:id="rId32"/>
+    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K47" r:id="rId33" xr:uid="{44E8D76C-47AB-4247-940B-39EB584E3339}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>98</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="25" max="25" width="20.6640625" customWidth="1"/>
-    <col min="26" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="36.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2521,7 +2712,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2562,7 +2753,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2585,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2593,7 +2784,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -2604,7 +2795,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -2617,39 +2808,216 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="Y4" r:id="rId6"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A899FB07-2CEC-45AE-B6CF-DD56536E91CF}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="18" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{053CC33F-88CC-44A2-8699-AB67F857578D}"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{E1C1F5B3-ABB4-45BE-A050-C8AB2F315C27}"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{4E960FB3-5FB3-4DCD-BBB3-265E63629A34}"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{972A3DDA-1955-4CBA-87B2-A6A864647692}"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{75B38858-E238-49EC-B55B-B8C8FE997E1D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2780,7 +3148,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2826,7 +3194,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -2847,7 +3215,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2861,7 +3229,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -2875,7 +3243,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -2888,7 +3256,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -2903,7 +3271,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -2918,7 +3286,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -2933,7 +3301,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -2943,39 +3311,39 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3079,7 +3447,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3095,27 +3463,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3123,7 +3491,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3136,36 +3504,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3239,7 +3607,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3290,7 +3658,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3342,7 +3710,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3396,7 +3764,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3423,7 +3791,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3438,7 +3806,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3451,38 +3819,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="B5" r:id="rId12"/>
-    <hyperlink ref="C5" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3589,7 +3957,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3637,7 +4005,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3646,7 +4014,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3657,7 +4025,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3670,7 +4038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3678,14 +4046,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3705,7 +4073,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -3734,7 +4102,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -3766,7 +4134,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3787,7 +4155,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -3798,7 +4166,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -3827,7 +4195,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -3854,7 +4222,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -3868,7 +4236,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -3876,7 +4244,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -3884,7 +4252,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -3892,39 +4260,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K2" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4037,7 +4405,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4083,7 +4451,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4092,7 +4460,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4101,7 +4469,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4112,7 +4480,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4125,7 +4493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4138,7 +4506,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4151,7 +4519,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4165,7 +4533,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4181,7 +4549,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4195,14 +4563,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4222,14 +4590,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4261,7 +4629,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4293,7 +4661,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4314,7 +4682,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4325,7 +4693,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4357,7 +4725,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4386,7 +4754,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4412,7 +4780,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4429,7 +4797,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4461,7 +4829,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4471,7 +4839,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4479,7 +4847,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4493,7 +4861,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4503,7 +4871,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4514,7 +4882,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4525,7 +4893,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4533,7 +4901,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4541,7 +4909,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -4552,7 +4920,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -4599,7 +4967,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -4610,7 +4978,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -4623,178 +4991,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K19" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K33" r:id="rId10"/>
+    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
+    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" t="s">
-        <v>209</v>
-      </c>
-      <c r="J2" t="s">
-        <v>210</v>
-      </c>
-      <c r="K2" t="s">
-        <v>211</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>214</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>98</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Drybar UK 59 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063EE81-08A3-465A-B770-B856B55837EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6744C581-B2B1-41F7-A48C-B72833569AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="286">
   <si>
     <t>UserName</t>
   </si>
@@ -884,6 +884,9 @@
   </si>
   <si>
     <t>good product</t>
+  </si>
+  <si>
+    <t>DRYQATEST20</t>
   </si>
 </sst>
 </file>
@@ -1299,39 +1302,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI47" sqref="AI47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="16" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1574,7 +1577,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1650,7 +1653,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1946,7 +1949,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -2012,7 +2015,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2053,12 +2056,12 @@
       <c r="AK29" s="7"/>
       <c r="AL29" s="7"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>146</v>
       </c>
       <c r="AD30" t="s">
-        <v>145</v>
+        <v>285</v>
       </c>
       <c r="AE30" t="s">
         <v>145</v>
@@ -2067,7 +2070,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2104,7 +2107,7 @@
       </c>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>167</v>
       </c>
@@ -2315,7 +2318,7 @@
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
@@ -2342,7 +2345,7 @@
       </c>
       <c r="M43" s="9"/>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>226</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>258</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>282</v>
       </c>
@@ -2453,9 +2456,9 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2614,16 +2617,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" customWidth="1"/>
-    <col min="28" max="28" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2712,7 +2715,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2753,7 +2756,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2784,7 +2787,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -2795,7 +2798,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2834,19 +2837,19 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -2901,7 +2904,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>278</v>
       </c>
@@ -2913,7 +2916,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -2929,7 +2932,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>279</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>235</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>279</v>
       </c>
@@ -2969,7 +2972,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -2983,7 +2986,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3011,13 +3014,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3148,7 +3151,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3194,7 +3197,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3215,7 +3218,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3229,7 +3232,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -3243,7 +3246,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3256,7 +3259,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3271,7 +3274,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3286,7 +3289,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -3301,7 +3304,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3311,7 +3314,7 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
@@ -3334,16 +3337,16 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3447,7 +3450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3477,13 +3480,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3491,7 +3494,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3512,28 +3515,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3607,7 +3610,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3658,7 +3661,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3710,7 +3713,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3764,7 +3767,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3791,7 +3794,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3806,7 +3809,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3845,12 +3848,12 @@
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4005,7 +4008,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4014,7 +4017,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4025,7 +4028,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4038,7 +4041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4046,14 +4049,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4073,7 +4076,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4102,7 +4105,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4134,7 +4137,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4155,7 +4158,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4166,7 +4169,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4195,7 +4198,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4222,7 +4225,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4236,7 +4239,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4244,7 +4247,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -4252,7 +4255,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -4260,7 +4263,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
@@ -4286,13 +4289,13 @@
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4451,7 +4454,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4460,7 +4463,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4469,7 +4472,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4480,7 +4483,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4506,7 +4509,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4549,7 +4552,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4563,14 +4566,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4590,14 +4593,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4629,7 +4632,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4661,7 +4664,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4682,7 +4685,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4725,7 +4728,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4754,7 +4757,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4780,7 +4783,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4797,7 +4800,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4829,7 +4832,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4839,7 +4842,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4847,7 +4850,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4871,7 +4874,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4882,7 +4885,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4893,7 +4896,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4901,7 +4904,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -4920,7 +4923,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -4967,7 +4970,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -4978,7 +4981,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>223</v>
       </c>

</xml_diff>

<commit_message>
Drybar UK 59 test case Drybar US 57, 59 changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6744C581-B2B1-41F7-A48C-B72833569AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A608AFE-58D3-4840-B000-F90DE36586B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="287">
   <si>
     <t>UserName</t>
   </si>
@@ -887,6 +887,9 @@
   </si>
   <si>
     <t>DRYQATEST20</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -1303,7 +1306,7 @@
   <dimension ref="A1:AM47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,6 +1979,9 @@
       </c>
       <c r="G25" t="s">
         <v>80</v>
+      </c>
+      <c r="I25" t="s">
+        <v>286</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Tax changes for drybar us and eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A608AFE-58D3-4840-B000-F90DE36586B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,8 +19,8 @@
     <sheet name="Outofstock" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="287">
   <si>
     <t>UserName</t>
   </si>
@@ -895,11 +894,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1295,21 +1294,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1337,7 +1336,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1456,7 +1455,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1580,7 +1579,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1625,7 +1624,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1639,7 +1638,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1692,7 +1691,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1713,7 +1712,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1736,7 +1735,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1970,7 +1969,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -2008,7 +2007,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -2021,7 +2020,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2032,7 +2031,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2062,7 +2061,7 @@
       <c r="AK29" s="7"/>
       <c r="AL29" s="7"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
         <v>146</v>
       </c>
@@ -2076,7 +2075,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2101,7 +2100,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2112,8 +2111,11 @@
         <v>68</v>
       </c>
       <c r="Z33" s="5"/>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -2135,8 +2137,11 @@
       <c r="K34" s="8" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -2150,8 +2155,11 @@
       <c r="AA35" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2171,14 +2179,20 @@
       <c r="AA36" s="5" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ36" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
         <v>181</v>
       </c>
       <c r="F37" t="s">
         <v>79</v>
       </c>
+      <c r="AJ37" t="s">
+        <v>262</v>
+      </c>
       <c r="AK37" t="s">
         <v>182</v>
       </c>
@@ -2186,7 +2200,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2199,8 +2213,11 @@
       <c r="D38" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2244,10 +2261,10 @@
         <v>189</v>
       </c>
       <c r="AJ39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -2263,8 +2280,11 @@
       <c r="E40" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ40" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -2292,8 +2312,11 @@
       <c r="S41">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ41" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39">
       <c r="A42" s="9" t="s">
         <v>167</v>
       </c>
@@ -2323,8 +2346,11 @@
       </c>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39">
       <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
@@ -2350,8 +2376,11 @@
         <v>221</v>
       </c>
       <c r="M43" s="9"/>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ43" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39">
       <c r="A44" s="9" t="s">
         <v>226</v>
       </c>
@@ -2361,16 +2390,22 @@
       <c r="Y44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
         <v>258</v>
       </c>
+      <c r="AJ45" t="s">
+        <v>262</v>
+      </c>
       <c r="AM45" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2401,8 +2436,11 @@
       <c r="S46">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AJ46" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39">
       <c r="A47" s="9" t="s">
         <v>282</v>
       </c>
@@ -2412,42 +2450,45 @@
       <c r="AI47" t="s">
         <v>284</v>
       </c>
+      <c r="AJ47" t="s">
+        <v>262</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K47" r:id="rId33" xr:uid="{44E8D76C-47AB-4247-940B-39EB584E3339}"/>
+    <hyperlink ref="K17" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K25" r:id="rId9"/>
+    <hyperlink ref="B34" r:id="rId10"/>
+    <hyperlink ref="D34" r:id="rId11"/>
+    <hyperlink ref="E34" r:id="rId12"/>
+    <hyperlink ref="K34" r:id="rId13"/>
+    <hyperlink ref="K39" r:id="rId14"/>
+    <hyperlink ref="B40" r:id="rId15"/>
+    <hyperlink ref="D40" r:id="rId16"/>
+    <hyperlink ref="E40" r:id="rId17"/>
+    <hyperlink ref="C40" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="E8" r:id="rId21"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K46" r:id="rId32"/>
+    <hyperlink ref="K47" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId34"/>
@@ -2455,16 +2496,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2538,7 +2579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +2620,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2604,11 +2645,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2616,14 +2657,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -2632,7 +2673,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2721,7 +2762,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2762,7 +2803,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2785,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2793,7 +2834,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -2804,7 +2845,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -2817,33 +2858,33 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A899FB07-2CEC-45AE-B6CF-DD56536E91CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -2855,7 +2896,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2890,7 +2931,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -2910,7 +2951,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>278</v>
       </c>
@@ -2922,7 +2963,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -2938,7 +2979,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
         <v>279</v>
       </c>
@@ -2956,7 +2997,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
         <v>235</v>
       </c>
@@ -2967,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
         <v>279</v>
       </c>
@@ -2978,7 +3019,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -2992,7 +3033,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3002,31 +3043,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{053CC33F-88CC-44A2-8699-AB67F857578D}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{E1C1F5B3-ABB4-45BE-A050-C8AB2F315C27}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{4E960FB3-5FB3-4DCD-BBB3-265E63629A34}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{972A3DDA-1955-4CBA-87B2-A6A864647692}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{75B38858-E238-49EC-B55B-B8C8FE997E1D}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3157,7 +3198,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3203,7 +3244,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3224,7 +3265,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3238,7 +3279,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -3252,7 +3293,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3265,7 +3306,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3280,7 +3321,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3295,7 +3336,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -3310,7 +3351,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3320,30 +3361,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -3352,7 +3393,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3456,7 +3497,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3472,27 +3513,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3500,7 +3541,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3514,14 +3555,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -3542,7 +3583,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3616,7 +3657,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3667,7 +3708,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3719,7 +3760,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3773,7 +3814,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3800,7 +3841,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3815,7 +3856,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3828,38 +3869,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3966,7 +4007,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4014,7 +4055,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4023,7 +4064,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4034,7 +4075,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4047,7 +4088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4055,14 +4096,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4082,7 +4123,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4111,7 +4152,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4143,7 +4184,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4164,7 +4205,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4175,7 +4216,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4204,7 +4245,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4231,7 +4272,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4245,7 +4286,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4253,7 +4294,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -4261,7 +4302,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -4269,39 +4310,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4414,7 +4455,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4460,7 +4501,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4469,7 +4510,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4478,7 +4519,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4489,7 +4530,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4502,7 +4543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4515,7 +4556,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4528,7 +4569,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4542,7 +4583,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4558,7 +4599,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4572,14 +4613,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4599,14 +4640,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4638,7 +4679,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4670,7 +4711,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4691,7 +4732,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4702,7 +4743,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4734,7 +4775,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4763,7 +4804,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4789,7 +4830,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4806,7 +4847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4838,7 +4879,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4848,7 +4889,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4856,7 +4897,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4870,7 +4911,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4880,7 +4921,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4891,7 +4932,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4902,7 +4943,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4910,7 +4951,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4918,7 +4959,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -4929,7 +4970,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -4976,7 +5017,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -4987,7 +5028,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -5000,16 +5041,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K33" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Drybar UK Commited 80 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5917BE-B321-4E35-BF4F-94BB09AA7702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -19,8 +20,8 @@
     <sheet name="Outofstock" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="289">
   <si>
     <t>UserName</t>
   </si>
@@ -889,16 +890,22 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Notify_me_Product</t>
+  </si>
+  <si>
+    <t>Liquid Glass Instant Glossing Rinse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1294,21 +1301,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1336,7 +1343,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1455,7 +1462,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1504,7 +1511,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1528,7 +1535,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1550,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1562,7 +1569,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1624,7 +1631,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1638,7 +1645,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1655,7 +1662,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1691,7 +1698,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1712,7 +1719,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1745,7 +1752,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1780,7 +1787,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1815,7 +1822,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1840,7 +1847,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1855,7 +1862,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1890,7 +1897,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1922,7 +1929,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1951,7 +1958,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -2007,7 +2014,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -2020,7 +2027,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2031,7 +2038,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2048,7 +2055,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2061,7 +2068,7 @@
       <c r="AK29" s="7"/>
       <c r="AL29" s="7"/>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>146</v>
       </c>
@@ -2075,7 +2082,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -2089,7 +2096,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2100,7 +2107,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2115,7 +2122,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -2141,7 +2148,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -2159,7 +2166,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2183,7 +2190,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2217,7 +2224,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2264,7 +2271,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -2284,7 +2291,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -2316,7 +2323,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>167</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
@@ -2380,7 +2387,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>226</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>258</v>
       </c>
@@ -2405,7 +2412,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2440,7 +2447,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>282</v>
       </c>
@@ -2454,58 +2461,73 @@
         <v>262</v>
       </c>
     </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="X48" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y48">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1"/>
-    <hyperlink ref="K18" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
-    <hyperlink ref="K25" r:id="rId9"/>
-    <hyperlink ref="B34" r:id="rId10"/>
-    <hyperlink ref="D34" r:id="rId11"/>
-    <hyperlink ref="E34" r:id="rId12"/>
-    <hyperlink ref="K34" r:id="rId13"/>
-    <hyperlink ref="K39" r:id="rId14"/>
-    <hyperlink ref="B40" r:id="rId15"/>
-    <hyperlink ref="D40" r:id="rId16"/>
-    <hyperlink ref="E40" r:id="rId17"/>
-    <hyperlink ref="C40" r:id="rId18"/>
-    <hyperlink ref="F8" r:id="rId19"/>
-    <hyperlink ref="D8" r:id="rId20"/>
-    <hyperlink ref="E8" r:id="rId21"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K46" r:id="rId32"/>
-    <hyperlink ref="K47" r:id="rId33"/>
+    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K47" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B48" r:id="rId34" xr:uid="{C70F62DB-35E5-43A4-B2E5-FDE48DDBA799}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2579,7 +2601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2620,7 +2642,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2645,11 +2667,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2657,14 +2679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -2673,7 +2695,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2762,7 +2784,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2803,7 +2825,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2826,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2834,7 +2856,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -2845,7 +2867,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -2858,33 +2880,33 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="Y4" r:id="rId6"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -2896,7 +2918,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2931,7 +2953,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -2951,7 +2973,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>278</v>
       </c>
@@ -2963,7 +2985,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -2979,7 +3001,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>279</v>
       </c>
@@ -2997,7 +3019,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>235</v>
       </c>
@@ -3008,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>279</v>
       </c>
@@ -3019,7 +3041,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3033,7 +3055,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3043,31 +3065,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3198,7 +3220,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3244,7 +3266,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3265,7 +3287,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3279,7 +3301,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -3293,7 +3315,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3306,7 +3328,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3321,7 +3343,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3336,7 +3358,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -3351,7 +3373,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3361,30 +3383,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -3393,7 +3415,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3497,7 +3519,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3513,27 +3535,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3541,7 +3563,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3555,14 +3577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -3583,7 +3605,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3657,7 +3679,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3708,7 +3730,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3760,7 +3782,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3814,7 +3836,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3841,7 +3863,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3856,7 +3878,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3869,38 +3891,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="B5" r:id="rId12"/>
-    <hyperlink ref="C5" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4007,7 +4029,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4055,7 +4077,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4064,7 +4086,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4075,7 +4097,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4088,7 +4110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4096,14 +4118,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4123,7 +4145,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4152,7 +4174,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4184,7 +4206,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4205,7 +4227,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4216,7 +4238,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4245,7 +4267,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4272,7 +4294,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4286,7 +4308,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4294,7 +4316,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -4302,7 +4324,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -4310,39 +4332,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K2" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4455,7 +4477,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4501,7 +4523,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4510,7 +4532,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4519,7 +4541,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4530,7 +4552,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4543,7 +4565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4556,7 +4578,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4569,7 +4591,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4583,7 +4605,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4599,7 +4621,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4613,14 +4635,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4640,14 +4662,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4679,7 +4701,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4711,7 +4733,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4732,7 +4754,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4743,7 +4765,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4775,7 +4797,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4804,7 +4826,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4830,7 +4852,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4847,7 +4869,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4879,7 +4901,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4889,7 +4911,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4897,7 +4919,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4911,7 +4933,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4921,7 +4943,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4932,7 +4954,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4943,7 +4965,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4951,7 +4973,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4959,7 +4981,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -4970,7 +4992,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -5017,7 +5039,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -5028,7 +5050,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -5041,16 +5063,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K19" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K33" r:id="rId10"/>
+    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Drybar UK Commited 39 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5917BE-B321-4E35-BF4F-94BB09AA7702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E805F0-7E65-4193-B51D-F528A45EA603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="291">
   <si>
     <t>UserName</t>
   </si>
@@ -896,6 +896,12 @@
   </si>
   <si>
     <t>Liquid Glass Instant Glossing Rinse</t>
+  </si>
+  <si>
+    <t>MyWishList</t>
+  </si>
+  <si>
+    <t>The Bouncer Diffuser</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM48"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,6 +2478,17 @@
         <v>288</v>
       </c>
       <c r="Y48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="X49" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y49">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drybar UK 45 Testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E805F0-7E65-4193-B51D-F528A45EA603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254D0C90-4249-4FF5-BAA5-A37357DB96C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="291">
   <si>
     <t>UserName</t>
   </si>
@@ -1315,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM49"/>
+  <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,17 +1750,42 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" t="s">
+        <v>50</v>
+      </c>
+      <c r="P16" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16">
+        <v>81504</v>
+      </c>
+      <c r="S16">
+        <v>9898989898</v>
+      </c>
       <c r="AJ16" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
         <v>47</v>
@@ -1772,19 +1797,19 @@
         <v>46</v>
       </c>
       <c r="N17" t="s">
-        <v>49</v>
+        <v>263</v>
       </c>
       <c r="O17" t="s">
-        <v>50</v>
+        <v>264</v>
       </c>
       <c r="P17" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
       <c r="Q17" t="s">
-        <v>51</v>
-      </c>
-      <c r="R17">
-        <v>81504</v>
+        <v>265</v>
+      </c>
+      <c r="R17" t="s">
+        <v>267</v>
       </c>
       <c r="S17">
         <v>9898989898</v>
@@ -1795,106 +1820,103 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N18" t="s">
-        <v>263</v>
-      </c>
-      <c r="O18" t="s">
-        <v>264</v>
-      </c>
-      <c r="P18" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>265</v>
-      </c>
-      <c r="R18" t="s">
-        <v>267</v>
-      </c>
-      <c r="S18">
-        <v>9898989898</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
       <c r="AJ18" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="X19" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z19" s="5"/>
       <c r="AJ19" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z20" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" t="s">
+        <v>74</v>
+      </c>
+      <c r="O20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>76</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="S20">
+        <v>9898989898</v>
+      </c>
       <c r="AJ20" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="N21" t="s">
-        <v>74</v>
+        <v>273</v>
       </c>
       <c r="O21" t="s">
-        <v>75</v>
+        <v>274</v>
       </c>
       <c r="P21" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
       <c r="Q21" t="s">
-        <v>76</v>
+        <v>275</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>77</v>
+        <v>276</v>
       </c>
       <c r="S21">
         <v>9898989898</v>
@@ -1905,78 +1927,84 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" t="s">
-        <v>80</v>
-      </c>
-      <c r="N22" t="s">
-        <v>273</v>
-      </c>
-      <c r="O22" t="s">
-        <v>274</v>
-      </c>
-      <c r="P22" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>275</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="S22">
-        <v>9898989898</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="7"/>
+      <c r="K22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22" t="s">
+        <v>88</v>
+      </c>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="2"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
       <c r="AJ22" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="7"/>
-      <c r="K23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M23" t="s">
-        <v>88</v>
-      </c>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="2"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="X23" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z23" s="5"/>
+      <c r="AA23" t="s">
+        <v>98</v>
+      </c>
       <c r="AJ23" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="X24" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z24" s="5"/>
-      <c r="AA24" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="F24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" t="s">
+        <v>286</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N24" t="s">
+        <v>100</v>
+      </c>
+      <c r="O24" t="s">
+        <v>101</v>
+      </c>
+      <c r="P24" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>102</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="S24" s="9">
+        <v>9898989898</v>
       </c>
       <c r="AJ24" t="s">
         <v>262</v>
@@ -1984,61 +2012,40 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" t="s">
-        <v>286</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O25" t="s">
-        <v>101</v>
-      </c>
-      <c r="P25" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>102</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="S25" s="9">
-        <v>9898989898</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="M25" t="s">
+        <v>270</v>
+      </c>
+      <c r="R25" s="10"/>
+      <c r="S25" s="9"/>
       <c r="AJ25" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M26" t="s">
-        <v>270</v>
-      </c>
-      <c r="R26" s="10"/>
-      <c r="S26" s="9"/>
+        <v>107</v>
+      </c>
       <c r="AJ26" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>106</v>
-      </c>
-      <c r="M27" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="U27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="V27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W27" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="AJ27" t="s">
         <v>262</v>
@@ -2046,109 +2053,110 @@
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="U28" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V28" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="W28" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="AJ28" t="s">
         <v>262</v>
       </c>
+      <c r="AK28" s="7"/>
+      <c r="AL28" s="7"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>88</v>
+        <v>146</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>145</v>
       </c>
       <c r="AJ29" t="s">
         <v>262</v>
       </c>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="7"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>285</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="AJ30" t="s">
         <v>262</v>
       </c>
+      <c r="AK30" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL30" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="M31" t="s">
+        <v>163</v>
       </c>
       <c r="AJ31" t="s">
         <v>262</v>
       </c>
-      <c r="AK31" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AL31" s="7" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>162</v>
-      </c>
-      <c r="M32" t="s">
-        <v>163</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="X32" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z32" s="5"/>
       <c r="AJ32" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>164</v>
-      </c>
-      <c r="X33" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z33" s="5"/>
+        <v>167</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" t="s">
+        <v>170</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>168</v>
+      </c>
       <c r="AJ33" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>167</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" t="s">
-        <v>170</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>168</v>
+        <v>175</v>
+      </c>
+      <c r="X34" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="AJ34" t="s">
         <v>262</v>
@@ -2156,17 +2164,23 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>175</v>
-      </c>
-      <c r="X35" t="s">
-        <v>96</v>
+        <v>176</v>
+      </c>
+      <c r="H35" t="s">
+        <v>177</v>
+      </c>
+      <c r="I35" t="s">
+        <v>178</v>
+      </c>
+      <c r="X35" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z35" s="5"/>
       <c r="AA35" s="5" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="AJ35" t="s">
         <v>262</v>
@@ -2174,57 +2188,80 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" t="s">
-        <v>177</v>
-      </c>
-      <c r="I36" t="s">
-        <v>178</v>
-      </c>
-      <c r="X36" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y36" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z36" s="5"/>
-      <c r="AA36" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="F36" t="s">
+        <v>79</v>
       </c>
       <c r="AJ36" t="s">
         <v>262</v>
       </c>
+      <c r="AK36" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL36" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>181</v>
-      </c>
-      <c r="F37" t="s">
-        <v>79</v>
+        <v>183</v>
+      </c>
+      <c r="B37" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" t="s">
+        <v>185</v>
       </c>
       <c r="AJ37" t="s">
         <v>262</v>
       </c>
-      <c r="AK37" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL37" s="7" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" t="s">
-        <v>184</v>
-      </c>
-      <c r="C38" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" t="s">
+        <v>80</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N38" t="s">
+        <v>81</v>
+      </c>
+      <c r="O38" t="s">
+        <v>82</v>
+      </c>
+      <c r="P38" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>83</v>
+      </c>
+      <c r="R38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S38">
+        <v>9898989898</v>
+      </c>
+      <c r="T38">
+        <v>888888</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V38" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="W38" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="AJ38" t="s">
         <v>262</v>
@@ -2232,46 +2269,19 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>186</v>
-      </c>
-      <c r="F39" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" t="s">
-        <v>80</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="N39" t="s">
-        <v>81</v>
-      </c>
-      <c r="O39" t="s">
-        <v>82</v>
-      </c>
-      <c r="P39" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>83</v>
-      </c>
-      <c r="R39" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S39">
-        <v>9898989898</v>
-      </c>
-      <c r="T39">
-        <v>888888</v>
-      </c>
-      <c r="U39" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V39" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="W39" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="AJ39" t="s">
         <v>262</v>
@@ -2279,85 +2289,95 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>190</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>169</v>
+        <v>192</v>
+      </c>
+      <c r="F40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" t="s">
+        <v>80</v>
+      </c>
+      <c r="N40" t="s">
+        <v>193</v>
+      </c>
+      <c r="O40" t="s">
+        <v>194</v>
+      </c>
+      <c r="P40" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>196</v>
+      </c>
+      <c r="R40" t="s">
+        <v>197</v>
+      </c>
+      <c r="S40">
+        <v>9898989898</v>
       </c>
       <c r="AJ40" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>192</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="A41" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G41" t="s">
-        <v>80</v>
-      </c>
-      <c r="N41" t="s">
-        <v>193</v>
-      </c>
-      <c r="O41" t="s">
-        <v>194</v>
-      </c>
-      <c r="P41" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>196</v>
-      </c>
-      <c r="R41" t="s">
-        <v>197</v>
-      </c>
-      <c r="S41">
-        <v>9898989898</v>
-      </c>
+      <c r="G41" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
       <c r="AJ41" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>167</v>
+        <v>218</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>216</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C42" s="9"/>
       <c r="D42" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>170</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L42" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>221</v>
+      </c>
       <c r="M42" s="9"/>
       <c r="AJ42" t="s">
         <v>262</v>
@@ -2365,89 +2385,73 @@
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="M43" s="9"/>
+        <v>226</v>
+      </c>
+      <c r="X43" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y43">
+        <v>2</v>
+      </c>
       <c r="AJ43" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="X44" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y44">
-        <v>2</v>
+        <v>258</v>
       </c>
       <c r="AJ44" t="s">
         <v>262</v>
       </c>
+      <c r="AM44" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>258</v>
+      <c r="A45" t="s">
+        <v>147</v>
+      </c>
+      <c r="F45" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" t="s">
+        <v>48</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N45" t="s">
+        <v>151</v>
+      </c>
+      <c r="O45" t="s">
+        <v>150</v>
+      </c>
+      <c r="P45" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>148</v>
+      </c>
+      <c r="R45" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="S45">
+        <v>9898989898</v>
       </c>
       <c r="AJ45" t="s">
         <v>262</v>
       </c>
-      <c r="AM45" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>147</v>
-      </c>
-      <c r="F46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" t="s">
-        <v>48</v>
+      <c r="A46" s="9" t="s">
+        <v>282</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N46" t="s">
-        <v>151</v>
-      </c>
-      <c r="O46" t="s">
-        <v>150</v>
-      </c>
-      <c r="P46" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>148</v>
-      </c>
-      <c r="R46" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="S46">
-        <v>9898989898</v>
+        <v>283</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>284</v>
       </c>
       <c r="AJ46" t="s">
         <v>262</v>
@@ -2455,79 +2459,65 @@
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>284</v>
-      </c>
-      <c r="AJ47" t="s">
-        <v>262</v>
+        <v>287</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="X47" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y47">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>184</v>
+        <v>289</v>
       </c>
       <c r="X48" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="Y48">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="X49" t="s">
-        <v>290</v>
-      </c>
-      <c r="Y49">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="K20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D33" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E33" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K33" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K38" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B39" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D39" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C39" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K47" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B48" r:id="rId34" xr:uid="{C70F62DB-35E5-43A4-B2E5-FDE48DDBA799}"/>
+    <hyperlink ref="B41" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C41" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D41" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E41" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K41" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B42" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D42" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E42" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K42" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L42" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K45" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K46" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B47" r:id="rId34" xr:uid="{C70F62DB-35E5-43A4-B2E5-FDE48DDBA799}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
Drybar UK Commited 140 & 143 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254D0C90-4249-4FF5-BAA5-A37357DB96C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E027C32-F3ED-4073-81D4-40844E71C98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="292">
   <si>
     <t>UserName</t>
   </si>
@@ -902,6 +902,9 @@
   </si>
   <si>
     <t>The Bouncer Diffuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Blow-Dryers</t>
   </si>
 </sst>
 </file>
@@ -1315,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM48"/>
+  <dimension ref="A1:AN48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1349,7 +1352,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1467,8 +1470,11 @@
       <c r="AM1" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AN1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1529,7 +1535,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1562,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1704,7 +1710,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1725,7 +1731,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1843,12 +1849,18 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>66</v>
       </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
       <c r="X19" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Y19" s="5" t="s">
         <v>68</v>
@@ -1857,8 +1869,11 @@
       <c r="AJ19" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1893,7 +1908,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -1954,7 +1969,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -1972,7 +1987,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2010,7 +2025,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2023,7 +2038,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -2034,7 +2049,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -2051,7 +2066,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -2064,7 +2079,7 @@
       <c r="AK28" s="7"/>
       <c r="AL28" s="7"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>146</v>
       </c>
@@ -2078,7 +2093,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>159</v>
       </c>
@@ -2092,7 +2107,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
116 testcase for drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E027C32-F3ED-4073-81D4-40844E71C98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,8 +19,8 @@
     <sheet name="Outofstock" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="295">
   <si>
     <t>UserName</t>
   </si>
@@ -905,16 +904,25 @@
   </si>
   <si>
     <t xml:space="preserve"> Blow-Dryers</t>
+  </si>
+  <si>
+    <t>Test Qa - 84/4 Great King Street, Edinburgh, MIDLOTHIAN, EH36QU</t>
+  </si>
+  <si>
+    <t>Express Paypal</t>
+  </si>
+  <si>
+    <t>Delivery - £0.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,7 +1022,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1037,6 +1045,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1310,21 +1319,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AN49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1352,7 +1361,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1523,7 +1532,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1535,7 +1544,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1547,7 +1556,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1562,7 +1571,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1598,7 +1607,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1643,7 +1652,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1674,7 +1683,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1710,7 +1719,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1731,7 +1740,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1754,7 +1763,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1789,7 +1798,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1849,7 +1858,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1908,7 +1917,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1940,7 +1949,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -1955,10 +1964,24 @@
       <c r="K22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M22" t="s">
-        <v>88</v>
-      </c>
-      <c r="S22" s="9"/>
+      <c r="N22" t="s">
+        <v>263</v>
+      </c>
+      <c r="O22" t="s">
+        <v>264</v>
+      </c>
+      <c r="P22" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>265</v>
+      </c>
+      <c r="R22" t="s">
+        <v>267</v>
+      </c>
+      <c r="S22" s="22" t="s">
+        <v>213</v>
+      </c>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
@@ -1969,7 +1992,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -1987,7 +2010,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2025,7 +2048,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2038,501 +2061,514 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40">
       <c r="A26" t="s">
+        <v>293</v>
+      </c>
+      <c r="M26" t="s">
+        <v>294</v>
+      </c>
+      <c r="N26" t="s">
+        <v>292</v>
+      </c>
+      <c r="R26" s="10"/>
+      <c r="S26" s="9"/>
+    </row>
+    <row r="27" spans="1:40">
+      <c r="A27" t="s">
         <v>106</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M27" t="s">
         <v>107</v>
-      </c>
-      <c r="AJ26" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>110</v>
-      </c>
-      <c r="U27" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V27" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="W27" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="AJ27" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40">
       <c r="A28" t="s">
-        <v>114</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>88</v>
+        <v>110</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W28" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="AJ28" t="s">
         <v>262</v>
       </c>
-      <c r="AK28" s="7"/>
-      <c r="AL28" s="7"/>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:40">
       <c r="A29" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>285</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>145</v>
+        <v>114</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="AJ29" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AK29" s="7"/>
+      <c r="AL29" s="7"/>
+    </row>
+    <row r="30" spans="1:40">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>146</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>145</v>
       </c>
       <c r="AJ30" t="s">
         <v>262</v>
       </c>
-      <c r="AK30" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AL30" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:40">
       <c r="A31" t="s">
-        <v>162</v>
-      </c>
-      <c r="M31" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AJ31" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AK31" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL31" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40">
       <c r="A32" t="s">
-        <v>164</v>
-      </c>
-      <c r="X32" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y32" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z32" s="5"/>
+        <v>162</v>
+      </c>
+      <c r="M32" t="s">
+        <v>163</v>
+      </c>
       <c r="AJ32" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F33" t="s">
-        <v>79</v>
-      </c>
-      <c r="G33" t="s">
-        <v>170</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>168</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="X33" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z33" s="5"/>
       <c r="AJ33" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
-        <v>175</v>
-      </c>
-      <c r="X34" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y34" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z34" s="5"/>
-      <c r="AA34" s="5" t="s">
-        <v>98</v>
+        <v>167</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="AJ34" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
-        <v>176</v>
-      </c>
-      <c r="H35" t="s">
-        <v>177</v>
-      </c>
-      <c r="I35" t="s">
-        <v>178</v>
-      </c>
-      <c r="X35" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="X35" t="s">
+        <v>96</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z35" s="5"/>
       <c r="AA35" s="5" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="AJ35" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
-        <v>181</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
+        <v>176</v>
+      </c>
+      <c r="H36" t="s">
+        <v>177</v>
+      </c>
+      <c r="I36" t="s">
+        <v>178</v>
+      </c>
+      <c r="X36" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="AJ36" t="s">
         <v>262</v>
       </c>
-      <c r="AK36" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL36" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" t="s">
-        <v>184</v>
-      </c>
-      <c r="C37" t="s">
-        <v>184</v>
-      </c>
-      <c r="D37" t="s">
-        <v>185</v>
+        <v>181</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
       </c>
       <c r="AJ37" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AK37" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL37" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
-        <v>186</v>
-      </c>
-      <c r="F38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" t="s">
-        <v>80</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="N38" t="s">
-        <v>81</v>
-      </c>
-      <c r="O38" t="s">
-        <v>82</v>
-      </c>
-      <c r="P38" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>83</v>
-      </c>
-      <c r="R38" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S38">
-        <v>9898989898</v>
-      </c>
-      <c r="T38">
-        <v>888888</v>
-      </c>
-      <c r="U38" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V38" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="W38" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" t="s">
+        <v>185</v>
       </c>
       <c r="AJ38" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>169</v>
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O39" t="s">
+        <v>82</v>
+      </c>
+      <c r="P39" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>83</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S39">
+        <v>9898989898</v>
+      </c>
+      <c r="T39">
+        <v>888888</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V39" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="W39" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="AJ39" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>192</v>
-      </c>
-      <c r="F40" t="s">
-        <v>79</v>
-      </c>
-      <c r="G40" t="s">
-        <v>80</v>
-      </c>
-      <c r="N40" t="s">
-        <v>193</v>
-      </c>
-      <c r="O40" t="s">
-        <v>194</v>
-      </c>
-      <c r="P40" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>196</v>
-      </c>
-      <c r="R40" t="s">
-        <v>197</v>
-      </c>
-      <c r="S40">
-        <v>9898989898</v>
+        <v>190</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="AJ40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F41" s="9" t="s">
+    <row r="41" spans="1:39">
+      <c r="A41" t="s">
+        <v>192</v>
+      </c>
+      <c r="F41" t="s">
         <v>79</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="G41" t="s">
+        <v>80</v>
+      </c>
+      <c r="N41" t="s">
+        <v>193</v>
+      </c>
+      <c r="O41" t="s">
+        <v>194</v>
+      </c>
+      <c r="P41" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>196</v>
+      </c>
+      <c r="R41" t="s">
+        <v>197</v>
+      </c>
+      <c r="S41">
+        <v>9898989898</v>
+      </c>
       <c r="AJ41" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39">
       <c r="A42" s="9" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" s="9"/>
+        <v>216</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>216</v>
+      </c>
       <c r="D42" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>221</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="AJ42" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39">
       <c r="A43" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="X43" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y43">
-        <v>2</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="M43" s="9"/>
       <c r="AJ43" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39">
       <c r="A44" s="9" t="s">
-        <v>258</v>
+        <v>226</v>
+      </c>
+      <c r="X44" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y44">
+        <v>2</v>
       </c>
       <c r="AJ44" t="s">
         <v>262</v>
       </c>
-      <c r="AM44" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>147</v>
-      </c>
-      <c r="F45" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" t="s">
-        <v>48</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N45" t="s">
-        <v>151</v>
-      </c>
-      <c r="O45" t="s">
-        <v>150</v>
-      </c>
-      <c r="P45" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>148</v>
-      </c>
-      <c r="R45" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="S45">
-        <v>9898989898</v>
+    </row>
+    <row r="45" spans="1:39">
+      <c r="A45" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="AJ45" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>282</v>
+      <c r="AM45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="AI46" t="s">
-        <v>284</v>
+        <v>46</v>
+      </c>
+      <c r="N46" t="s">
+        <v>151</v>
+      </c>
+      <c r="O46" t="s">
+        <v>150</v>
+      </c>
+      <c r="P46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>148</v>
+      </c>
+      <c r="R46" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="S46">
+        <v>9898989898</v>
       </c>
       <c r="AJ46" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39">
       <c r="A47" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>284</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39">
+      <c r="A48" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="X47" t="s">
+      <c r="X48" t="s">
         <v>288</v>
-      </c>
-      <c r="Y47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="X48" t="s">
-        <v>290</v>
       </c>
       <c r="Y48">
         <v>2</v>
       </c>
     </row>
+    <row r="49" spans="1:25">
+      <c r="A49" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="X49" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y49">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D33" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E33" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K33" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K38" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B39" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D39" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C39" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B41" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C41" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D41" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E41" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K41" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B42" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D42" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E42" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K42" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L42" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K45" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K46" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B47" r:id="rId34" xr:uid="{C70F62DB-35E5-43A4-B2E5-FDE48DDBA799}"/>
+    <hyperlink ref="K16" r:id="rId1"/>
+    <hyperlink ref="K17" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K20" r:id="rId7"/>
+    <hyperlink ref="K22" r:id="rId8"/>
+    <hyperlink ref="K24" r:id="rId9"/>
+    <hyperlink ref="B34" r:id="rId10"/>
+    <hyperlink ref="D34" r:id="rId11"/>
+    <hyperlink ref="E34" r:id="rId12"/>
+    <hyperlink ref="K34" r:id="rId13"/>
+    <hyperlink ref="K39" r:id="rId14"/>
+    <hyperlink ref="B40" r:id="rId15"/>
+    <hyperlink ref="D40" r:id="rId16"/>
+    <hyperlink ref="E40" r:id="rId17"/>
+    <hyperlink ref="C40" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="E8" r:id="rId21"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K46" r:id="rId32"/>
+    <hyperlink ref="K47" r:id="rId33"/>
+    <hyperlink ref="B48" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2540,16 +2576,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2623,7 +2659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2664,7 +2700,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2689,11 +2725,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2701,14 +2737,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -2717,7 +2753,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2806,7 +2842,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2847,7 +2883,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2870,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2878,7 +2914,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -2889,7 +2925,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -2902,33 +2938,33 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -2940,7 +2976,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2975,7 +3011,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -2995,7 +3031,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>278</v>
       </c>
@@ -3007,7 +3043,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3023,7 +3059,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
         <v>279</v>
       </c>
@@ -3041,7 +3077,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
         <v>235</v>
       </c>
@@ -3052,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
         <v>279</v>
       </c>
@@ -3063,7 +3099,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3077,7 +3113,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3087,31 +3123,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3242,7 +3278,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3288,7 +3324,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3309,7 +3345,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3323,7 +3359,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -3337,7 +3373,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3350,7 +3386,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3365,7 +3401,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3380,7 +3416,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -3395,7 +3431,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3405,30 +3441,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -3437,7 +3473,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3541,7 +3577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3557,27 +3593,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3585,7 +3621,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3599,14 +3635,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -3627,7 +3663,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3701,7 +3737,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3752,7 +3788,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -3804,7 +3840,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -3858,7 +3894,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -3885,7 +3921,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3900,7 +3936,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3913,38 +3949,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4051,7 +4087,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4099,7 +4135,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4108,7 +4144,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4119,7 +4155,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4132,7 +4168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4140,14 +4176,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4167,7 +4203,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4196,7 +4232,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4228,7 +4264,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4249,7 +4285,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4260,7 +4296,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4289,7 +4325,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4316,7 +4352,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4330,7 +4366,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4338,7 +4374,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -4346,7 +4382,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -4354,39 +4390,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4499,7 +4535,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4545,7 +4581,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4554,7 +4590,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4563,7 +4599,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4574,7 +4610,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4587,7 +4623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4600,7 +4636,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4613,7 +4649,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4627,7 +4663,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4643,7 +4679,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4657,14 +4693,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4684,14 +4720,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4723,7 +4759,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -4755,7 +4791,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4776,7 +4812,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4787,7 +4823,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -4819,7 +4855,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -4848,7 +4884,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4874,7 +4910,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4891,7 +4927,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4923,7 +4959,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4933,7 +4969,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4941,7 +4977,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -4955,7 +4991,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -4965,7 +5001,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -4976,7 +5012,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -4987,7 +5023,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -4995,7 +5031,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5003,7 +5039,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -5014,7 +5050,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -5061,7 +5097,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -5072,7 +5108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -5085,16 +5121,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K33" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
009 testcase for drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1319,7 +1319,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -1869,7 +1869,7 @@
         <v>64</v>
       </c>
       <c r="X19" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y19" s="5" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
testcases for drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="My AccountPage" sheetId="5" r:id="rId8"/>
     <sheet name="Bundles" sheetId="6" r:id="rId9"/>
     <sheet name="Outofstock" sheetId="7" r:id="rId10"/>
+    <sheet name="MyFavorites" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="299">
   <si>
     <t>UserName</t>
   </si>
@@ -913,6 +914,18 @@
   </si>
   <si>
     <t>Delivery - £0.00</t>
+  </si>
+  <si>
+    <t>Scent</t>
+  </si>
+  <si>
+    <t>AETHER™ 55</t>
+  </si>
+  <si>
+    <t>Checkout my wishlist</t>
+  </si>
+  <si>
+    <t>hmarm@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1046,6 +1059,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1319,7 +1333,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1329,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -2736,6 +2750,208 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" t="s">
+        <v>264</v>
+      </c>
+      <c r="K2" t="s">
+        <v>266</v>
+      </c>
+      <c r="L2" t="s">
+        <v>265</v>
+      </c>
+      <c r="M2" t="s">
+        <v>267</v>
+      </c>
+      <c r="N2">
+        <v>9898989898</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="S3" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="U3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V3" t="s">
+        <v>296</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>297</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="AC4" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>

</xml_diff>

<commit_message>
DRY UK 60 Testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF2FA13-ED24-4C90-A256-8A8159035B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,8 +21,8 @@
     <sheet name="MyFavorites" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="300">
   <si>
     <t>UserName</t>
   </si>
@@ -926,16 +927,19 @@
   </si>
   <si>
     <t>hmarm@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Product &lt;50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1333,21 +1337,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1375,7 +1379,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1497,7 +1501,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1546,7 +1550,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1558,7 +1562,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1604,7 +1608,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1621,7 +1625,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1666,7 +1670,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1697,7 +1701,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1716,7 +1720,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1733,7 +1737,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1744,7 +1748,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1754,7 +1758,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1777,7 +1781,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1847,7 +1851,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -1896,7 +1900,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -2006,7 +2010,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2062,7 +2066,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2075,7 +2079,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>293</v>
       </c>
@@ -2088,7 +2092,7 @@
       <c r="R26" s="10"/>
       <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2099,7 +2103,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2116,7 +2120,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2129,7 +2133,7 @@
       <c r="AK29" s="7"/>
       <c r="AL29" s="7"/>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>146</v>
       </c>
@@ -2143,7 +2147,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -2157,7 +2161,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2183,7 +2187,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -2209,7 +2213,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -2227,7 +2231,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2285,7 +2289,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2332,7 +2336,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -2384,7 +2388,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>167</v>
       </c>
@@ -2418,7 +2422,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>226</v>
       </c>
@@ -2462,7 +2466,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>258</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2508,7 +2512,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>282</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>287</v>
       </c>
@@ -2536,7 +2540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>289</v>
       </c>
@@ -2547,42 +2551,66 @@
         <v>2</v>
       </c>
     </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>299</v>
+      </c>
+      <c r="H50" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" t="s">
+        <v>64</v>
+      </c>
+      <c r="X50" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z50" s="5"/>
+      <c r="AJ50" t="s">
+        <v>262</v>
+      </c>
+      <c r="AN50" t="s">
+        <v>291</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K16" r:id="rId1"/>
-    <hyperlink ref="K17" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K20" r:id="rId7"/>
-    <hyperlink ref="K22" r:id="rId8"/>
-    <hyperlink ref="K24" r:id="rId9"/>
-    <hyperlink ref="B34" r:id="rId10"/>
-    <hyperlink ref="D34" r:id="rId11"/>
-    <hyperlink ref="E34" r:id="rId12"/>
-    <hyperlink ref="K34" r:id="rId13"/>
-    <hyperlink ref="K39" r:id="rId14"/>
-    <hyperlink ref="B40" r:id="rId15"/>
-    <hyperlink ref="D40" r:id="rId16"/>
-    <hyperlink ref="E40" r:id="rId17"/>
-    <hyperlink ref="C40" r:id="rId18"/>
-    <hyperlink ref="F8" r:id="rId19"/>
-    <hyperlink ref="D8" r:id="rId20"/>
-    <hyperlink ref="E8" r:id="rId21"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K46" r:id="rId32"/>
-    <hyperlink ref="K47" r:id="rId33"/>
-    <hyperlink ref="B48" r:id="rId34"/>
+    <hyperlink ref="K16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K47" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B48" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2590,16 +2618,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2673,7 +2701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2714,7 +2742,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2739,11 +2767,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2751,14 +2779,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
@@ -2773,7 +2801,7 @@
     <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2862,7 +2890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2907,7 +2935,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2928,7 +2956,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>279</v>
       </c>
@@ -2941,26 +2969,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="AC4" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -2969,7 +2997,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3058,7 +3086,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3099,7 +3127,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -3122,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -3130,7 +3158,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -3141,7 +3169,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -3154,33 +3182,33 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="Y4" r:id="rId6"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -3192,7 +3220,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3227,7 +3255,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -3247,7 +3275,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>278</v>
       </c>
@@ -3259,7 +3287,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3275,7 +3303,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>279</v>
       </c>
@@ -3293,7 +3321,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>235</v>
       </c>
@@ -3304,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>279</v>
       </c>
@@ -3315,7 +3343,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3329,7 +3357,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3339,31 +3367,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3494,7 +3522,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3540,7 +3568,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3561,7 +3589,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3575,7 +3603,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -3589,7 +3617,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3602,7 +3630,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3617,7 +3645,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3632,7 +3660,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -3647,7 +3675,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3657,30 +3685,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -3689,7 +3717,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3793,7 +3821,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3809,27 +3837,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3837,7 +3865,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3851,14 +3879,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -3879,7 +3907,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3953,7 +3981,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -4004,7 +4032,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4056,7 +4084,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -4110,7 +4138,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -4137,7 +4165,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4152,7 +4180,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4165,38 +4193,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="B5" r:id="rId12"/>
-    <hyperlink ref="C5" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4303,7 +4331,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4351,7 +4379,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4360,7 +4388,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4371,7 +4399,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4384,7 +4412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4392,14 +4420,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4419,7 +4447,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4448,7 +4476,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4480,7 +4508,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4501,7 +4529,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4512,7 +4540,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4541,7 +4569,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4568,7 +4596,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4582,7 +4610,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4590,7 +4618,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -4598,7 +4626,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -4606,39 +4634,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K2" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4751,7 +4779,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4797,7 +4825,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4806,7 +4834,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4815,7 +4843,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4826,7 +4854,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4839,7 +4867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4852,7 +4880,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4865,7 +4893,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4879,7 +4907,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4895,7 +4923,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4909,14 +4937,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4936,14 +4964,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4975,7 +5003,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -5007,7 +5035,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5028,7 +5056,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5039,7 +5067,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5071,7 +5099,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5100,7 +5128,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5126,7 +5154,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -5143,7 +5171,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -5175,7 +5203,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -5185,7 +5213,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -5193,7 +5221,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -5207,7 +5235,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -5217,7 +5245,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -5228,7 +5256,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -5239,7 +5267,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -5247,7 +5275,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5255,7 +5283,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -5266,7 +5294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -5313,7 +5341,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -5324,7 +5352,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -5337,16 +5365,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K19" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K33" r:id="rId10"/>
+    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
174 testcase for the drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF2FA13-ED24-4C90-A256-8A8159035B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -19,10 +18,11 @@
     <sheet name="Bundles" sheetId="6" r:id="rId9"/>
     <sheet name="Outofstock" sheetId="7" r:id="rId10"/>
     <sheet name="MyFavorites" sheetId="11" r:id="rId11"/>
+    <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="307">
   <si>
     <t>UserName</t>
   </si>
@@ -930,16 +930,41 @@
   </si>
   <si>
     <t>Product &lt;50</t>
+  </si>
+  <si>
+    <t>Shipping address</t>
+  </si>
+  <si>
+    <t>9999999999</t>
+  </si>
+  <si>
+    <t>6 Sillerton House</t>
+  </si>
+  <si>
+    <t>Create Account</t>
+  </si>
+  <si>
+    <t>New ShippingAddress</t>
+  </si>
+  <si>
+    <t>New BillingAddress</t>
+  </si>
+  <si>
+    <t>QA TEST
+93 York House
+Bradford, West Yorkshire, BD109ET
+United Kingdom
+T: 9999999999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1039,7 +1064,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1064,6 +1089,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1337,21 +1365,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1379,7 +1407,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1501,7 +1529,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1578,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1562,7 +1590,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1574,7 +1602,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1589,7 +1617,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1608,7 +1636,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1625,7 +1653,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1670,7 +1698,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1684,7 +1712,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1701,7 +1729,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1720,7 +1748,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1737,7 +1765,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1748,7 +1776,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1758,7 +1786,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1781,7 +1809,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1816,7 +1844,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1851,7 +1879,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1876,7 +1904,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -1900,7 +1928,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1935,7 +1963,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +1995,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -2010,7 +2038,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -2028,7 +2056,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2066,7 +2094,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2079,7 +2107,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40">
       <c r="A26" t="s">
         <v>293</v>
       </c>
@@ -2092,7 +2120,7 @@
       <c r="R26" s="10"/>
       <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2103,7 +2131,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2120,7 +2148,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2133,7 +2161,7 @@
       <c r="AK29" s="7"/>
       <c r="AL29" s="7"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40">
       <c r="A30" t="s">
         <v>146</v>
       </c>
@@ -2147,7 +2175,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -2161,7 +2189,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2172,7 +2200,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2187,7 +2215,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -2213,7 +2241,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -2231,7 +2259,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2255,7 +2283,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -2272,7 +2300,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2289,7 +2317,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2336,7 +2364,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -2356,7 +2384,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -2388,7 +2416,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39">
       <c r="A42" s="9" t="s">
         <v>167</v>
       </c>
@@ -2422,7 +2450,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39">
       <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
@@ -2452,7 +2480,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39">
       <c r="A44" s="9" t="s">
         <v>226</v>
       </c>
@@ -2466,7 +2494,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
         <v>258</v>
       </c>
@@ -2477,7 +2505,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2512,7 +2540,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39">
       <c r="A47" s="9" t="s">
         <v>282</v>
       </c>
@@ -2526,7 +2554,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39">
       <c r="A48" s="9" t="s">
         <v>287</v>
       </c>
@@ -2540,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:40">
       <c r="A49" s="9" t="s">
         <v>289</v>
       </c>
@@ -2551,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:40">
       <c r="A50" t="s">
         <v>299</v>
       </c>
@@ -2577,40 +2605,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C40" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K47" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B48" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="K16" r:id="rId1"/>
+    <hyperlink ref="K17" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K20" r:id="rId7"/>
+    <hyperlink ref="K22" r:id="rId8"/>
+    <hyperlink ref="K24" r:id="rId9"/>
+    <hyperlink ref="B34" r:id="rId10"/>
+    <hyperlink ref="D34" r:id="rId11"/>
+    <hyperlink ref="E34" r:id="rId12"/>
+    <hyperlink ref="K34" r:id="rId13"/>
+    <hyperlink ref="K39" r:id="rId14"/>
+    <hyperlink ref="B40" r:id="rId15"/>
+    <hyperlink ref="D40" r:id="rId16"/>
+    <hyperlink ref="E40" r:id="rId17"/>
+    <hyperlink ref="C40" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="E8" r:id="rId21"/>
+    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K46" r:id="rId32"/>
+    <hyperlink ref="K47" r:id="rId33"/>
+    <hyperlink ref="B48" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2618,16 +2646,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2701,7 +2729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2742,7 +2770,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2767,11 +2795,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2779,14 +2807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
@@ -2801,7 +2829,7 @@
     <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2890,7 +2918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2935,7 +2963,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2956,7 +2984,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>279</v>
       </c>
@@ -2969,26 +2997,280 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="AC4" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
+        <v>302</v>
+      </c>
+      <c r="J3" t="s">
+        <v>274</v>
+      </c>
+      <c r="K3" t="s">
+        <v>275</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>304</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>302</v>
+      </c>
+      <c r="J5" t="s">
+        <v>274</v>
+      </c>
+      <c r="K5" t="s">
+        <v>275</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="187.2">
+      <c r="A6" t="s">
+        <v>305</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J6" t="s">
+        <v>210</v>
+      </c>
+      <c r="K6" t="s">
+        <v>211</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="N7" s="24"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -2997,7 +3279,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3086,7 +3368,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3127,7 +3409,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -3150,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -3158,7 +3440,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>233</v>
       </c>
@@ -3169,7 +3451,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -3182,33 +3464,33 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -3220,7 +3502,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3255,7 +3537,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -3275,7 +3557,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>278</v>
       </c>
@@ -3287,7 +3569,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3303,7 +3585,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
         <v>279</v>
       </c>
@@ -3321,7 +3603,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
         <v>235</v>
       </c>
@@ -3332,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
         <v>279</v>
       </c>
@@ -3343,7 +3625,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3357,7 +3639,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3367,31 +3649,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3522,7 +3804,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3568,7 +3850,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3589,7 +3871,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3603,7 +3885,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>245</v>
       </c>
@@ -3617,7 +3899,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3630,7 +3912,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3645,7 +3927,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3660,7 +3942,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -3675,7 +3957,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3685,30 +3967,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -3717,7 +3999,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3821,7 +4103,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3837,27 +4119,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3865,7 +4147,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3879,14 +4161,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -3907,7 +4189,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3981,7 +4263,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -4032,7 +4314,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4084,7 +4366,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -4138,7 +4420,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -4165,7 +4447,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4180,7 +4462,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4193,38 +4475,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4331,7 +4613,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4379,7 +4661,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4388,7 +4670,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4399,7 +4681,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4412,7 +4694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4420,14 +4702,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4447,7 +4729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4476,7 +4758,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4508,7 +4790,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4529,7 +4811,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4540,7 +4822,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4569,7 +4851,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4596,7 +4878,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4610,7 +4892,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4618,7 +4900,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -4626,7 +4908,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -4634,39 +4916,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4779,7 +5061,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4825,7 +5107,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4834,7 +5116,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4843,7 +5125,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4854,7 +5136,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4867,7 +5149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4880,7 +5162,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4893,7 +5175,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4907,7 +5189,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4923,7 +5205,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -4937,14 +5219,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4964,14 +5246,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5003,7 +5285,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -5035,7 +5317,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5056,7 +5338,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5067,7 +5349,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5099,7 +5381,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5128,7 +5410,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5154,7 +5436,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -5171,7 +5453,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -5203,7 +5485,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -5213,7 +5495,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -5221,7 +5503,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -5235,7 +5517,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -5245,7 +5527,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -5256,7 +5538,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -5267,7 +5549,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -5275,7 +5557,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5283,7 +5565,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -5294,7 +5576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -5341,7 +5623,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -5352,7 +5634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -5365,16 +5647,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K33" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
007 Gift card testcase for drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="309">
   <si>
     <t>UserName</t>
   </si>
@@ -955,6 +955,12 @@
 Bradford, West Yorkshire, BD109ET
 United Kingdom
 T: 9999999999</t>
+  </si>
+  <si>
+    <t>Partial GiftCode</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_7297</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1375,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL13" sqref="AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -2177,13 +2183,13 @@
     </row>
     <row r="31" spans="1:40">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>307</v>
       </c>
       <c r="AJ31" t="s">
         <v>262</v>
       </c>
       <c r="AK31" s="7" t="s">
-        <v>157</v>
+        <v>308</v>
       </c>
       <c r="AL31" s="7" t="s">
         <v>158</v>
@@ -3012,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
74 Testcase for Drybar EU
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="311">
   <si>
     <t>UserName</t>
   </si>
@@ -961,6 +961,12 @@
   </si>
   <si>
     <t>TEST_DRYBAR_PROMO_7297</t>
+  </si>
+  <si>
+    <t>3d_Secure</t>
+  </si>
+  <si>
+    <t>4000000000003220</t>
   </si>
 </sst>
 </file>
@@ -1379,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN50"/>
+  <dimension ref="A1:AN51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -1773,78 +1779,60 @@
     </row>
     <row r="13" spans="1:40">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U13" s="5"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="5"/>
+        <v>309</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="W13">
+        <v>123</v>
+      </c>
       <c r="AJ13" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:40">
       <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="5"/>
       <c r="AJ14" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:40">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+        <v>32</v>
+      </c>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
-      <c r="U15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="W15">
-        <v>123</v>
-      </c>
       <c r="AJ15" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:40">
       <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16" t="s">
-        <v>49</v>
-      </c>
-      <c r="O16" t="s">
-        <v>50</v>
-      </c>
-      <c r="P16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>51</v>
-      </c>
-      <c r="R16">
-        <v>81504</v>
-      </c>
-      <c r="S16">
-        <v>9898989898</v>
+        <v>14</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="U16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="W16">
+        <v>123</v>
       </c>
       <c r="AJ16" t="s">
         <v>262</v>
@@ -1852,7 +1840,7 @@
     </row>
     <row r="17" spans="1:40">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
         <v>47</v>
@@ -1864,19 +1852,19 @@
         <v>46</v>
       </c>
       <c r="N17" t="s">
-        <v>263</v>
+        <v>49</v>
       </c>
       <c r="O17" t="s">
-        <v>264</v>
+        <v>50</v>
       </c>
       <c r="P17" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="Q17" t="s">
-        <v>265</v>
-      </c>
-      <c r="R17" t="s">
-        <v>267</v>
+        <v>51</v>
+      </c>
+      <c r="R17">
+        <v>81504</v>
       </c>
       <c r="S17">
         <v>9898989898</v>
@@ -1887,32 +1875,42 @@
     </row>
     <row r="18" spans="1:40">
       <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" t="s">
-        <v>65</v>
-      </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" t="s">
+        <v>263</v>
+      </c>
+      <c r="O18" t="s">
+        <v>264</v>
+      </c>
+      <c r="P18" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>265</v>
+      </c>
+      <c r="R18" t="s">
+        <v>267</v>
+      </c>
+      <c r="S18">
+        <v>9898989898</v>
+      </c>
       <c r="AJ18" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:40">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>63</v>
@@ -1920,79 +1918,72 @@
       <c r="I19" t="s">
         <v>64</v>
       </c>
-      <c r="X19" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z19" s="5"/>
+      <c r="J19" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
       <c r="AJ19" t="s">
         <v>262</v>
       </c>
-      <c r="AN19" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="20" spans="1:40">
       <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>78</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N20" t="s">
-        <v>74</v>
-      </c>
-      <c r="O20" t="s">
-        <v>75</v>
-      </c>
-      <c r="P20" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>76</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="S20">
-        <v>9898989898</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>64</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z20" s="5"/>
       <c r="AJ20" t="s">
         <v>262</v>
       </c>
+      <c r="AN20" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="21" spans="1:40">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="N21" t="s">
-        <v>273</v>
+        <v>74</v>
       </c>
       <c r="O21" t="s">
-        <v>274</v>
+        <v>75</v>
       </c>
       <c r="P21" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="Q21" t="s">
-        <v>275</v>
+        <v>76</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>276</v>
+        <v>77</v>
       </c>
       <c r="S21">
         <v>9898989898</v>
@@ -2003,98 +1994,92 @@
     </row>
     <row r="22" spans="1:40">
       <c r="A22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="7"/>
-      <c r="K22" s="2" t="s">
-        <v>86</v>
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
       </c>
       <c r="N22" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="O22" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="P22" t="s">
         <v>266</v>
       </c>
       <c r="Q22" t="s">
-        <v>265</v>
-      </c>
-      <c r="R22" t="s">
-        <v>267</v>
-      </c>
-      <c r="S22" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="2"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="5"/>
+        <v>275</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="S22">
+        <v>9898989898</v>
+      </c>
       <c r="AJ22" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:40">
       <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="X23" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z23" s="5"/>
-      <c r="AA23" t="s">
-        <v>98</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="K23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N23" t="s">
+        <v>263</v>
+      </c>
+      <c r="O23" t="s">
+        <v>264</v>
+      </c>
+      <c r="P23" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>265</v>
+      </c>
+      <c r="R23" t="s">
+        <v>267</v>
+      </c>
+      <c r="S23" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="2"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
       <c r="AJ23" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:40">
       <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" t="s">
-        <v>286</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N24" t="s">
-        <v>100</v>
-      </c>
-      <c r="O24" t="s">
-        <v>101</v>
-      </c>
-      <c r="P24" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>102</v>
-      </c>
-      <c r="R24" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="S24" s="9">
-        <v>9898989898</v>
+        <v>95</v>
+      </c>
+      <c r="X24" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z24" s="5"/>
+      <c r="AA24" t="s">
+        <v>98</v>
       </c>
       <c r="AJ24" t="s">
         <v>262</v>
@@ -2102,53 +2087,74 @@
     </row>
     <row r="25" spans="1:40">
       <c r="A25" t="s">
-        <v>105</v>
-      </c>
-      <c r="M25" t="s">
-        <v>270</v>
-      </c>
-      <c r="R25" s="10"/>
-      <c r="S25" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" t="s">
+        <v>286</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P25" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="S25" s="9">
+        <v>9898989898</v>
+      </c>
       <c r="AJ25" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:40">
       <c r="A26" t="s">
-        <v>293</v>
+        <v>105</v>
       </c>
       <c r="M26" t="s">
-        <v>294</v>
-      </c>
-      <c r="N26" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="R26" s="10"/>
       <c r="S26" s="9"/>
+      <c r="AJ26" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="27" spans="1:40">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>293</v>
       </c>
       <c r="M27" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>262</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="N27" t="s">
+        <v>292</v>
+      </c>
+      <c r="R27" s="10"/>
+      <c r="S27" s="9"/>
     </row>
     <row r="28" spans="1:40">
       <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="U28" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V28" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="W28" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="M28" t="s">
+        <v>107</v>
       </c>
       <c r="AJ28" t="s">
         <v>262</v>
@@ -2156,110 +2162,109 @@
     </row>
     <row r="29" spans="1:40">
       <c r="A29" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>88</v>
+        <v>110</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="V29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="AJ29" t="s">
         <v>262</v>
       </c>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="7"/>
     </row>
     <row r="30" spans="1:40">
       <c r="A30" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>285</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>145</v>
+        <v>114</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="AJ30" t="s">
         <v>262</v>
       </c>
+      <c r="AK30" s="7"/>
+      <c r="AL30" s="7"/>
     </row>
     <row r="31" spans="1:40">
       <c r="A31" t="s">
-        <v>307</v>
+        <v>146</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>145</v>
       </c>
       <c r="AJ31" t="s">
         <v>262</v>
       </c>
-      <c r="AK31" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="AL31" s="7" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="32" spans="1:40">
       <c r="A32" t="s">
-        <v>162</v>
-      </c>
-      <c r="M32" t="s">
-        <v>163</v>
+        <v>307</v>
       </c>
       <c r="AJ32" t="s">
         <v>262</v>
       </c>
+      <c r="AK32" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="AL32" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="33" spans="1:39">
       <c r="A33" t="s">
-        <v>164</v>
-      </c>
-      <c r="X33" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z33" s="5"/>
+        <v>162</v>
+      </c>
+      <c r="M33" t="s">
+        <v>163</v>
+      </c>
       <c r="AJ33" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:39">
       <c r="A34" t="s">
-        <v>167</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" t="s">
-        <v>170</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>168</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="X34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z34" s="5"/>
       <c r="AJ34" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:39">
       <c r="A35" t="s">
-        <v>175</v>
-      </c>
-      <c r="X35" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z35" s="5"/>
-      <c r="AA35" s="5" t="s">
-        <v>98</v>
+        <v>167</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" t="s">
+        <v>170</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="AJ35" t="s">
         <v>262</v>
@@ -2267,23 +2272,17 @@
     </row>
     <row r="36" spans="1:39">
       <c r="A36" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" t="s">
-        <v>177</v>
-      </c>
-      <c r="I36" t="s">
-        <v>178</v>
-      </c>
-      <c r="X36" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="X36" t="s">
+        <v>96</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z36" s="5"/>
       <c r="AA36" s="5" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="AJ36" t="s">
         <v>262</v>
@@ -2291,80 +2290,57 @@
     </row>
     <row r="37" spans="1:39">
       <c r="A37" t="s">
-        <v>181</v>
-      </c>
-      <c r="F37" t="s">
-        <v>79</v>
+        <v>176</v>
+      </c>
+      <c r="H37" t="s">
+        <v>177</v>
+      </c>
+      <c r="I37" t="s">
+        <v>178</v>
+      </c>
+      <c r="X37" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="AJ37" t="s">
         <v>262</v>
       </c>
-      <c r="AK37" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL37" s="7" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="38" spans="1:39">
       <c r="A38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" t="s">
-        <v>184</v>
-      </c>
-      <c r="C38" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" t="s">
-        <v>185</v>
+        <v>181</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
       </c>
       <c r="AJ38" t="s">
         <v>262</v>
       </c>
+      <c r="AK38" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL38" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="39" spans="1:39">
       <c r="A39" t="s">
-        <v>186</v>
-      </c>
-      <c r="F39" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" t="s">
-        <v>80</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="N39" t="s">
-        <v>81</v>
-      </c>
-      <c r="O39" t="s">
-        <v>82</v>
-      </c>
-      <c r="P39" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>83</v>
-      </c>
-      <c r="R39" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S39">
-        <v>9898989898</v>
-      </c>
-      <c r="T39">
-        <v>888888</v>
-      </c>
-      <c r="U39" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V39" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="W39" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
+      </c>
+      <c r="B39" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" t="s">
+        <v>185</v>
       </c>
       <c r="AJ39" t="s">
         <v>262</v>
@@ -2372,19 +2348,46 @@
     </row>
     <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>190</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>169</v>
+        <v>186</v>
+      </c>
+      <c r="F40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" t="s">
+        <v>80</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N40" t="s">
+        <v>81</v>
+      </c>
+      <c r="O40" t="s">
+        <v>82</v>
+      </c>
+      <c r="P40" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>83</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S40">
+        <v>9898989898</v>
+      </c>
+      <c r="T40">
+        <v>888888</v>
+      </c>
+      <c r="U40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V40" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="AJ40" t="s">
         <v>262</v>
@@ -2392,95 +2395,85 @@
     </row>
     <row r="41" spans="1:39">
       <c r="A41" t="s">
-        <v>192</v>
-      </c>
-      <c r="F41" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" t="s">
-        <v>80</v>
-      </c>
-      <c r="N41" t="s">
-        <v>193</v>
-      </c>
-      <c r="O41" t="s">
-        <v>194</v>
-      </c>
-      <c r="P41" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>196</v>
-      </c>
-      <c r="R41" t="s">
-        <v>197</v>
-      </c>
-      <c r="S41">
-        <v>9898989898</v>
+        <v>190</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="AJ41" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:39">
-      <c r="A42" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F42" s="9" t="s">
+      <c r="A42" t="s">
+        <v>192</v>
+      </c>
+      <c r="F42" t="s">
         <v>79</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
+      <c r="G42" t="s">
+        <v>80</v>
+      </c>
+      <c r="N42" t="s">
+        <v>193</v>
+      </c>
+      <c r="O42" t="s">
+        <v>194</v>
+      </c>
+      <c r="P42" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>196</v>
+      </c>
+      <c r="R42" t="s">
+        <v>197</v>
+      </c>
+      <c r="S42">
+        <v>9898989898</v>
+      </c>
       <c r="AJ42" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:39">
       <c r="A43" s="9" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C43" s="9"/>
+        <v>216</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>216</v>
+      </c>
       <c r="D43" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>221</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="AJ43" t="s">
         <v>262</v>
@@ -2488,73 +2481,89 @@
     </row>
     <row r="44" spans="1:39">
       <c r="A44" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="X44" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y44">
-        <v>2</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="M44" s="9"/>
       <c r="AJ44" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
-        <v>258</v>
+        <v>226</v>
+      </c>
+      <c r="X45" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y45">
+        <v>2</v>
       </c>
       <c r="AJ45" t="s">
         <v>262</v>
       </c>
-      <c r="AM45" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="46" spans="1:39">
-      <c r="A46" t="s">
-        <v>147</v>
-      </c>
-      <c r="F46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" t="s">
-        <v>48</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N46" t="s">
-        <v>151</v>
-      </c>
-      <c r="O46" t="s">
-        <v>150</v>
-      </c>
-      <c r="P46" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>148</v>
-      </c>
-      <c r="R46" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="S46">
-        <v>9898989898</v>
+      <c r="A46" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="AJ46" t="s">
         <v>262</v>
       </c>
+      <c r="AM46" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="47" spans="1:39">
-      <c r="A47" s="9" t="s">
-        <v>282</v>
+      <c r="A47" t="s">
+        <v>147</v>
+      </c>
+      <c r="F47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
+        <v>48</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>284</v>
+        <v>46</v>
+      </c>
+      <c r="N47" t="s">
+        <v>151</v>
+      </c>
+      <c r="O47" t="s">
+        <v>150</v>
+      </c>
+      <c r="P47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>148</v>
+      </c>
+      <c r="R47" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="S47">
+        <v>9898989898</v>
       </c>
       <c r="AJ47" t="s">
         <v>262</v>
@@ -2562,89 +2571,103 @@
     </row>
     <row r="48" spans="1:39">
       <c r="A48" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="X48" t="s">
-        <v>288</v>
-      </c>
-      <c r="Y48">
-        <v>2</v>
+        <v>282</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>284</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:40">
       <c r="A49" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>184</v>
       </c>
       <c r="X49" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Y49">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:40">
-      <c r="A50" t="s">
+      <c r="A50" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="X50" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40">
+      <c r="A51" t="s">
         <v>299</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
         <v>63</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I51" t="s">
         <v>64</v>
       </c>
-      <c r="X50" s="5" t="s">
+      <c r="X51" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="Y50" s="5" t="s">
+      <c r="Y51" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z50" s="5"/>
-      <c r="AJ50" t="s">
+      <c r="Z51" s="5"/>
+      <c r="AJ51" t="s">
         <v>262</v>
       </c>
-      <c r="AN50" t="s">
+      <c r="AN51" t="s">
         <v>291</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K16" r:id="rId1"/>
-    <hyperlink ref="K17" r:id="rId2"/>
+    <hyperlink ref="K17" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId2"/>
     <hyperlink ref="D2" r:id="rId3"/>
     <hyperlink ref="E2" r:id="rId4"/>
     <hyperlink ref="C2" r:id="rId5"/>
     <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K20" r:id="rId7"/>
-    <hyperlink ref="K22" r:id="rId8"/>
-    <hyperlink ref="K24" r:id="rId9"/>
-    <hyperlink ref="B34" r:id="rId10"/>
-    <hyperlink ref="D34" r:id="rId11"/>
-    <hyperlink ref="E34" r:id="rId12"/>
-    <hyperlink ref="K34" r:id="rId13"/>
-    <hyperlink ref="K39" r:id="rId14"/>
-    <hyperlink ref="B40" r:id="rId15"/>
-    <hyperlink ref="D40" r:id="rId16"/>
-    <hyperlink ref="E40" r:id="rId17"/>
-    <hyperlink ref="C40" r:id="rId18"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K25" r:id="rId9"/>
+    <hyperlink ref="B35" r:id="rId10"/>
+    <hyperlink ref="D35" r:id="rId11"/>
+    <hyperlink ref="E35" r:id="rId12"/>
+    <hyperlink ref="K35" r:id="rId13"/>
+    <hyperlink ref="K40" r:id="rId14"/>
+    <hyperlink ref="B41" r:id="rId15"/>
+    <hyperlink ref="D41" r:id="rId16"/>
+    <hyperlink ref="E41" r:id="rId17"/>
+    <hyperlink ref="C41" r:id="rId18"/>
     <hyperlink ref="F8" r:id="rId19"/>
     <hyperlink ref="D8" r:id="rId20"/>
     <hyperlink ref="E8" r:id="rId21"/>
-    <hyperlink ref="B42" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C42" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D42" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E42" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K42" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B43" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D43" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E43" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K43" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L43" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K46" r:id="rId32"/>
-    <hyperlink ref="K47" r:id="rId33"/>
-    <hyperlink ref="B48" r:id="rId34"/>
+    <hyperlink ref="B43" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C43" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E43" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K43" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B44" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D44" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E44" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K44" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L44" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K47" r:id="rId32"/>
+    <hyperlink ref="K48" r:id="rId33"/>
+    <hyperlink ref="B49" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
154 Testcase Dryabr UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19E989-C533-4628-9EF3-52B51B71FC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -21,8 +22,8 @@
     <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="313">
   <si>
     <t>UserName</t>
   </si>
@@ -576,9 +577,6 @@
   </si>
   <si>
     <t>GiftCode Full Redeem</t>
-  </si>
-  <si>
-    <t>GLDDRY-QA-TEST-1</t>
   </si>
   <si>
     <t>AccountDetail</t>
@@ -968,15 +966,24 @@
   <si>
     <t>4000000000003220</t>
   </si>
+  <si>
+    <t>Product_2</t>
+  </si>
+  <si>
+    <t>Buttercup Blow-Dryer</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_5759</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1377,49 +1384,49 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ19" sqref="AJ19"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK39" sqref="AK39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="16" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1503,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>97</v>
@@ -1535,13 +1542,13 @@
         <v>156</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1567,19 +1574,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>262</v>
+      </c>
+      <c r="O2" t="s">
         <v>263</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q2" t="s">
         <v>264</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>266</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>265</v>
-      </c>
-      <c r="R2" t="s">
-        <v>267</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -1587,10 +1594,10 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AJ2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1599,10 +1606,10 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AJ3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1611,32 +1618,32 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AJ4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AJ5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -1645,110 +1652,105 @@
         <v>4</v>
       </c>
       <c r="AJ6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="X7" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y7" s="5" t="s">
+      <c r="X7" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="X8" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y8" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="Z7" s="5"/>
-      <c r="AJ7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40">
-      <c r="A8" t="s">
+      <c r="Z8" s="5"/>
+      <c r="AJ8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>153</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="N8" t="s">
-        <v>269</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="K9" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="N9" t="s">
+        <v>268</v>
+      </c>
+      <c r="O9" t="s">
         <v>58</v>
       </c>
-      <c r="P8" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="P9" t="s">
         <v>265</v>
       </c>
-      <c r="R8" t="s">
-        <v>268</v>
-      </c>
-      <c r="S8" s="5" t="s">
+      <c r="Q9" t="s">
+        <v>264</v>
+      </c>
+      <c r="R9" t="s">
+        <v>267</v>
+      </c>
+      <c r="S9" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="AG8" s="8" t="s">
+      <c r="AG9" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="AJ8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40">
-      <c r="A9" t="s">
+      <c r="AJ9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="Y9" s="5">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="Y10" s="5">
         <v>2</v>
       </c>
-      <c r="Z9" s="5"/>
-      <c r="AJ9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40">
-      <c r="A10" t="s">
+      <c r="Z10" s="5"/>
+      <c r="AJ10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="U10" s="5" t="s">
+      <c r="U11" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="V10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="W10">
-        <v>123</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="U11" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>55</v>
@@ -1757,32 +1759,34 @@
         <v>123</v>
       </c>
       <c r="AJ11" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
       <c r="U12" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="W12">
         <v>123</v>
       </c>
       <c r="AJ12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>309</v>
+        <v>28</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>310</v>
+        <v>71</v>
       </c>
       <c r="V13" s="6" t="s">
         <v>72</v>
@@ -1791,91 +1795,73 @@
         <v>123</v>
       </c>
       <c r="AJ13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>308</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="W14">
+        <v>123</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="U14" s="5"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="5"/>
-      <c r="AJ14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40">
-      <c r="A15" t="s">
+      <c r="U15" s="5"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="5"/>
+      <c r="AJ15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="AJ15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="U16" s="5" t="s">
+      <c r="AJ16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="U17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V16" s="5" t="s">
+      <c r="V17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="W16">
+      <c r="W17">
         <v>123</v>
       </c>
-      <c r="AJ16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="1:40">
-      <c r="A17" t="s">
+      <c r="AJ17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" t="s">
-        <v>50</v>
-      </c>
-      <c r="P17" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>51</v>
-      </c>
-      <c r="R17">
-        <v>81504</v>
-      </c>
-      <c r="S17">
-        <v>9898989898</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40">
-      <c r="A18" t="s">
-        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>47</v>
@@ -1887,55 +1873,65 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>263</v>
+        <v>49</v>
       </c>
       <c r="O18" t="s">
-        <v>264</v>
+        <v>50</v>
       </c>
       <c r="P18" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="Q18" t="s">
-        <v>265</v>
-      </c>
-      <c r="R18" t="s">
-        <v>267</v>
+        <v>51</v>
+      </c>
+      <c r="R18">
+        <v>81504</v>
       </c>
       <c r="S18">
         <v>9898989898</v>
       </c>
       <c r="AJ18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="19" spans="1:40">
-      <c r="A19" t="s">
+      <c r="O19" t="s">
+        <v>263</v>
+      </c>
+      <c r="P19" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>264</v>
+      </c>
+      <c r="R19" t="s">
+        <v>266</v>
+      </c>
+      <c r="S19">
+        <v>9898989898</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>63</v>
-      </c>
-      <c r="H19" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AJ19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40">
-      <c r="A20" t="s">
-        <v>66</v>
       </c>
       <c r="H20" t="s">
         <v>63</v>
@@ -1943,731 +1939,756 @@
       <c r="I20" t="s">
         <v>64</v>
       </c>
-      <c r="X20" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y20" s="5" t="s">
+      <c r="J20" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AJ20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" t="s">
+        <v>64</v>
+      </c>
+      <c r="X21" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z20" s="5"/>
-      <c r="AJ20" t="s">
-        <v>262</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40">
-      <c r="A21" t="s">
+      <c r="Z21" s="5"/>
+      <c r="AJ21" t="s">
+        <v>261</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>73</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>48</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N22" t="s">
         <v>74</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>75</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P22" t="s">
         <v>52</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q22" t="s">
         <v>76</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="R22" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="S21">
-        <v>9898989898</v>
-      </c>
-      <c r="AJ21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" t="s">
-        <v>80</v>
-      </c>
-      <c r="N22" t="s">
-        <v>273</v>
-      </c>
-      <c r="O22" t="s">
-        <v>274</v>
-      </c>
-      <c r="P22" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>275</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
       </c>
       <c r="AJ22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+      <c r="N23" t="s">
+        <v>272</v>
+      </c>
+      <c r="O23" t="s">
+        <v>273</v>
+      </c>
+      <c r="P23" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>274</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="S23">
+        <v>9898989898</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="7"/>
+      <c r="K24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N24" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="23" spans="1:40">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="7"/>
-      <c r="K23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="O24" t="s">
         <v>263</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P24" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q24" t="s">
         <v>264</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R24" t="s">
         <v>266</v>
       </c>
-      <c r="Q23" t="s">
-        <v>265</v>
-      </c>
-      <c r="R23" t="s">
-        <v>267</v>
-      </c>
-      <c r="S23" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="2"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-      <c r="AJ23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:40">
-      <c r="A24" t="s">
+      <c r="S24" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="2"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AJ24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>95</v>
       </c>
-      <c r="X24" t="s">
+      <c r="X25" t="s">
         <v>96</v>
       </c>
-      <c r="Y24" s="5" t="s">
+      <c r="Y25" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z24" s="5"/>
-      <c r="AA24" t="s">
+      <c r="Z25" s="5"/>
+      <c r="AA25" t="s">
         <v>98</v>
       </c>
-      <c r="AJ24" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="25" spans="1:40">
-      <c r="A25" t="s">
+      <c r="AJ25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>99</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>79</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>80</v>
       </c>
-      <c r="I25" t="s">
-        <v>286</v>
-      </c>
-      <c r="K25" s="8" t="s">
+      <c r="I26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K26" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N26" t="s">
         <v>100</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O26" t="s">
         <v>101</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P26" t="s">
         <v>52</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q26" t="s">
         <v>102</v>
       </c>
-      <c r="R25" s="11" t="s">
+      <c r="R26" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="S25" s="9">
+      <c r="S26" s="9">
         <v>9898989898</v>
       </c>
-      <c r="AJ25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:40">
-      <c r="A26" t="s">
+      <c r="AJ26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>105</v>
       </c>
-      <c r="M26" t="s">
-        <v>270</v>
-      </c>
-      <c r="R26" s="10"/>
-      <c r="S26" s="9"/>
-      <c r="AJ26" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:40">
-      <c r="A27" t="s">
-        <v>293</v>
-      </c>
       <c r="M27" t="s">
-        <v>294</v>
-      </c>
-      <c r="N27" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
-    </row>
-    <row r="28" spans="1:40">
+      <c r="AJ27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>292</v>
+      </c>
+      <c r="M28" t="s">
+        <v>293</v>
+      </c>
+      <c r="N28" t="s">
+        <v>291</v>
+      </c>
+      <c r="R28" s="10"/>
+      <c r="S28" s="9"/>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>106</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M29" t="s">
         <v>107</v>
       </c>
-      <c r="AJ28" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:40">
-      <c r="A29" t="s">
+      <c r="AJ29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>110</v>
       </c>
-      <c r="U29" s="5" t="s">
+      <c r="U30" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="V29" s="5" t="s">
+      <c r="V30" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="W29" s="5" t="s">
+      <c r="W30" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AJ29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40">
-      <c r="A30" t="s">
+      <c r="AJ30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>114</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="M31" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AJ30" t="s">
-        <v>262</v>
-      </c>
-      <c r="AK30" s="7"/>
-      <c r="AL30" s="7"/>
-    </row>
-    <row r="31" spans="1:40">
-      <c r="A31" t="s">
+      <c r="AJ31" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK31" s="7"/>
+      <c r="AL31" s="7"/>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>146</v>
       </c>
-      <c r="AD31" t="s">
-        <v>285</v>
-      </c>
-      <c r="AE31" t="s">
+      <c r="AD32" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE32" t="s">
         <v>145</v>
       </c>
-      <c r="AJ31" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="32" spans="1:40">
-      <c r="A32" t="s">
+      <c r="AJ32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>306</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK33" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="AJ32" t="s">
-        <v>262</v>
-      </c>
-      <c r="AK32" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="AL32" s="7" t="s">
+      <c r="AL33" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
-      <c r="A33" t="s">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>162</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M34" t="s">
         <v>163</v>
       </c>
-      <c r="AJ33" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="1:39">
-      <c r="A34" t="s">
+      <c r="AJ34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>164</v>
       </c>
-      <c r="X34" t="s">
+      <c r="X35" t="s">
         <v>165</v>
       </c>
-      <c r="Y34" s="5" t="s">
+      <c r="Y35" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z34" s="5"/>
-      <c r="AJ34" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:39">
-      <c r="A35" t="s">
+      <c r="Z35" s="5"/>
+      <c r="AJ35" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>79</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>170</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K36" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="AJ35" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="1:39">
-      <c r="A36" t="s">
+      <c r="AJ36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>175</v>
       </c>
-      <c r="X36" t="s">
+      <c r="X37" t="s">
         <v>96</v>
-      </c>
-      <c r="Y36" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z36" s="5"/>
-      <c r="AA36" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="AJ36" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="37" spans="1:39">
-      <c r="A37" t="s">
-        <v>176</v>
-      </c>
-      <c r="H37" t="s">
-        <v>177</v>
-      </c>
-      <c r="I37" t="s">
-        <v>178</v>
-      </c>
-      <c r="X37" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="Y37" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z37" s="5"/>
       <c r="AA37" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" t="s">
+        <v>177</v>
+      </c>
+      <c r="I38" t="s">
+        <v>178</v>
+      </c>
+      <c r="X38" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="AJ37" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="38" spans="1:39">
-      <c r="A38" t="s">
+      <c r="AJ38" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>181</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="AJ38" t="s">
-        <v>262</v>
-      </c>
-      <c r="AK38" t="s">
+      <c r="AJ39" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>312</v>
+      </c>
+      <c r="AL39" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>182</v>
       </c>
-      <c r="AL38" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:39">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
         <v>183</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" t="s">
         <v>184</v>
       </c>
-      <c r="C39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="AJ40" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>185</v>
       </c>
-      <c r="AJ39" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39">
-      <c r="A40" t="s">
+      <c r="F41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" t="s">
+        <v>80</v>
+      </c>
+      <c r="K41" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="F40" t="s">
+      <c r="N41" t="s">
+        <v>81</v>
+      </c>
+      <c r="O41" t="s">
+        <v>82</v>
+      </c>
+      <c r="P41" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>83</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S41">
+        <v>9898989898</v>
+      </c>
+      <c r="T41">
+        <v>888888</v>
+      </c>
+      <c r="U41" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V41" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="W41" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>191</v>
+      </c>
+      <c r="F43" t="s">
         <v>79</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G43" t="s">
         <v>80</v>
       </c>
-      <c r="K40" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="N40" t="s">
-        <v>81</v>
-      </c>
-      <c r="O40" t="s">
-        <v>82</v>
-      </c>
-      <c r="P40" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>83</v>
-      </c>
-      <c r="R40" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S40">
+      <c r="N43" t="s">
+        <v>192</v>
+      </c>
+      <c r="O43" t="s">
+        <v>193</v>
+      </c>
+      <c r="P43" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>195</v>
+      </c>
+      <c r="R43" t="s">
+        <v>196</v>
+      </c>
+      <c r="S43">
         <v>9898989898</v>
       </c>
-      <c r="T40">
-        <v>888888</v>
-      </c>
-      <c r="U40" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V40" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="W40" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="AJ40" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="41" spans="1:39">
-      <c r="A41" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ41" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="42" spans="1:39">
-      <c r="A42" t="s">
-        <v>192</v>
-      </c>
-      <c r="F42" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" t="s">
-        <v>80</v>
-      </c>
-      <c r="N42" t="s">
-        <v>193</v>
-      </c>
-      <c r="O42" t="s">
-        <v>194</v>
-      </c>
-      <c r="P42" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>196</v>
-      </c>
-      <c r="R42" t="s">
-        <v>197</v>
-      </c>
-      <c r="S42">
-        <v>9898989898</v>
-      </c>
-      <c r="AJ42" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:39">
-      <c r="A43" s="9" t="s">
+      <c r="AJ43" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="AJ43" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="44" spans="1:39">
-      <c r="A44" s="9" t="s">
-        <v>218</v>
-      </c>
       <c r="B44" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C44" s="9"/>
+        <v>215</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="D44" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L44" s="8" t="s">
-        <v>221</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="AJ44" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="45" spans="1:39">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="M45" s="9"/>
+      <c r="AJ45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="X46" t="s">
         <v>226</v>
       </c>
-      <c r="X45" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y45">
+      <c r="Y46">
         <v>2</v>
       </c>
-      <c r="AJ45" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39">
-      <c r="A46" s="9" t="s">
+      <c r="AJ46" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>261</v>
+      </c>
+      <c r="AM47" t="s">
         <v>258</v>
       </c>
-      <c r="AJ46" t="s">
-        <v>262</v>
-      </c>
-      <c r="AM46" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:39">
-      <c r="A47" t="s">
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>147</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>47</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>48</v>
       </c>
-      <c r="K47" s="8" t="s">
+      <c r="K48" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N48" t="s">
         <v>151</v>
       </c>
-      <c r="O47" t="s">
+      <c r="O48" t="s">
         <v>150</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P48" t="s">
         <v>52</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="Q48" t="s">
         <v>148</v>
       </c>
-      <c r="R47" s="10" t="s">
+      <c r="R48" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="S47">
+      <c r="S48">
         <v>9898989898</v>
       </c>
-      <c r="AJ47" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39">
-      <c r="A48" s="9" t="s">
+      <c r="AJ48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="K49" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="K48" s="8" t="s">
+      <c r="AI49" t="s">
         <v>283</v>
       </c>
-      <c r="AI48" t="s">
-        <v>284</v>
-      </c>
-      <c r="AJ48" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="49" spans="1:40">
-      <c r="A49" s="9" t="s">
+      <c r="AJ49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="X50" t="s">
         <v>287</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="X49" t="s">
-        <v>288</v>
-      </c>
-      <c r="Y49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:40">
-      <c r="A50" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="X50" t="s">
-        <v>290</v>
       </c>
       <c r="Y50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:40">
-      <c r="A51" t="s">
-        <v>299</v>
-      </c>
-      <c r="H51" t="s">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="X51" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>298</v>
+      </c>
+      <c r="H52" t="s">
         <v>63</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>64</v>
       </c>
-      <c r="X51" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y51" s="5" t="s">
+      <c r="X52" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y52" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z51" s="5"/>
-      <c r="AJ51" t="s">
-        <v>262</v>
-      </c>
-      <c r="AN51" t="s">
-        <v>291</v>
+      <c r="Z52" s="5"/>
+      <c r="AJ52" t="s">
+        <v>261</v>
+      </c>
+      <c r="AN52" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1"/>
-    <hyperlink ref="K18" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
-    <hyperlink ref="K25" r:id="rId9"/>
-    <hyperlink ref="B35" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="E35" r:id="rId12"/>
-    <hyperlink ref="K35" r:id="rId13"/>
-    <hyperlink ref="K40" r:id="rId14"/>
-    <hyperlink ref="B41" r:id="rId15"/>
-    <hyperlink ref="D41" r:id="rId16"/>
-    <hyperlink ref="E41" r:id="rId17"/>
-    <hyperlink ref="C41" r:id="rId18"/>
-    <hyperlink ref="F8" r:id="rId19"/>
-    <hyperlink ref="D8" r:id="rId20"/>
-    <hyperlink ref="E8" r:id="rId21"/>
-    <hyperlink ref="B43" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C43" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D43" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E43" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K43" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B44" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D44" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E44" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K44" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L44" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K47" r:id="rId32"/>
-    <hyperlink ref="K48" r:id="rId33"/>
-    <hyperlink ref="B49" r:id="rId34"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D36" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E36" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B42" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D42" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E42" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C42" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B44" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C44" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D44" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E44" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K44" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B45" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D45" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E45" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K45" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L45" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K48" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K49" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B50" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2675,16 +2696,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2725,10 +2746,10 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>18</v>
@@ -2737,7 +2758,7 @@
         <v>124</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>21</v>
@@ -2746,19 +2767,19 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2784,39 +2805,39 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" t="s">
         <v>209</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>210</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="M2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>214</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q3" t="s">
         <v>98</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -2824,11 +2845,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2836,29 +2857,29 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2917,7 +2938,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>124</v>
@@ -2947,7 +2968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2970,19 +2991,19 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
+        <v>262</v>
+      </c>
+      <c r="J2" t="s">
         <v>263</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L2" t="s">
         <v>264</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>266</v>
-      </c>
-      <c r="L2" t="s">
-        <v>265</v>
-      </c>
-      <c r="M2" t="s">
-        <v>267</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
@@ -2992,76 +3013,76 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2"/>
       <c r="S3" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U3" t="s">
         <v>98</v>
       </c>
       <c r="V3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>68</v>
       </c>
       <c r="AB3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29">
-      <c r="A4" t="s">
-        <v>279</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>297</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>298</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="AC4" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3102,7 +3123,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>22</v>
@@ -3129,9 +3150,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -3155,22 +3176,22 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" t="s">
         <v>209</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>210</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3181,33 +3202,33 @@
         <v>80</v>
       </c>
       <c r="I3" t="s">
+        <v>301</v>
+      </c>
+      <c r="J3" t="s">
+        <v>273</v>
+      </c>
+      <c r="K3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>302</v>
       </c>
-      <c r="J3" t="s">
-        <v>274</v>
-      </c>
-      <c r="K3" t="s">
-        <v>275</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>303</v>
-      </c>
       <c r="B4" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>61</v>
@@ -3222,9 +3243,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G5" t="s">
         <v>79</v>
@@ -3233,24 +3254,24 @@
         <v>80</v>
       </c>
       <c r="I5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J5" t="s">
+        <v>273</v>
+      </c>
+      <c r="K5" t="s">
         <v>274</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>276</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="187.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G6" t="s">
         <v>79</v>
@@ -3259,56 +3280,56 @@
         <v>80</v>
       </c>
       <c r="I6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J6" t="s">
         <v>209</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>210</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="25" max="25" width="36.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" customWidth="1"/>
-    <col min="28" max="28" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="36.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3349,10 +3370,10 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>18</v>
@@ -3361,7 +3382,7 @@
         <v>124</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>21</v>
@@ -3370,13 +3391,13 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>11</v>
@@ -3388,16 +3409,16 @@
         <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3423,66 +3444,66 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" t="s">
         <v>209</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>210</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="M2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29">
-      <c r="A3" t="s">
-        <v>214</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q3" t="s">
         <v>98</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y4" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Y4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="5" spans="1:29">
-      <c r="A5" t="s">
+      <c r="AB5" t="s">
         <v>233</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>234</v>
       </c>
       <c r="AC5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -3493,45 +3514,45 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="Y4" r:id="rId6"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3566,9 +3587,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>46</v>
@@ -3586,9 +3607,9 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3598,7 +3619,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3607,34 +3628,34 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="18" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>165</v>
@@ -3643,18 +3664,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>165</v>
       </c>
       <c r="H7" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3668,41 +3689,41 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3728,25 +3749,25 @@
         <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>65</v>
@@ -3833,12 +3854,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>46</v>
@@ -3874,12 +3895,12 @@
         <v>60</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3887,7 +3908,7 @@
         <v>177</v>
       </c>
       <c r="I3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P3" s="2"/>
       <c r="S3" s="2"/>
@@ -3900,68 +3921,68 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
       <c r="H4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J4" t="s">
         <v>243</v>
-      </c>
-      <c r="J4" t="s">
-        <v>244</v>
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K5" t="s">
         <v>245</v>
-      </c>
-      <c r="H5" t="s">
-        <v>243</v>
-      </c>
-      <c r="K5" t="s">
-        <v>246</v>
       </c>
       <c r="AF5" s="3"/>
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" t="s">
         <v>247</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>248</v>
-      </c>
-      <c r="L6" t="s">
-        <v>249</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="H7" t="s">
         <v>250</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
         <v>251</v>
-      </c>
-      <c r="M7" t="s">
-        <v>252</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>252</v>
+      </c>
+      <c r="H8" t="s">
         <v>253</v>
-      </c>
-      <c r="H8" t="s">
-        <v>254</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
@@ -3971,22 +3992,22 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H9" t="s">
         <v>255</v>
       </c>
-      <c r="H9" t="s">
+      <c r="O9" t="s">
         <v>256</v>
-      </c>
-      <c r="O9" t="s">
-        <v>257</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -3996,39 +4017,39 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4132,7 +4153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -4148,27 +4169,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4176,7 +4197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -4190,35 +4211,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4292,7 +4313,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -4316,10 +4337,10 @@
         <v>125</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>144</v>
@@ -4343,7 +4364,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4367,10 +4388,10 @@
         <v>132</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>144</v>
@@ -4395,7 +4416,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -4419,10 +4440,10 @@
         <v>135</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>68</v>
@@ -4449,7 +4470,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -4470,33 +4491,33 @@
       </c>
       <c r="H5" s="8"/>
       <c r="K5" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>68</v>
       </c>
       <c r="V6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>139</v>
@@ -4504,38 +4525,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="B5" r:id="rId12"/>
-    <hyperlink ref="C5" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4639,10 +4660,10 @@
         <v>39</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4670,19 +4691,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>262</v>
+      </c>
+      <c r="O2" t="s">
         <v>263</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q2" t="s">
         <v>264</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>266</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>265</v>
-      </c>
-      <c r="R2" t="s">
-        <v>267</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -4690,7 +4711,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4699,18 +4720,18 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4723,7 +4744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4731,14 +4752,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4758,7 +4779,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4769,25 +4790,25 @@
         <v>48</v>
       </c>
       <c r="N9" t="s">
+        <v>208</v>
+      </c>
+      <c r="O9" t="s">
         <v>209</v>
-      </c>
-      <c r="O9" t="s">
-        <v>210</v>
       </c>
       <c r="P9" t="s">
         <v>52</v>
       </c>
       <c r="Q9" t="s">
+        <v>210</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="S9">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4801,25 +4822,25 @@
         <v>46</v>
       </c>
       <c r="N10" t="s">
+        <v>262</v>
+      </c>
+      <c r="O10" t="s">
         <v>263</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q10" t="s">
         <v>264</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>266</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>265</v>
-      </c>
-      <c r="R10" t="s">
-        <v>267</v>
       </c>
       <c r="S10">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4840,7 +4861,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4851,7 +4872,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4862,25 +4883,25 @@
         <v>80</v>
       </c>
       <c r="N13" t="s">
+        <v>208</v>
+      </c>
+      <c r="O13" t="s">
         <v>209</v>
-      </c>
-      <c r="O13" t="s">
-        <v>210</v>
       </c>
       <c r="P13" t="s">
         <v>52</v>
       </c>
       <c r="Q13" t="s">
+        <v>210</v>
+      </c>
+      <c r="R13" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="S13">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4907,7 +4928,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4921,7 +4942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4929,55 +4950,55 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI17" t="s">
         <v>198</v>
       </c>
-      <c r="AI17" t="s">
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="18" spans="1:35">
-      <c r="A18" t="s">
+      <c r="AI18" t="s">
         <v>200</v>
       </c>
-      <c r="AI18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35">
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K2" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5090,7 +5111,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5136,7 +5157,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5145,7 +5166,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5154,7 +5175,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5165,7 +5186,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5178,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -5191,7 +5212,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5204,7 +5225,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5218,7 +5239,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5234,7 +5255,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5248,14 +5269,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5275,14 +5296,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5314,7 +5335,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -5346,7 +5367,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5367,7 +5388,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5378,7 +5399,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5410,7 +5431,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5439,7 +5460,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5465,7 +5486,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -5482,7 +5503,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -5514,7 +5535,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -5524,7 +5545,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -5532,7 +5553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -5546,7 +5567,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -5556,7 +5577,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -5567,7 +5588,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -5578,7 +5599,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -5586,7 +5607,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5594,7 +5615,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -5605,9 +5626,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F33" t="s">
         <v>79</v>
@@ -5616,7 +5637,7 @@
         <v>80</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N33" t="s">
         <v>81</v>
@@ -5643,32 +5664,32 @@
         <v>54</v>
       </c>
       <c r="V33" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="W33" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="W33" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="AI33" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y34" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>68</v>
@@ -5676,16 +5697,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K19" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K33" r:id="rId10"/>
+    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
152 - Drybar UK test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19E989-C533-4628-9EF3-52B51B71FC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DAFF68-8F30-407D-8E69-11B549721EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1394,39 +1394,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK39" sqref="AK39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="16" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1548,21 +1548,21 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -1597,7 +1597,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>310</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>308</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>292</v>
       </c>
@@ -2170,7 +2170,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2211,7 +2211,7 @@
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>146</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>306</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>162</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>167</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>175</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>176</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>182</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>167</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>217</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>225</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>257</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>281</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>286</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>288</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>298</v>
       </c>
@@ -2703,9 +2703,9 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -2864,22 +2864,22 @@
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>278</v>
       </c>
@@ -3066,23 +3066,23 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>276</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>302</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>303</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>304</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
@@ -3320,16 +3320,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" customWidth="1"/>
-    <col min="28" max="28" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3540,19 +3540,19 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>276</v>
       </c>
@@ -3607,7 +3607,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>277</v>
       </c>
@@ -3619,7 +3619,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>278</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>234</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>278</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3717,13 +3717,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3900,7 +3900,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3921,7 +3921,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3935,7 +3935,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -3949,7 +3949,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -3962,7 +3962,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -3977,7 +3977,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -4007,7 +4007,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4017,7 +4017,7 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
@@ -4040,16 +4040,16 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -4183,13 +4183,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -4218,28 +4218,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4512,7 +4512,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4551,12 +4551,12 @@
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4720,7 +4720,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4752,14 +4752,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4861,7 +4861,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4928,7 +4928,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>197</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>199</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
@@ -4992,13 +4992,13 @@
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5157,7 +5157,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5166,7 +5166,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5175,7 +5175,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5269,14 +5269,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5296,14 +5296,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5388,7 +5388,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5486,7 +5486,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -5545,7 +5545,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -5577,7 +5577,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>185</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>221</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>222</v>
       </c>

</xml_diff>

<commit_message>
Gold Drybar Uk Add to cart issue Test data & helper updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DAFF68-8F30-407D-8E69-11B549721EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC93552-58FA-45F4-8025-6C74F9785A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="314">
   <si>
     <t>UserName</t>
   </si>
@@ -974,6 +974,9 @@
   </si>
   <si>
     <t>TEST_DRYBAR_PROMO_5759</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All Hair Tools</t>
   </si>
 </sst>
 </file>
@@ -1394,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1905,7 +1908,7 @@
         <v>48</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="N19" t="s">
         <v>262</v>
@@ -1934,10 +1937,10 @@
         <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>313</v>
       </c>
       <c r="J20" t="s">
         <v>65</v>
@@ -1959,13 +1962,13 @@
         <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>313</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>68</v>
@@ -4037,7 +4040,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4214,7 +4217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -4547,8 +4550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4848,7 +4851,7 @@
         <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>313</v>
       </c>
       <c r="J11" t="s">
         <v>65</v>
@@ -4932,8 +4935,8 @@
       <c r="A15" t="s">
         <v>95</v>
       </c>
-      <c r="X15" t="s">
-        <v>96</v>
+      <c r="X15" s="5" t="s">
+        <v>311</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
181 testcase for drybar EU
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC93552-58FA-45F4-8025-6C74F9785A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,8 +21,8 @@
     <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="316">
   <si>
     <t>UserName</t>
   </si>
@@ -978,15 +977,21 @@
   <si>
     <t xml:space="preserve"> All Hair Tools</t>
   </si>
+  <si>
+    <t>Partial GiftCode1</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_3484</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1387,21 +1392,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1429,7 +1434,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1556,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1600,7 +1605,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1612,7 +1617,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1624,7 +1629,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1639,7 +1644,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1658,7 +1663,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40">
       <c r="A7" t="s">
         <v>310</v>
       </c>
@@ -1672,7 +1677,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -1689,7 +1694,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1734,7 +1739,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1748,7 +1753,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1765,7 +1770,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1801,7 +1806,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40">
       <c r="A14" t="s">
         <v>308</v>
       </c>
@@ -1818,7 +1823,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1829,7 +1834,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1839,7 +1844,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1867,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1897,7 +1902,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1932,7 +1937,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1981,7 +1986,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -2016,7 +2021,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2048,7 +2053,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -2091,7 +2096,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -2109,7 +2114,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2147,7 +2152,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2160,7 +2165,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40">
       <c r="A28" t="s">
         <v>292</v>
       </c>
@@ -2173,7 +2178,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -2184,7 +2189,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2201,7 +2206,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2214,7 +2219,7 @@
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40">
       <c r="A32" t="s">
         <v>146</v>
       </c>
@@ -2228,7 +2233,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>306</v>
       </c>
@@ -2242,456 +2247,468 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
-        <v>162</v>
-      </c>
-      <c r="M34" t="s">
-        <v>163</v>
+        <v>314</v>
       </c>
       <c r="AJ34" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AK34" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="AL34" s="7"/>
+    </row>
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
-        <v>164</v>
-      </c>
-      <c r="X35" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z35" s="5"/>
+        <v>162</v>
+      </c>
+      <c r="M35" t="s">
+        <v>163</v>
+      </c>
       <c r="AJ35" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
-        <v>167</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" t="s">
-        <v>170</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>168</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="X36" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z36" s="5"/>
       <c r="AJ36" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
-        <v>175</v>
-      </c>
-      <c r="X37" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5" t="s">
-        <v>98</v>
+        <v>167</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" t="s">
+        <v>170</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="AJ37" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
-        <v>176</v>
-      </c>
-      <c r="H38" t="s">
-        <v>177</v>
-      </c>
-      <c r="I38" t="s">
-        <v>178</v>
-      </c>
-      <c r="X38" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="X38" t="s">
+        <v>96</v>
       </c>
       <c r="Y38" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Z38" s="5"/>
       <c r="AA38" s="5" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="AJ38" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" t="s">
-        <v>79</v>
+        <v>176</v>
+      </c>
+      <c r="H39" t="s">
+        <v>177</v>
+      </c>
+      <c r="I39" t="s">
+        <v>178</v>
+      </c>
+      <c r="X39" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="AJ39" t="s">
         <v>261</v>
       </c>
-      <c r="AK39" t="s">
-        <v>312</v>
-      </c>
-      <c r="AL39" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>182</v>
-      </c>
-      <c r="B40" t="s">
-        <v>183</v>
-      </c>
-      <c r="C40" t="s">
-        <v>183</v>
-      </c>
-      <c r="D40" t="s">
-        <v>184</v>
+        <v>181</v>
+      </c>
+      <c r="F40" t="s">
+        <v>79</v>
       </c>
       <c r="AJ40" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AK40" t="s">
+        <v>312</v>
+      </c>
+      <c r="AL40" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
-        <v>185</v>
-      </c>
-      <c r="F41" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" t="s">
-        <v>80</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="N41" t="s">
-        <v>81</v>
-      </c>
-      <c r="O41" t="s">
-        <v>82</v>
-      </c>
-      <c r="P41" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>83</v>
-      </c>
-      <c r="R41" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S41">
-        <v>9898989898</v>
-      </c>
-      <c r="T41">
-        <v>888888</v>
-      </c>
-      <c r="U41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V41" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="W41" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
+      </c>
+      <c r="B41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D41" t="s">
+        <v>184</v>
       </c>
       <c r="AJ41" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39">
       <c r="A42" t="s">
-        <v>189</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>169</v>
+        <v>185</v>
+      </c>
+      <c r="F42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" t="s">
+        <v>80</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="N42" t="s">
+        <v>81</v>
+      </c>
+      <c r="O42" t="s">
+        <v>82</v>
+      </c>
+      <c r="P42" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>83</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S42">
+        <v>9898989898</v>
+      </c>
+      <c r="T42">
+        <v>888888</v>
+      </c>
+      <c r="U42" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V42" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="W42" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="AJ42" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39">
       <c r="A43" t="s">
-        <v>191</v>
-      </c>
-      <c r="F43" t="s">
-        <v>79</v>
-      </c>
-      <c r="G43" t="s">
-        <v>80</v>
-      </c>
-      <c r="N43" t="s">
-        <v>192</v>
-      </c>
-      <c r="O43" t="s">
-        <v>193</v>
-      </c>
-      <c r="P43" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>195</v>
-      </c>
-      <c r="R43" t="s">
-        <v>196</v>
-      </c>
-      <c r="S43">
-        <v>9898989898</v>
+        <v>189</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="AJ43" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F44" s="9" t="s">
+    <row r="44" spans="1:39">
+      <c r="A44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F44" t="s">
         <v>79</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
+      <c r="G44" t="s">
+        <v>80</v>
+      </c>
+      <c r="N44" t="s">
+        <v>192</v>
+      </c>
+      <c r="O44" t="s">
+        <v>193</v>
+      </c>
+      <c r="P44" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>195</v>
+      </c>
+      <c r="R44" t="s">
+        <v>196</v>
+      </c>
+      <c r="S44">
+        <v>9898989898</v>
+      </c>
       <c r="AJ44" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="C45" s="9"/>
+        <v>215</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="D45" s="8" t="s">
         <v>169</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>220</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="AJ45" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39">
       <c r="A46" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="X46" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y46">
-        <v>2</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="M46" s="9"/>
       <c r="AJ46" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39">
       <c r="A47" s="9" t="s">
-        <v>257</v>
+        <v>225</v>
+      </c>
+      <c r="X47" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y47">
+        <v>2</v>
       </c>
       <c r="AJ47" t="s">
         <v>261</v>
       </c>
-      <c r="AM47" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>147</v>
-      </c>
-      <c r="F48" t="s">
-        <v>47</v>
-      </c>
-      <c r="G48" t="s">
-        <v>48</v>
-      </c>
-      <c r="K48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N48" t="s">
-        <v>151</v>
-      </c>
-      <c r="O48" t="s">
-        <v>150</v>
-      </c>
-      <c r="P48" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>148</v>
-      </c>
-      <c r="R48" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="S48">
-        <v>9898989898</v>
+    </row>
+    <row r="48" spans="1:39">
+      <c r="A48" s="9" t="s">
+        <v>257</v>
       </c>
       <c r="AJ48" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>281</v>
+      <c r="AM48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40">
+      <c r="A49" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" t="s">
+        <v>48</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI49" t="s">
-        <v>283</v>
+        <v>46</v>
+      </c>
+      <c r="N49" t="s">
+        <v>151</v>
+      </c>
+      <c r="O49" t="s">
+        <v>150</v>
+      </c>
+      <c r="P49" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>148</v>
+      </c>
+      <c r="R49" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="S49">
+        <v>9898989898</v>
       </c>
       <c r="AJ49" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:40">
       <c r="A50" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>283</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40">
+      <c r="A51" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="X50" t="s">
+      <c r="X51" t="s">
         <v>287</v>
-      </c>
-      <c r="Y50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="X51" t="s">
-        <v>289</v>
       </c>
       <c r="Y51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:40">
+      <c r="A52" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="X52" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:40">
+      <c r="A53" t="s">
         <v>298</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" t="s">
         <v>63</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" t="s">
         <v>64</v>
       </c>
-      <c r="X52" s="5" t="s">
+      <c r="X53" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="Y52" s="5" t="s">
+      <c r="Y53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z52" s="5"/>
-      <c r="AJ52" t="s">
+      <c r="Z53" s="5"/>
+      <c r="AJ53" t="s">
         <v>261</v>
       </c>
-      <c r="AN52" t="s">
+      <c r="AN53" t="s">
         <v>290</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D36" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E36" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B42" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D42" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E42" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C42" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B44" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C44" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D44" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E44" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K44" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B45" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D45" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E45" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K45" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L45" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K48" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K49" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B50" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K19" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K22" r:id="rId7"/>
+    <hyperlink ref="K24" r:id="rId8"/>
+    <hyperlink ref="K26" r:id="rId9"/>
+    <hyperlink ref="B37" r:id="rId10"/>
+    <hyperlink ref="D37" r:id="rId11"/>
+    <hyperlink ref="E37" r:id="rId12"/>
+    <hyperlink ref="K37" r:id="rId13"/>
+    <hyperlink ref="K42" r:id="rId14"/>
+    <hyperlink ref="B43" r:id="rId15"/>
+    <hyperlink ref="D43" r:id="rId16"/>
+    <hyperlink ref="E43" r:id="rId17"/>
+    <hyperlink ref="C43" r:id="rId18"/>
+    <hyperlink ref="F9" r:id="rId19"/>
+    <hyperlink ref="D9" r:id="rId20"/>
+    <hyperlink ref="E9" r:id="rId21"/>
+    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K49" r:id="rId32"/>
+    <hyperlink ref="K50" r:id="rId33"/>
+    <hyperlink ref="B51" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2699,16 +2716,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2782,7 +2799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2823,7 +2840,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -2848,11 +2865,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2860,14 +2877,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
@@ -2882,7 +2899,7 @@
     <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2971,7 +2988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3016,7 +3033,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3037,7 +3054,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>278</v>
       </c>
@@ -3050,26 +3067,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="AC4" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -3085,7 +3102,7 @@
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3153,7 +3170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>276</v>
       </c>
@@ -3194,7 +3211,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3220,7 +3237,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>302</v>
       </c>
@@ -3246,7 +3263,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>303</v>
       </c>
@@ -3272,7 +3289,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="187.2">
       <c r="A6" t="s">
         <v>304</v>
       </c>
@@ -3301,29 +3318,29 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
-    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -3332,7 +3349,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3421,7 +3438,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3462,7 +3479,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3485,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -3493,7 +3510,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -3504,7 +3521,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -3517,33 +3534,33 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -3555,7 +3572,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3590,7 +3607,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
         <v>276</v>
       </c>
@@ -3610,7 +3627,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>277</v>
       </c>
@@ -3622,7 +3639,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3638,7 +3655,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
         <v>278</v>
       </c>
@@ -3656,7 +3673,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
         <v>234</v>
       </c>
@@ -3667,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
         <v>278</v>
       </c>
@@ -3678,7 +3695,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3692,7 +3709,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -3702,31 +3719,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3857,7 +3874,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3903,7 +3920,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3924,7 +3941,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3938,7 +3955,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -3952,7 +3969,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -3965,7 +3982,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -3980,7 +3997,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -3995,7 +4012,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -4010,7 +4027,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4020,30 +4037,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -4052,7 +4069,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4156,7 +4173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -4172,27 +4189,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4200,7 +4217,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -4214,14 +4231,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -4242,7 +4259,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4316,7 +4333,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -4367,7 +4384,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4419,7 +4436,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -4473,7 +4490,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -4500,7 +4517,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4515,7 +4532,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4528,38 +4545,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4666,7 +4683,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4714,7 +4731,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4723,7 +4740,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4734,7 +4751,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4747,7 +4764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4755,14 +4772,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4782,7 +4799,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4811,7 +4828,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4843,7 +4860,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4864,7 +4881,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -4875,7 +4892,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4904,7 +4921,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -4931,7 +4948,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -4945,7 +4962,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4953,7 +4970,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>197</v>
       </c>
@@ -4961,7 +4978,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>199</v>
       </c>
@@ -4969,39 +4986,39 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5114,7 +5131,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5160,7 +5177,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5169,7 +5186,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5178,7 +5195,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5189,7 +5206,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5202,7 +5219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -5215,7 +5232,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5228,7 +5245,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5242,7 +5259,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5258,7 +5275,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5272,14 +5289,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5299,14 +5316,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5338,7 +5355,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -5370,7 +5387,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5391,7 +5408,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5402,7 +5419,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5434,7 +5451,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5463,7 +5480,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5489,7 +5506,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -5506,7 +5523,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -5538,7 +5555,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -5548,7 +5565,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -5556,7 +5573,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -5570,7 +5587,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -5580,7 +5597,7 @@
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -5591,7 +5608,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -5602,7 +5619,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -5610,7 +5627,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5618,7 +5635,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>173</v>
       </c>
@@ -5629,7 +5646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>185</v>
       </c>
@@ -5676,7 +5693,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
         <v>221</v>
       </c>
@@ -5687,7 +5704,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
         <v>222</v>
       </c>
@@ -5700,16 +5717,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="K23" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K33" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel changes for EU
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="317">
   <si>
     <t>UserName</t>
   </si>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -2071,6 +2071,9 @@
       <c r="K24" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="M24" t="s">
+        <v>293</v>
+      </c>
       <c r="N24" t="s">
         <v>262</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>106</v>
       </c>
       <c r="M29" t="s">
-        <v>107</v>
+        <v>293</v>
       </c>
       <c r="AJ29" t="s">
         <v>261</v>
@@ -2723,7 +2726,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
83 testcase for drybar UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="316">
   <si>
     <t>UserName</t>
   </si>
@@ -191,9 +191,6 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Standard (5 - 7 Business Days)</t>
-  </si>
-  <si>
     <t>4242424242424242</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
   </si>
   <si>
     <t>Bundle Product</t>
-  </si>
-  <si>
-    <t>The Ready to Refresh Special Value Set Hover Image</t>
   </si>
   <si>
     <t>Sticky Cart Product</t>
@@ -985,6 +979,9 @@
   </si>
   <si>
     <t>Double Pint Large Round Ceramic Brush</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo Bundle Test</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1392,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1405,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -1460,13 +1457,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -1514,10 +1511,10 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>22</v>
@@ -1544,19 +1541,19 @@
         <v>39</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="AM1" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:40">
@@ -1564,16 +1561,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -1585,19 +1582,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>260</v>
+      </c>
+      <c r="O2" t="s">
+        <v>261</v>
+      </c>
+      <c r="P2" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q2" t="s">
         <v>262</v>
       </c>
-      <c r="O2" t="s">
-        <v>263</v>
-      </c>
-      <c r="P2" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>264</v>
-      </c>
-      <c r="R2" t="s">
-        <v>266</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -1605,7 +1602,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AJ2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:40">
@@ -1617,7 +1614,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AJ3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -1629,7 +1626,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AJ4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:40">
@@ -1637,14 +1634,14 @@
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AJ5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:40">
@@ -1654,7 +1651,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -1663,17 +1660,17 @@
         <v>4</v>
       </c>
       <c r="AJ6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:40">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Y7" s="5">
         <v>2</v>
@@ -1682,19 +1679,19 @@
     </row>
     <row r="8" spans="1:40">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Z8" s="5"/>
       <c r="AJ8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:40">
@@ -1702,44 +1699,44 @@
         <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="F9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="s">
         <v>152</v>
       </c>
-      <c r="G9" t="s">
-        <v>153</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L9" s="2"/>
       <c r="N9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="O9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P9" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>262</v>
+      </c>
+      <c r="R9" t="s">
         <v>265</v>
       </c>
-      <c r="Q9" t="s">
-        <v>264</v>
-      </c>
-      <c r="R9" t="s">
-        <v>267</v>
-      </c>
       <c r="S9" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG9" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AJ9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:40">
@@ -1753,7 +1750,7 @@
       </c>
       <c r="Z10" s="5"/>
       <c r="AJ10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:40">
@@ -1761,16 +1758,16 @@
         <v>26</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W11">
         <v>123</v>
       </c>
       <c r="AJ11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:40">
@@ -1780,16 +1777,16 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="U12" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W12">
         <v>123</v>
       </c>
       <c r="AJ12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:40">
@@ -1797,33 +1794,33 @@
         <v>28</v>
       </c>
       <c r="U13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="V13" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="W13">
         <v>123</v>
       </c>
       <c r="AJ13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:40">
       <c r="A14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W14">
         <v>123</v>
       </c>
       <c r="AJ14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:40">
@@ -1834,7 +1831,7 @@
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
       <c r="AJ15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:40">
@@ -1844,7 +1841,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="AJ16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:40">
@@ -1858,16 +1855,16 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="U17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V17" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="V17" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="W17">
         <v>123</v>
       </c>
       <c r="AJ17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:40">
@@ -1902,12 +1899,12 @@
         <v>9898989898</v>
       </c>
       <c r="AJ18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:40">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -1916,42 +1913,42 @@
         <v>48</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N19" t="s">
+        <v>260</v>
+      </c>
+      <c r="O19" t="s">
+        <v>261</v>
+      </c>
+      <c r="P19" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q19" t="s">
         <v>262</v>
       </c>
-      <c r="O19" t="s">
-        <v>263</v>
-      </c>
-      <c r="P19" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>264</v>
-      </c>
-      <c r="R19" t="s">
-        <v>266</v>
       </c>
       <c r="S19">
         <v>9898989898</v>
       </c>
       <c r="AJ19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:40">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
@@ -1962,66 +1959,66 @@
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
       <c r="AJ20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:40">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I21" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z21" s="5"/>
       <c r="AJ21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AN21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:40">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
         <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>46</v>
       </c>
       <c r="N22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O22" t="s">
         <v>74</v>
-      </c>
-      <c r="O22" t="s">
-        <v>75</v>
       </c>
       <c r="P22" t="s">
         <v>52</v>
       </c>
       <c r="Q22" t="s">
+        <v>75</v>
+      </c>
+      <c r="R22" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
       </c>
       <c r="AJ22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:40">
@@ -2029,68 +2026,68 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
         <v>79</v>
       </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
       <c r="N23" t="s">
+        <v>270</v>
+      </c>
+      <c r="O23" t="s">
+        <v>271</v>
+      </c>
+      <c r="P23" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q23" t="s">
         <v>272</v>
       </c>
-      <c r="O23" t="s">
+      <c r="R23" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="P23" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>274</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>275</v>
       </c>
       <c r="S23">
         <v>9898989898</v>
       </c>
       <c r="AJ23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:40">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="7"/>
       <c r="K24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N24" t="s">
+        <v>260</v>
+      </c>
+      <c r="O24" t="s">
+        <v>261</v>
+      </c>
+      <c r="P24" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q24" t="s">
         <v>262</v>
       </c>
-      <c r="O24" t="s">
-        <v>263</v>
-      </c>
-      <c r="P24" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>264</v>
       </c>
-      <c r="R24" t="s">
-        <v>266</v>
-      </c>
       <c r="S24" s="22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
@@ -2099,327 +2096,327 @@
       <c r="AE24" s="5"/>
       <c r="AF24" s="5"/>
       <c r="AJ24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:40">
       <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="X25" t="s">
         <v>95</v>
       </c>
-      <c r="X25" t="s">
-        <v>96</v>
-      </c>
       <c r="Y25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z25" s="5"/>
       <c r="AA25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AJ25" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:40">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" t="s">
         <v>79</v>
       </c>
-      <c r="G26" t="s">
-        <v>80</v>
-      </c>
       <c r="I26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>46</v>
       </c>
       <c r="N26" t="s">
+        <v>99</v>
+      </c>
+      <c r="O26" t="s">
         <v>100</v>
-      </c>
-      <c r="O26" t="s">
-        <v>101</v>
       </c>
       <c r="P26" t="s">
         <v>52</v>
       </c>
       <c r="Q26" t="s">
+        <v>101</v>
+      </c>
+      <c r="R26" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="S26" s="9">
         <v>9898989898</v>
       </c>
       <c r="AJ26" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:40">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M27" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
       <c r="AJ27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:40">
       <c r="A28" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M28" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N28" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="1:40">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AJ29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:40">
       <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="U30" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="U30" s="5" t="s">
+      <c r="V30" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="V30" s="5" t="s">
+      <c r="W30" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="W30" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="AJ30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:40">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AJ31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
     <row r="32" spans="1:40">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AE32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:39">
       <c r="A33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AJ33" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AK33" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AL33" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:39">
       <c r="A34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AJ34" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AK34" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AL34" s="7"/>
     </row>
     <row r="35" spans="1:39">
       <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="M35" t="s">
         <v>162</v>
       </c>
-      <c r="M35" t="s">
-        <v>163</v>
-      </c>
       <c r="AJ35" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:39">
       <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="X36" t="s">
         <v>164</v>
       </c>
-      <c r="X36" t="s">
-        <v>165</v>
-      </c>
       <c r="Y36" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z36" s="5"/>
       <c r="AJ36" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:39">
       <c r="A37" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" t="s">
         <v>169</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" t="s">
-        <v>170</v>
-      </c>
       <c r="K37" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AJ37" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:39">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="X38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y38" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z38" s="5"/>
       <c r="AA38" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AJ38" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:39">
       <c r="A39" t="s">
+        <v>174</v>
+      </c>
+      <c r="H39" t="s">
+        <v>175</v>
+      </c>
+      <c r="I39" t="s">
         <v>176</v>
       </c>
-      <c r="H39" t="s">
+      <c r="X39" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="I39" t="s">
-        <v>178</v>
-      </c>
-      <c r="X39" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="Y39" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z39" s="5"/>
       <c r="AA39" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AJ39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AJ40" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AK40" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AL40" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:39">
       <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" t="s">
         <v>182</v>
       </c>
-      <c r="B41" t="s">
-        <v>183</v>
-      </c>
-      <c r="C41" t="s">
-        <v>183</v>
-      </c>
-      <c r="D41" t="s">
-        <v>184</v>
-      </c>
       <c r="AJ41" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:39">
       <c r="A42" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F42" t="s">
+        <v>78</v>
+      </c>
+      <c r="G42" t="s">
         <v>79</v>
       </c>
-      <c r="G42" t="s">
+      <c r="K42" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N42" t="s">
         <v>80</v>
       </c>
-      <c r="K42" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
         <v>81</v>
-      </c>
-      <c r="O42" t="s">
-        <v>82</v>
       </c>
       <c r="P42" t="s">
         <v>52</v>
       </c>
       <c r="Q42" t="s">
+        <v>82</v>
+      </c>
+      <c r="R42" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="R42" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="S42">
         <v>9898989898</v>
@@ -2428,117 +2425,117 @@
         <v>888888</v>
       </c>
       <c r="U42" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V42" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="W42" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AJ42" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:39">
       <c r="A43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AJ43" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:39">
       <c r="A44" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N44" t="s">
+        <v>190</v>
+      </c>
+      <c r="O44" t="s">
         <v>191</v>
       </c>
-      <c r="F44" t="s">
-        <v>79</v>
-      </c>
-      <c r="G44" t="s">
-        <v>80</v>
-      </c>
-      <c r="N44" t="s">
+      <c r="P44" t="s">
         <v>192</v>
       </c>
-      <c r="O44" t="s">
+      <c r="Q44" t="s">
         <v>193</v>
       </c>
-      <c r="P44" t="s">
+      <c r="R44" t="s">
         <v>194</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>195</v>
-      </c>
-      <c r="R44" t="s">
-        <v>196</v>
       </c>
       <c r="S44">
         <v>9898989898</v>
       </c>
       <c r="AJ44" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D45" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="AJ45" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:39">
       <c r="A46" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -2549,41 +2546,41 @@
         <v>46</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M46" s="9"/>
       <c r="AJ46" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:39">
       <c r="A47" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="X47" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Y47">
         <v>2</v>
       </c>
       <c r="AJ47" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:39">
       <c r="A48" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AJ48" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AM48" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:40">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F49" t="s">
         <v>47</v>
@@ -2595,50 +2592,50 @@
         <v>46</v>
       </c>
       <c r="N49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P49" t="s">
         <v>52</v>
       </c>
       <c r="Q49" t="s">
+        <v>147</v>
+      </c>
+      <c r="R49" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="R49" s="10" t="s">
-        <v>149</v>
       </c>
       <c r="S49">
         <v>9898989898</v>
       </c>
       <c r="AJ49" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:40">
       <c r="A50" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI50" t="s">
         <v>281</v>
       </c>
-      <c r="K50" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI50" t="s">
-        <v>283</v>
-      </c>
       <c r="AJ50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:40">
       <c r="A51" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="X51" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="Y51">
         <v>2</v>
@@ -2646,10 +2643,10 @@
     </row>
     <row r="52" spans="1:40">
       <c r="A52" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="X52" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="Y52">
         <v>2</v>
@@ -2657,26 +2654,26 @@
     </row>
     <row r="53" spans="1:40">
       <c r="A53" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H53" t="s">
+        <v>62</v>
+      </c>
+      <c r="I53" t="s">
         <v>63</v>
       </c>
-      <c r="I53" t="s">
-        <v>64</v>
-      </c>
       <c r="X53" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Y53" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z53" s="5"/>
       <c r="AJ53" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AN53" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2772,19 +2769,19 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>21</v>
@@ -2793,13 +2790,13 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>11</v>
@@ -2819,51 +2816,51 @@
         <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
-        <v>80</v>
-      </c>
       <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K2" t="s">
         <v>208</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -2928,7 +2925,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -2949,25 +2946,25 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>21</v>
@@ -3005,31 +3002,31 @@
         <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
       <c r="I2" t="s">
+        <v>260</v>
+      </c>
+      <c r="J2" t="s">
+        <v>261</v>
+      </c>
+      <c r="K2" t="s">
+        <v>263</v>
+      </c>
+      <c r="L2" t="s">
         <v>262</v>
       </c>
-      <c r="J2" t="s">
-        <v>263</v>
-      </c>
-      <c r="K2" t="s">
-        <v>265</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>264</v>
-      </c>
-      <c r="M2" t="s">
-        <v>266</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
@@ -3045,30 +3042,30 @@
       </c>
       <c r="B3" s="2"/>
       <c r="S3" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="U3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AB4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3149,13 +3146,13 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>21</v>
@@ -3178,7 +3175,7 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -3190,31 +3187,31 @@
         <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
-        <v>80</v>
-      </c>
       <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K2" t="s">
         <v>208</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="K2" t="s">
-        <v>210</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -3222,106 +3219,106 @@
         <v>32</v>
       </c>
       <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" t="s">
-        <v>80</v>
-      </c>
       <c r="I3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J3" t="s">
+        <v>271</v>
+      </c>
+      <c r="K3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="K3" t="s">
-        <v>274</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>275</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
         <v>79</v>
-      </c>
-      <c r="H4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
         <v>79</v>
       </c>
-      <c r="H5" t="s">
-        <v>80</v>
-      </c>
       <c r="I5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="K5" t="s">
-        <v>274</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>275</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="187.2">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" t="s">
         <v>79</v>
       </c>
-      <c r="H6" t="s">
-        <v>80</v>
-      </c>
       <c r="I6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J6" t="s">
+        <v>207</v>
+      </c>
+      <c r="K6" t="s">
         <v>208</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="K6" t="s">
-        <v>210</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -3396,19 +3393,19 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>21</v>
@@ -3417,13 +3414,13 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>11</v>
@@ -3435,13 +3432,13 @@
         <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -3458,51 +3455,51 @@
         <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
-        <v>80</v>
-      </c>
       <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K2" t="s">
         <v>208</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -3510,34 +3507,34 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AB5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AC5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="Y6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -3604,18 +3601,18 @@
         <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>46</v>
@@ -3627,7 +3624,7 @@
         <v>46</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
@@ -3635,7 +3632,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3654,37 +3651,37 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3692,35 +3689,35 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" t="s">
         <v>278</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
       </c>
-      <c r="I8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>64</v>
-      </c>
-      <c r="K8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3772,31 +3769,31 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>13</v>
@@ -3844,7 +3841,7 @@
         <v>24</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>22</v>
@@ -3871,13 +3868,13 @@
         <v>39</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AP1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:47">
@@ -3885,16 +3882,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -3906,35 +3903,35 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" t="s">
         <v>57</v>
-      </c>
-      <c r="U2" t="s">
-        <v>58</v>
       </c>
       <c r="V2" t="s">
         <v>52</v>
       </c>
       <c r="W2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="Y2" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
     <row r="3" spans="1:47">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P3" s="2"/>
       <c r="S3" s="2"/>
@@ -3949,13 +3946,13 @@
     </row>
     <row r="4" spans="1:47">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="4"/>
@@ -3963,13 +3960,13 @@
     </row>
     <row r="5" spans="1:47">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AF5" s="3"/>
       <c r="AG5" s="4"/>
@@ -3977,26 +3974,26 @@
     </row>
     <row r="6" spans="1:47">
       <c r="A6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H6" t="s">
+        <v>245</v>
+      </c>
+      <c r="L6" t="s">
         <v>246</v>
-      </c>
-      <c r="H6" t="s">
-        <v>247</v>
-      </c>
-      <c r="L6" t="s">
-        <v>248</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
     <row r="7" spans="1:47">
       <c r="A7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7" t="s">
+        <v>248</v>
+      </c>
+      <c r="M7" t="s">
         <v>249</v>
-      </c>
-      <c r="H7" t="s">
-        <v>250</v>
-      </c>
-      <c r="M7" t="s">
-        <v>251</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Y7" s="7"/>
@@ -4005,10 +4002,10 @@
     </row>
     <row r="8" spans="1:47">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
@@ -4020,13 +4017,13 @@
     </row>
     <row r="9" spans="1:47">
       <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H9" t="s">
+        <v>253</v>
+      </c>
+      <c r="O9" t="s">
         <v>254</v>
-      </c>
-      <c r="H9" t="s">
-        <v>255</v>
-      </c>
-      <c r="O9" t="s">
-        <v>256</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Y9" s="2"/>
@@ -4098,16 +4095,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>42</v>
@@ -4181,10 +4178,10 @@
     </row>
     <row r="2" spans="1:34">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J2" t="s">
         <v>47</v>
@@ -4225,10 +4222,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -4291,13 +4288,13 @@
         <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -4306,28 +4303,28 @@
         <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="V1" s="12" t="s">
         <v>18</v>
@@ -4336,191 +4333,191 @@
         <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>126</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O2">
         <v>10</v>
       </c>
       <c r="P2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q2" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="S2" t="s">
         <v>129</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>130</v>
-      </c>
-      <c r="T2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O3">
         <v>10</v>
       </c>
       <c r="P3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="S3" t="s">
+        <v>129</v>
+      </c>
+      <c r="U3" t="s">
         <v>133</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>128</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="S3" t="s">
-        <v>130</v>
-      </c>
-      <c r="U3" t="s">
-        <v>134</v>
       </c>
       <c r="X3" s="7"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O4">
         <v>10</v>
       </c>
       <c r="P4" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>127</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="S4" t="s">
+        <v>129</v>
+      </c>
+      <c r="T4" t="s">
+        <v>130</v>
+      </c>
+      <c r="U4" t="s">
         <v>136</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>128</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="S4" t="s">
-        <v>130</v>
-      </c>
-      <c r="T4" t="s">
-        <v>131</v>
-      </c>
-      <c r="U4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="H5" s="8"/>
       <c r="K5" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -4528,13 +4525,13 @@
         <v>17</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="X6" s="7"/>
     </row>
@@ -4543,10 +4540,10 @@
         <v>23</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4605,13 +4602,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -4659,7 +4656,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>22</v>
@@ -4686,7 +4683,7 @@
         <v>39</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:35">
@@ -4700,10 +4697,10 @@
         <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -4717,19 +4714,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>260</v>
+      </c>
+      <c r="O2" t="s">
+        <v>261</v>
+      </c>
+      <c r="P2" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q2" t="s">
         <v>262</v>
       </c>
-      <c r="O2" t="s">
-        <v>263</v>
-      </c>
-      <c r="P2" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>264</v>
-      </c>
-      <c r="R2" t="s">
-        <v>266</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -4751,7 +4748,7 @@
         <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="4"/>
@@ -4796,10 +4793,10 @@
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="U8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V8" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="W8">
         <v>123</v>
@@ -4816,19 +4813,19 @@
         <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P9" t="s">
         <v>52</v>
       </c>
       <c r="Q9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="S9">
         <v>9898989898</v>
@@ -4836,7 +4833,7 @@
     </row>
     <row r="10" spans="1:35">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
         <v>47</v>
@@ -4848,19 +4845,19 @@
         <v>46</v>
       </c>
       <c r="N10" t="s">
+        <v>260</v>
+      </c>
+      <c r="O10" t="s">
+        <v>261</v>
+      </c>
+      <c r="P10" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q10" t="s">
         <v>262</v>
       </c>
-      <c r="O10" t="s">
-        <v>263</v>
-      </c>
-      <c r="P10" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>264</v>
-      </c>
-      <c r="R10" t="s">
-        <v>266</v>
       </c>
       <c r="S10">
         <v>9898989898</v>
@@ -4868,16 +4865,16 @@
     </row>
     <row r="11" spans="1:35">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -4889,13 +4886,13 @@
     </row>
     <row r="12" spans="1:35">
       <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="Y12" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="Y12" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:35">
@@ -4903,25 +4900,25 @@
         <v>34</v>
       </c>
       <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" t="s">
         <v>79</v>
       </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
       <c r="N13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P13" t="s">
         <v>52</v>
       </c>
       <c r="Q13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="S13">
         <v>9898989898</v>
@@ -4929,21 +4926,21 @@
     </row>
     <row r="14" spans="1:35">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="7"/>
       <c r="K14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="9"/>
@@ -4956,40 +4953,40 @@
     </row>
     <row r="15" spans="1:35">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:35">
       <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="M16" t="s">
         <v>106</v>
-      </c>
-      <c r="M16" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:35">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:35">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AI18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:35">
@@ -5014,8 +5011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5047,13 +5044,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -5101,7 +5098,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>22</v>
@@ -5128,13 +5125,13 @@
         <v>39</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -5148,10 +5145,10 @@
         <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -5163,19 +5160,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>260</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>263</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>60</v>
+        <v>262</v>
+      </c>
+      <c r="R2" t="s">
+        <v>264</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -5206,7 +5203,7 @@
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>53</v>
+        <v>267</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
@@ -5227,15 +5224,15 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -5248,7 +5245,7 @@
         <v>2</v>
       </c>
       <c r="AI8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -5256,10 +5253,10 @@
         <v>26</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W9">
         <v>123</v>
@@ -5272,10 +5269,10 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="U10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W10">
         <v>123</v>
@@ -5286,10 +5283,10 @@
         <v>28</v>
       </c>
       <c r="U11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="V11" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="W11">
         <v>123</v>
@@ -5313,10 +5310,10 @@
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="U13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V13" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="V13" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="W13">
         <v>123</v>
@@ -5331,7 +5328,7 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
         <v>47</v>
@@ -5343,19 +5340,19 @@
         <v>46</v>
       </c>
       <c r="N15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" t="s">
         <v>57</v>
-      </c>
-      <c r="O15" t="s">
-        <v>58</v>
       </c>
       <c r="P15" t="s">
         <v>52</v>
       </c>
       <c r="Q15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R15" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="R15" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="S15">
         <v>9898989898</v>
@@ -5363,7 +5360,7 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F16" t="s">
         <v>47</v>
@@ -5375,19 +5372,19 @@
         <v>46</v>
       </c>
       <c r="N16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P16" t="s">
         <v>52</v>
       </c>
       <c r="Q16" t="s">
+        <v>147</v>
+      </c>
+      <c r="R16" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>149</v>
       </c>
       <c r="S16">
         <v>9898989898</v>
@@ -5395,16 +5392,16 @@
     </row>
     <row r="17" spans="1:37">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" t="s">
         <v>63</v>
       </c>
-      <c r="H17" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>64</v>
-      </c>
-      <c r="J17" t="s">
-        <v>65</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -5416,42 +5413,42 @@
     </row>
     <row r="18" spans="1:37">
       <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="X18" s="5" t="s">
+      <c r="Y18" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="Y18" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:37">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
         <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>46</v>
       </c>
       <c r="N19" t="s">
+        <v>73</v>
+      </c>
+      <c r="O19" t="s">
         <v>74</v>
-      </c>
-      <c r="O19" t="s">
-        <v>75</v>
       </c>
       <c r="P19" t="s">
         <v>52</v>
       </c>
       <c r="Q19" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="S19">
         <v>9898989898</v>
@@ -5462,25 +5459,25 @@
         <v>34</v>
       </c>
       <c r="F20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" t="s">
         <v>79</v>
       </c>
-      <c r="G20" t="s">
+      <c r="N20" t="s">
         <v>80</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>81</v>
-      </c>
-      <c r="O20" t="s">
-        <v>82</v>
       </c>
       <c r="P20" t="s">
         <v>52</v>
       </c>
       <c r="Q20" t="s">
+        <v>82</v>
+      </c>
+      <c r="R20" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="S20">
         <v>9898989898</v>
@@ -5488,21 +5485,21 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="7"/>
       <c r="K21" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
@@ -5514,48 +5511,48 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="X22" t="s">
         <v>95</v>
       </c>
-      <c r="X22" t="s">
-        <v>96</v>
-      </c>
       <c r="Y22" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AI22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:37">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
         <v>79</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>46</v>
       </c>
       <c r="N23" t="s">
+        <v>99</v>
+      </c>
+      <c r="O23" t="s">
         <v>100</v>
-      </c>
-      <c r="O23" t="s">
-        <v>101</v>
       </c>
       <c r="P23" t="s">
         <v>52</v>
       </c>
       <c r="Q23" t="s">
+        <v>101</v>
+      </c>
+      <c r="R23" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="R23" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="S23" s="9">
         <v>9898989898</v>
@@ -5563,122 +5560,122 @@
     </row>
     <row r="24" spans="1:37">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="9"/>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="M25" t="s">
         <v>106</v>
-      </c>
-      <c r="M25" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:37">
       <c r="A26" t="s">
+        <v>109</v>
+      </c>
+      <c r="U26" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="U26" s="5" t="s">
+      <c r="V26" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="V26" s="5" t="s">
+      <c r="W26" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:37">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
     </row>
     <row r="28" spans="1:37">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AC28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AI28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:37">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AJ29" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AK29" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="AK29" s="7" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:37">
       <c r="A30" t="s">
+        <v>161</v>
+      </c>
+      <c r="M30" t="s">
         <v>162</v>
-      </c>
-      <c r="M30" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:37">
       <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="X31" t="s">
         <v>164</v>
-      </c>
-      <c r="X31" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:37">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X32" s="5" t="s">
-        <v>174</v>
+        <v>315</v>
       </c>
       <c r="Y32" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:35">
       <c r="A33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" t="s">
         <v>79</v>
       </c>
-      <c r="G33" t="s">
+      <c r="K33" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N33" t="s">
         <v>80</v>
       </c>
-      <c r="K33" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>81</v>
-      </c>
-      <c r="O33" t="s">
-        <v>82</v>
       </c>
       <c r="P33" t="s">
         <v>52</v>
       </c>
       <c r="Q33" t="s">
+        <v>82</v>
+      </c>
+      <c r="R33" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="S33">
         <v>9898989898</v>
@@ -5687,38 +5684,38 @@
         <v>888888</v>
       </c>
       <c r="U33" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V33" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="W33" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AI33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:35">
       <c r="A34" t="s">
+        <v>219</v>
+      </c>
+      <c r="X34" t="s">
         <v>221</v>
       </c>
-      <c r="X34" t="s">
-        <v>223</v>
-      </c>
       <c r="Y34" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:35">
       <c r="A35" t="s">
+        <v>220</v>
+      </c>
+      <c r="X35" t="s">
         <v>222</v>
       </c>
-      <c r="X35" t="s">
-        <v>224</v>
-      </c>
       <c r="Y35" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
67 testcase for drybar UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="320">
   <si>
     <t>UserName</t>
   </si>
@@ -982,6 +982,18 @@
   </si>
   <si>
     <t>Detox Dry Shampoo Bundle Test</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo</t>
+  </si>
+  <si>
+    <t>Travel Size: 40g/1.4 oz.</t>
+  </si>
+  <si>
+    <t>scent</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1402,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -5011,8 +5023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5101,7 +5113,7 @@
         <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>22</v>
+        <v>318</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5216,7 +5228,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>44</v>
+        <v>269</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -5514,13 +5526,16 @@
         <v>94</v>
       </c>
       <c r="X22" t="s">
-        <v>95</v>
+        <v>316</v>
       </c>
       <c r="Y22" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z22" t="s">
-        <v>97</v>
+        <v>317</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>319</v>
       </c>
       <c r="AI22" t="s">
         <v>142</v>

</xml_diff>

<commit_message>
167 testcase for drybar uk
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="320">
   <si>
     <t>UserName</t>
   </si>
@@ -1404,7 +1404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1414,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -5021,10 +5021,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK35"/>
+  <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5511,9 +5511,26 @@
         <v>85</v>
       </c>
       <c r="M21" t="s">
-        <v>87</v>
-      </c>
-      <c r="S21" s="9"/>
+        <v>291</v>
+      </c>
+      <c r="N21" t="s">
+        <v>260</v>
+      </c>
+      <c r="O21" t="s">
+        <v>261</v>
+      </c>
+      <c r="P21" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>262</v>
+      </c>
+      <c r="R21" t="s">
+        <v>264</v>
+      </c>
+      <c r="S21" s="9">
+        <v>9898989898</v>
+      </c>
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
@@ -5523,213 +5540,238 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" t="s">
-        <v>94</v>
-      </c>
-      <c r="X22" t="s">
-        <v>316</v>
-      </c>
-      <c r="Y22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>317</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>319</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>142</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="7"/>
+      <c r="K22" s="2"/>
+      <c r="M22" t="s">
+        <v>291</v>
+      </c>
+      <c r="N22" t="s">
+        <v>289</v>
+      </c>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="2"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
     </row>
     <row r="23" spans="1:37">
       <c r="A23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" t="s">
-        <v>78</v>
-      </c>
-      <c r="G23" t="s">
-        <v>79</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N23" t="s">
-        <v>99</v>
-      </c>
-      <c r="O23" t="s">
-        <v>100</v>
-      </c>
-      <c r="P23" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>101</v>
-      </c>
-      <c r="R23" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="S23" s="9">
-        <v>9898989898</v>
+        <v>94</v>
+      </c>
+      <c r="X23" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>317</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:37">
       <c r="A24" t="s">
-        <v>104</v>
-      </c>
-      <c r="M24" t="s">
-        <v>103</v>
-      </c>
-      <c r="R24" s="10"/>
-      <c r="S24" s="9"/>
+        <v>98</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" t="s">
+        <v>79</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N24" t="s">
+        <v>99</v>
+      </c>
+      <c r="O24" t="s">
+        <v>100</v>
+      </c>
+      <c r="P24" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>101</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="S24" s="9">
+        <v>9898989898</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M25" t="s">
-        <v>106</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="R25" s="10"/>
+      <c r="S25" s="9"/>
     </row>
     <row r="26" spans="1:37">
       <c r="A26" t="s">
-        <v>109</v>
-      </c>
-      <c r="U26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="V26" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+      <c r="M26" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:37">
       <c r="A27" t="s">
-        <v>113</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ27" s="7"/>
-      <c r="AK27" s="7"/>
+        <v>109</v>
+      </c>
+      <c r="U27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="V27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="W27" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="28" spans="1:37">
       <c r="A28" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI28" t="s">
-        <v>142</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ28" s="7"/>
+      <c r="AK28" s="7"/>
     </row>
     <row r="29" spans="1:37">
       <c r="A29" t="s">
-        <v>158</v>
-      </c>
-      <c r="AJ29" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="AK29" s="7" t="s">
-        <v>157</v>
+        <v>145</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:37">
       <c r="A30" t="s">
-        <v>161</v>
-      </c>
-      <c r="M30" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="AJ30" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AK30" s="7" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:37">
       <c r="A31" t="s">
-        <v>163</v>
-      </c>
-      <c r="X31" t="s">
-        <v>164</v>
+        <v>161</v>
+      </c>
+      <c r="M31" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:37">
       <c r="A32" t="s">
-        <v>172</v>
-      </c>
-      <c r="X32" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="Y32" s="5" t="s">
-        <v>67</v>
+        <v>163</v>
+      </c>
+      <c r="X32" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:35">
       <c r="A33" t="s">
-        <v>183</v>
-      </c>
-      <c r="F33" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" t="s">
-        <v>79</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="N33" t="s">
-        <v>80</v>
-      </c>
-      <c r="O33" t="s">
-        <v>81</v>
-      </c>
-      <c r="P33" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>82</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S33">
-        <v>9898989898</v>
-      </c>
-      <c r="T33">
-        <v>888888</v>
-      </c>
-      <c r="U33" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V33" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W33" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI33" t="s">
-        <v>142</v>
+        <v>172</v>
+      </c>
+      <c r="X33" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y33" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:35">
       <c r="A34" t="s">
-        <v>219</v>
-      </c>
-      <c r="X34" t="s">
-        <v>221</v>
-      </c>
-      <c r="Y34" s="5" t="s">
-        <v>67</v>
+        <v>183</v>
+      </c>
+      <c r="F34" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" t="s">
+        <v>79</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N34" t="s">
+        <v>80</v>
+      </c>
+      <c r="O34" t="s">
+        <v>81</v>
+      </c>
+      <c r="P34" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S34">
+        <v>9898989898</v>
+      </c>
+      <c r="T34">
+        <v>888888</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V34" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="W34" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:35">
       <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="X35" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y35" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35">
+      <c r="A36" t="s">
         <v>220</v>
       </c>
-      <c r="X35" t="s">
+      <c r="X36" t="s">
         <v>222</v>
       </c>
-      <c r="Y35" s="5" t="s">
+      <c r="Y36" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -5742,9 +5784,9 @@
     <hyperlink ref="B2" r:id="rId5"/>
     <hyperlink ref="K19" r:id="rId6"/>
     <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K23" r:id="rId8"/>
+    <hyperlink ref="K24" r:id="rId8"/>
     <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K33" r:id="rId10"/>
+    <hyperlink ref="K34" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Drybar UK Commited 75 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DAA280-1928-4931-A65D-D446A7179847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -21,8 +22,8 @@
     <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -999,11 +1000,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1404,21 +1405,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="N34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1446,7 +1447,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1675,7 +1676,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1689,7 +1690,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1818,7 +1819,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1846,7 +1847,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2129,7 +2130,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2193,7 +2194,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2234,7 +2235,7 @@
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -2262,7 +2263,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -2274,7 +2275,7 @@
       </c>
       <c r="AL34" s="7"/>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2368,7 +2369,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2469,7 +2470,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:40">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:40">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:40">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:40">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:40">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2674,8 +2675,8 @@
       <c r="I53" t="s">
         <v>63</v>
       </c>
-      <c r="X53" s="5" t="s">
-        <v>268</v>
+      <c r="X53" t="s">
+        <v>287</v>
       </c>
       <c r="Y53" s="5" t="s">
         <v>67</v>
@@ -2690,40 +2691,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
-    <hyperlink ref="K19" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K22" r:id="rId7"/>
-    <hyperlink ref="K24" r:id="rId8"/>
-    <hyperlink ref="K26" r:id="rId9"/>
-    <hyperlink ref="B37" r:id="rId10"/>
-    <hyperlink ref="D37" r:id="rId11"/>
-    <hyperlink ref="E37" r:id="rId12"/>
-    <hyperlink ref="K37" r:id="rId13"/>
-    <hyperlink ref="K42" r:id="rId14"/>
-    <hyperlink ref="B43" r:id="rId15"/>
-    <hyperlink ref="D43" r:id="rId16"/>
-    <hyperlink ref="E43" r:id="rId17"/>
-    <hyperlink ref="C43" r:id="rId18"/>
-    <hyperlink ref="F9" r:id="rId19"/>
-    <hyperlink ref="D9" r:id="rId20"/>
-    <hyperlink ref="E9" r:id="rId21"/>
-    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K49" r:id="rId32"/>
-    <hyperlink ref="K50" r:id="rId33"/>
-    <hyperlink ref="B51" r:id="rId34"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B43" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D43" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C43" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2731,16 +2732,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2880,11 +2881,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2892,14 +2893,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
@@ -2914,7 +2915,7 @@
     <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3048,7 +3049,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3069,7 +3070,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3082,26 +3083,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="AC4" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -3117,7 +3118,7 @@
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -3304,7 +3305,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="187.2">
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -3333,29 +3334,29 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -3364,7 +3365,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3453,7 +3454,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3494,7 +3495,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3517,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3525,7 +3526,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3536,7 +3537,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3549,33 +3550,33 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="Y4" r:id="rId6"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -3587,7 +3588,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3622,7 +3623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3642,7 +3643,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3654,7 +3655,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3670,7 +3671,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3699,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3710,7 +3711,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3724,7 +3725,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3734,31 +3735,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3889,7 +3890,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3935,7 +3936,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3956,7 +3957,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -3970,7 +3971,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -3984,7 +3985,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -3997,7 +3998,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4012,7 +4013,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4027,7 +4028,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4042,7 +4043,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4052,30 +4053,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -4084,7 +4085,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4188,7 +4189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4204,27 +4205,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4232,7 +4233,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4246,14 +4247,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -4274,7 +4275,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4348,7 +4349,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4399,7 +4400,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4451,7 +4452,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4505,7 +4506,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4547,7 +4548,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4560,38 +4561,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="B5" r:id="rId12"/>
-    <hyperlink ref="C5" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4698,7 +4699,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4746,7 +4747,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4755,7 +4756,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4766,7 +4767,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4787,14 +4788,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4814,7 +4815,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4843,7 +4844,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4875,7 +4876,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4896,7 +4897,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4907,7 +4908,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4963,7 +4964,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -4993,7 +4994,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5001,39 +5002,39 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K2" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5146,7 +5147,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5192,7 +5193,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5201,7 +5202,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5210,7 +5211,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5221,7 +5222,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5234,7 +5235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5247,7 +5248,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5260,7 +5261,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5274,7 +5275,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5290,7 +5291,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5304,14 +5305,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5331,14 +5332,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -5370,7 +5371,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -5423,7 +5424,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -5434,7 +5435,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -5466,7 +5467,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5495,7 +5496,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -5538,7 +5539,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>290</v>
       </c>
@@ -5563,7 +5564,7 @@
       <c r="AD22" s="5"/>
       <c r="AE22" s="5"/>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -5583,7 +5584,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -5625,7 +5626,7 @@
       <c r="R25" s="10"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -5633,7 +5634,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -5647,7 +5648,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -5657,7 +5658,7 @@
       <c r="AJ28" s="7"/>
       <c r="AK28" s="7"/>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>145</v>
       </c>
@@ -5668,7 +5669,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>158</v>
       </c>
@@ -5679,7 +5680,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>161</v>
       </c>
@@ -5687,7 +5688,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -5695,7 +5696,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -5706,7 +5707,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -5753,7 +5754,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>219</v>
       </c>
@@ -5764,7 +5765,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>220</v>
       </c>
@@ -5777,16 +5778,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K19" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K24" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K34" r:id="rId10"/>
+    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="K34" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testcdata changes for UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DAA280-1928-4931-A65D-D446A7179847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,8 +21,8 @@
     <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="321">
   <si>
     <t>UserName</t>
   </si>
@@ -996,15 +995,18 @@
   <si>
     <t>Original</t>
   </si>
+  <si>
+    <t>Big Swig Thickening Spray</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1405,21 +1407,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="N34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1447,7 +1449,7 @@
     <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1569,7 +1571,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1618,7 +1620,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1632,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1690,7 +1692,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1707,7 +1709,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1752,7 +1754,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1766,7 +1768,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1783,7 +1785,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1802,7 +1804,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1819,7 +1821,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1836,7 +1838,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1847,7 +1849,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1915,7 +1917,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1950,7 +1952,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1975,7 +1977,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1999,7 +2001,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2034,7 +2036,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2066,7 +2068,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2168,7 +2170,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2194,7 +2196,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2205,7 +2207,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2235,7 +2237,7 @@
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2249,7 +2251,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -2263,7 +2265,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -2275,7 +2277,7 @@
       </c>
       <c r="AL34" s="7"/>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2286,7 +2288,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2327,7 +2329,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2345,7 +2347,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2369,7 +2371,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2386,7 +2388,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2403,7 +2405,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2470,7 +2472,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2502,7 +2504,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2536,7 +2538,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2566,7 +2568,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2580,7 +2582,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:40">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2626,7 +2628,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:40">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2640,7 +2642,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:40">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:40">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2665,7 +2667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:40">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2691,40 +2693,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B43" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D43" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C43" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K19" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K22" r:id="rId7"/>
+    <hyperlink ref="K24" r:id="rId8"/>
+    <hyperlink ref="K26" r:id="rId9"/>
+    <hyperlink ref="B37" r:id="rId10"/>
+    <hyperlink ref="D37" r:id="rId11"/>
+    <hyperlink ref="E37" r:id="rId12"/>
+    <hyperlink ref="K37" r:id="rId13"/>
+    <hyperlink ref="K42" r:id="rId14"/>
+    <hyperlink ref="B43" r:id="rId15"/>
+    <hyperlink ref="D43" r:id="rId16"/>
+    <hyperlink ref="E43" r:id="rId17"/>
+    <hyperlink ref="C43" r:id="rId18"/>
+    <hyperlink ref="F9" r:id="rId19"/>
+    <hyperlink ref="D9" r:id="rId20"/>
+    <hyperlink ref="E9" r:id="rId21"/>
+    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K49" r:id="rId32"/>
+    <hyperlink ref="K50" r:id="rId33"/>
+    <hyperlink ref="B51" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2732,16 +2734,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:X3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2814,8 +2820,11 @@
       <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2856,7 +2865,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2864,28 +2873,31 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="Q3" t="s">
         <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
+      <c r="Y3" t="s">
+        <v>259</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2893,14 +2905,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
@@ -2915,7 +2927,7 @@
     <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3004,7 +3016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3049,7 +3061,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3070,7 +3082,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3083,26 +3095,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="AC4" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -3118,7 +3130,7 @@
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3186,7 +3198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3227,7 +3239,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3253,7 +3265,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3279,7 +3291,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -3305,7 +3317,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="187.2">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -3334,29 +3346,29 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
-    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -3365,7 +3377,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3454,7 +3466,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3495,7 +3507,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3518,7 +3530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3526,7 +3538,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3537,7 +3549,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3550,33 +3562,33 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -3588,7 +3600,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3623,7 +3635,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3643,7 +3655,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3655,7 +3667,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3671,7 +3683,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3689,7 +3701,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3700,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3711,7 +3723,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3725,7 +3737,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3735,31 +3747,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3890,7 +3902,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3936,7 +3948,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3957,7 +3969,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -3971,7 +3983,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -3985,7 +3997,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -3998,7 +4010,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4013,7 +4025,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4028,7 +4040,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4043,7 +4055,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4053,30 +4065,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -4085,7 +4097,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4189,7 +4201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4205,27 +4217,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4233,7 +4245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4247,14 +4259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -4275,7 +4287,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4349,7 +4361,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4400,7 +4412,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4452,7 +4464,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4506,7 +4518,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4533,7 +4545,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4548,7 +4560,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4561,38 +4573,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4699,7 +4711,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4747,7 +4759,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4756,7 +4768,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4767,7 +4779,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4780,7 +4792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4788,14 +4800,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4815,7 +4827,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4844,7 +4856,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4876,7 +4888,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4897,7 +4909,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4908,7 +4920,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4937,7 +4949,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4964,7 +4976,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4978,7 +4990,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4986,7 +4998,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -4994,7 +5006,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5002,39 +5014,39 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5147,7 +5159,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5193,7 +5205,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5202,7 +5214,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5211,7 +5223,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5222,7 +5234,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5235,7 +5247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5248,7 +5260,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5261,7 +5273,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5275,7 +5287,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5291,7 +5303,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5305,14 +5317,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5332,14 +5344,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -5371,7 +5383,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -5403,7 +5415,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -5424,7 +5436,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -5435,7 +5447,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -5467,7 +5479,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5496,7 +5508,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -5539,7 +5551,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>290</v>
       </c>
@@ -5564,7 +5576,7 @@
       <c r="AD22" s="5"/>
       <c r="AE22" s="5"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -5584,7 +5596,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -5616,7 +5628,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -5626,7 +5638,7 @@
       <c r="R25" s="10"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -5634,7 +5646,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -5648,7 +5660,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -5658,7 +5670,7 @@
       <c r="AJ28" s="7"/>
       <c r="AK28" s="7"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
         <v>145</v>
       </c>
@@ -5669,7 +5681,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
         <v>158</v>
       </c>
@@ -5680,7 +5692,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
         <v>161</v>
       </c>
@@ -5688,7 +5700,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -5696,7 +5708,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -5707,7 +5719,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -5754,7 +5766,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
         <v>219</v>
       </c>
@@ -5765,7 +5777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35">
       <c r="A36" t="s">
         <v>220</v>
       </c>
@@ -5778,16 +5790,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="K34" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K19" r:id="rId6"/>
+    <hyperlink ref="K21" r:id="rId7"/>
+    <hyperlink ref="K24" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K34" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
004 Testcase Drybar UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AFD5F0-E3FC-4526-B363-C3B9CA3A0C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -21,8 +22,8 @@
     <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="322">
   <si>
     <t>UserName</t>
   </si>
@@ -998,15 +999,18 @@
   <si>
     <t>Big Swig Thickening Spray</t>
   </si>
+  <si>
+    <t>Full Size: 100g/3.5 Oz.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1078,6 +1082,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1106,7 +1117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1134,6 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1407,49 +1419,49 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView topLeftCell="N34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X53" sqref="X53"/>
+    <sheetView tabSelected="1" topLeftCell="P2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="16" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1571,7 +1583,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1620,7 +1632,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1632,7 +1644,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1659,7 +1671,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1678,7 +1690,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1692,7 +1704,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1709,7 +1721,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1754,7 +1766,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1768,7 +1780,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1785,7 +1797,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1804,7 +1816,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1821,7 +1833,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1859,7 +1871,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1882,7 +1894,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1952,7 +1964,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1977,7 +1989,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2001,7 +2013,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2036,7 +2048,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2114,25 +2126,25 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
       <c r="X25" t="s">
-        <v>95</v>
+        <v>316</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z25" s="5"/>
-      <c r="AA25" t="s">
-        <v>97</v>
+      <c r="AA25" s="25" t="s">
+        <v>321</v>
       </c>
       <c r="AJ25" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2170,7 +2182,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2183,7 +2195,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2196,7 +2208,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2207,7 +2219,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2224,7 +2236,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2237,7 +2249,7 @@
       <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2251,7 +2263,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -2265,7 +2277,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -2277,7 +2289,7 @@
       </c>
       <c r="AL34" s="7"/>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2288,7 +2300,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2303,7 +2315,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2329,7 +2341,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2347,7 +2359,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2371,7 +2383,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2388,7 +2400,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2405,7 +2417,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2452,7 +2464,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2504,7 +2516,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2538,7 +2550,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2568,7 +2580,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2582,7 +2594,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2593,7 +2605,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:40">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2628,7 +2640,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:40">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2642,7 +2654,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:40">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:40">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2667,7 +2679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:40">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2693,40 +2705,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
-    <hyperlink ref="K19" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="K22" r:id="rId7"/>
-    <hyperlink ref="K24" r:id="rId8"/>
-    <hyperlink ref="K26" r:id="rId9"/>
-    <hyperlink ref="B37" r:id="rId10"/>
-    <hyperlink ref="D37" r:id="rId11"/>
-    <hyperlink ref="E37" r:id="rId12"/>
-    <hyperlink ref="K37" r:id="rId13"/>
-    <hyperlink ref="K42" r:id="rId14"/>
-    <hyperlink ref="B43" r:id="rId15"/>
-    <hyperlink ref="D43" r:id="rId16"/>
-    <hyperlink ref="E43" r:id="rId17"/>
-    <hyperlink ref="C43" r:id="rId18"/>
-    <hyperlink ref="F9" r:id="rId19"/>
-    <hyperlink ref="D9" r:id="rId20"/>
-    <hyperlink ref="E9" r:id="rId21"/>
-    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123"/>
-    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123"/>
-    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
-    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123"/>
-    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234"/>
-    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
-    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
-    <hyperlink ref="K49" r:id="rId32"/>
-    <hyperlink ref="K50" r:id="rId33"/>
-    <hyperlink ref="B51" r:id="rId34"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B43" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D43" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C43" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2734,20 +2746,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2824,7 +2836,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2865,7 +2877,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2893,11 +2905,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2905,29 +2917,29 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3016,7 +3028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3061,7 +3073,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3082,7 +3094,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3095,42 +3107,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="AC4" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3198,7 +3210,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3239,7 +3251,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3265,7 +3277,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3291,7 +3303,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -3317,7 +3329,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="187.2">
+    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -3346,38 +3358,38 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="25" max="25" width="36.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" customWidth="1"/>
-    <col min="28" max="28" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="36.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3466,7 +3478,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3507,7 +3519,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3530,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3538,7 +3550,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3549,7 +3561,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3562,45 +3574,45 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
-    <hyperlink ref="Y4" r:id="rId6"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3635,7 +3647,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3655,7 +3667,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3667,7 +3679,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3683,7 +3695,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3701,7 +3713,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3712,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3723,7 +3735,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3737,7 +3749,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3747,31 +3759,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3902,7 +3914,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3948,7 +3960,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3969,7 +3981,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -3983,7 +3995,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -3997,7 +4009,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4010,7 +4022,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4025,7 +4037,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4040,7 +4052,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4055,7 +4067,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4065,39 +4077,39 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4201,7 +4213,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4217,27 +4229,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4245,7 +4257,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4259,35 +4271,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4361,7 +4373,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4412,7 +4424,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4464,7 +4476,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4518,7 +4530,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4545,7 +4557,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4560,7 +4572,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4573,38 +4585,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="B5" r:id="rId12"/>
-    <hyperlink ref="C5" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4711,7 +4723,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4759,7 +4771,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4768,7 +4780,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4779,7 +4791,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4792,7 +4804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4800,14 +4812,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4827,7 +4839,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4856,7 +4868,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4888,7 +4900,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4909,7 +4921,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4920,7 +4932,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4949,7 +4961,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4976,7 +4988,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4990,7 +5002,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4998,7 +5010,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -5006,7 +5018,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5014,39 +5026,39 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K2" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5159,7 +5171,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5205,7 +5217,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5214,7 +5226,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5223,7 +5235,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5234,7 +5246,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5247,7 +5259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5260,7 +5272,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5273,7 +5285,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5287,7 +5299,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5303,7 +5315,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5317,14 +5329,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5344,14 +5356,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -5383,7 +5395,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -5415,7 +5427,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -5436,7 +5448,7 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -5447,7 +5459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -5479,7 +5491,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5508,7 +5520,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -5551,7 +5563,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>290</v>
       </c>
@@ -5576,7 +5588,7 @@
       <c r="AD22" s="5"/>
       <c r="AE22" s="5"/>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -5596,7 +5608,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -5628,7 +5640,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -5638,7 +5650,7 @@
       <c r="R25" s="10"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -5646,7 +5658,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -5660,7 +5672,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -5670,7 +5682,7 @@
       <c r="AJ28" s="7"/>
       <c r="AK28" s="7"/>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>145</v>
       </c>
@@ -5681,7 +5693,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>158</v>
       </c>
@@ -5692,7 +5704,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>161</v>
       </c>
@@ -5700,7 +5712,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -5708,7 +5720,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -5719,7 +5731,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -5766,7 +5778,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>219</v>
       </c>
@@ -5777,7 +5789,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>220</v>
       </c>
@@ -5790,16 +5802,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="K19" r:id="rId6"/>
-    <hyperlink ref="K21" r:id="rId7"/>
-    <hyperlink ref="K24" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K34" r:id="rId10"/>
+    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="K34" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
004 Testcase testdata and method change
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AFD5F0-E3FC-4526-B363-C3B9CA3A0C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9FA400-4B39-4F57-8BCF-F7984A75C336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="323">
   <si>
     <t>UserName</t>
   </si>
@@ -1000,7 +1000,10 @@
     <t>Big Swig Thickening Spray</t>
   </si>
   <si>
-    <t>Full Size: 100g/3.5 Oz.</t>
+    <t>Lush</t>
+  </si>
+  <si>
+    <t>Full Size: 100g/3.5 oz.</t>
   </si>
 </sst>
 </file>
@@ -1083,11 +1086,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color rgb="FF17C6A3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1427,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN53"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA25" sqref="AA25"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,11 +1459,11 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.28515625" customWidth="1"/>
+    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1538,52 +1540,55 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1628,11 +1633,11 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1640,11 +1645,11 @@
       <c r="E3" s="2"/>
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1652,11 +1657,11 @@
       <c r="E4" s="2"/>
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1667,11 +1672,12 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-      <c r="AJ5" t="s">
+      <c r="AA5" s="5"/>
+      <c r="AK5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1683,14 +1689,15 @@
       <c r="Y6" s="5">
         <v>2</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5">
         <v>4</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1703,8 +1710,9 @@
         <v>2</v>
       </c>
       <c r="Z7" s="5"/>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AA7" s="5"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1717,11 +1725,12 @@
         <v>160</v>
       </c>
       <c r="Z8" s="5"/>
-      <c r="AJ8" t="s">
+      <c r="AA8" s="5"/>
+      <c r="AK8" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1759,14 +1768,14 @@
       <c r="S9" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="AG9" s="8" t="s">
+      <c r="AH9" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1776,11 +1785,12 @@
         <v>2</v>
       </c>
       <c r="Z10" s="5"/>
-      <c r="AJ10" t="s">
+      <c r="AA10" s="5"/>
+      <c r="AK10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1793,11 +1803,11 @@
       <c r="W11">
         <v>123</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AK11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1812,11 +1822,11 @@
       <c r="W12">
         <v>123</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AK12" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1829,11 +1839,11 @@
       <c r="W13">
         <v>123</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AK13" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1846,32 +1856,32 @@
       <c r="W14">
         <v>123</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AK14" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
-      <c r="AJ15" t="s">
+      <c r="AK15" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="AJ16" t="s">
+      <c r="AK16" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1890,11 +1900,11 @@
       <c r="W17">
         <v>123</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AK17" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1925,11 +1935,11 @@
       <c r="S18">
         <v>9898989898</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AK18" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1960,11 +1970,11 @@
       <c r="S19">
         <v>9898989898</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AK19" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1985,11 +1995,12 @@
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
-      <c r="AJ20" t="s">
+      <c r="AA20" s="9"/>
+      <c r="AK20" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2006,14 +2017,15 @@
         <v>67</v>
       </c>
       <c r="Z21" s="5"/>
-      <c r="AJ21" t="s">
+      <c r="AA21" s="5"/>
+      <c r="AK21" t="s">
         <v>259</v>
       </c>
-      <c r="AN21" t="s">
+      <c r="AO21" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2044,11 +2056,11 @@
       <c r="S22">
         <v>9898989898</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AK22" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2076,11 +2088,11 @@
       <c r="S23">
         <v>9898989898</v>
       </c>
-      <c r="AJ23" t="s">
+      <c r="AK23" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2120,13 +2132,13 @@
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
       <c r="W24" s="2"/>
-      <c r="AE24" s="5"/>
       <c r="AF24" s="5"/>
-      <c r="AJ24" t="s">
+      <c r="AG24" s="5"/>
+      <c r="AK24" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2136,15 +2148,18 @@
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="25" t="s">
+      <c r="Z25" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="AJ25" t="s">
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="AK25" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2178,11 +2193,11 @@
       <c r="S26" s="9">
         <v>9898989898</v>
       </c>
-      <c r="AJ26" t="s">
+      <c r="AK26" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2191,11 +2206,11 @@
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
-      <c r="AJ27" t="s">
+      <c r="AK27" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2208,18 +2223,18 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
       <c r="M29" t="s">
         <v>291</v>
       </c>
-      <c r="AJ29" t="s">
+      <c r="AK29" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2232,75 +2247,75 @@
       <c r="W30" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AJ30" t="s">
+      <c r="AK30" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AJ31" t="s">
+      <c r="AK31" t="s">
         <v>259</v>
       </c>
-      <c r="AK31" s="7"/>
       <c r="AL31" s="7"/>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AM31" s="7"/>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AE32" t="s">
         <v>282</v>
       </c>
-      <c r="AE32" t="s">
+      <c r="AF32" t="s">
         <v>144</v>
       </c>
-      <c r="AJ32" t="s">
+      <c r="AK32" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>304</v>
       </c>
-      <c r="AJ33" t="s">
+      <c r="AK33" t="s">
         <v>259</v>
       </c>
-      <c r="AK33" s="7" t="s">
+      <c r="AL33" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="AL33" s="7" t="s">
+      <c r="AM33" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>312</v>
       </c>
-      <c r="AJ34" t="s">
+      <c r="AK34" t="s">
         <v>259</v>
       </c>
-      <c r="AK34" s="7" t="s">
+      <c r="AL34" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="AL34" s="7"/>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM34" s="7"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>161</v>
       </c>
       <c r="M35" t="s">
         <v>162</v>
       </c>
-      <c r="AJ35" t="s">
+      <c r="AK35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2311,11 +2326,12 @@
         <v>67</v>
       </c>
       <c r="Z36" s="5"/>
-      <c r="AJ36" t="s">
+      <c r="AA36" s="5"/>
+      <c r="AK36" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2337,11 +2353,11 @@
       <c r="K37" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="AJ37" t="s">
+      <c r="AK37" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2352,14 +2368,15 @@
         <v>67</v>
       </c>
       <c r="Z38" s="5"/>
-      <c r="AA38" s="5" t="s">
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="AJ38" t="s">
+      <c r="AK38" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2376,31 +2393,32 @@
         <v>67</v>
       </c>
       <c r="Z39" s="5"/>
-      <c r="AA39" s="5" t="s">
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="AJ39" t="s">
+      <c r="AK39" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>179</v>
       </c>
       <c r="F40" t="s">
         <v>78</v>
       </c>
-      <c r="AJ40" t="s">
+      <c r="AK40" t="s">
         <v>259</v>
       </c>
-      <c r="AK40" t="s">
+      <c r="AL40" t="s">
         <v>310</v>
       </c>
-      <c r="AL40" s="7" t="s">
+      <c r="AM40" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2413,11 +2431,11 @@
       <c r="D41" t="s">
         <v>182</v>
       </c>
-      <c r="AJ41" t="s">
+      <c r="AK41" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2460,11 +2478,11 @@
       <c r="W42" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="AJ42" t="s">
+      <c r="AK42" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2480,11 +2498,11 @@
       <c r="E43" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="AJ43" t="s">
+      <c r="AK43" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2512,11 +2530,11 @@
       <c r="S44">
         <v>9898989898</v>
       </c>
-      <c r="AJ44" t="s">
+      <c r="AK44" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2546,11 +2564,11 @@
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
-      <c r="AJ45" t="s">
+      <c r="AK45" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2576,11 +2594,11 @@
         <v>218</v>
       </c>
       <c r="M46" s="9"/>
-      <c r="AJ46" t="s">
+      <c r="AK46" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2590,22 +2608,22 @@
       <c r="Y47">
         <v>2</v>
       </c>
-      <c r="AJ47" t="s">
+      <c r="AK47" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="AJ48" t="s">
+      <c r="AK48" t="s">
         <v>259</v>
       </c>
-      <c r="AM48" t="s">
+      <c r="AN48" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2636,25 +2654,25 @@
       <c r="S49">
         <v>9898989898</v>
       </c>
-      <c r="AJ49" t="s">
+      <c r="AK49" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
       <c r="K50" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="AI50" t="s">
+      <c r="AJ50" t="s">
         <v>281</v>
       </c>
-      <c r="AJ50" t="s">
+      <c r="AK50" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2668,7 +2686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2679,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2696,10 +2714,11 @@
         <v>67</v>
       </c>
       <c r="Z53" s="5"/>
-      <c r="AJ53" t="s">
+      <c r="AA53" s="5"/>
+      <c r="AK53" t="s">
         <v>259</v>
       </c>
-      <c r="AN53" t="s">
+      <c r="AO53" t="s">
         <v>288</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drybar Uk - 175 & Drybar US - 180 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9FA400-4B39-4F57-8BCF-F7984A75C336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EC5636-942F-42C3-BE6C-0267D50A6C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="323">
   <si>
     <t>UserName</t>
   </si>
@@ -1431,39 +1431,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC18" sqref="AC18"/>
+    <sheetView topLeftCell="AJ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL33" sqref="AL33:AL34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="16" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.28515625" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.33203125" customWidth="1"/>
+    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1712,7 +1712,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2223,7 +2223,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="AM34" s="7"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2772,13 +2772,13 @@
       <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2943,22 +2943,22 @@
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3092,7 +3092,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3145,23 +3145,23 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
@@ -3399,16 +3399,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" customWidth="1"/>
-    <col min="28" max="28" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3619,19 +3619,19 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3698,7 +3698,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3796,13 +3796,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3979,7 +3979,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -4000,7 +4000,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -4028,7 +4028,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4056,7 +4056,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4071,7 +4071,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4086,7 +4086,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4096,7 +4096,7 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
@@ -4119,16 +4119,16 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4262,13 +4262,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4297,28 +4297,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4630,12 +4630,12 @@
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4790,7 +4790,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4799,7 +4799,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4810,7 +4810,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4831,14 +4831,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4940,7 +4940,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -5007,7 +5007,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
@@ -5065,19 +5065,24 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AK36"/>
+  <dimension ref="A1:AK38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5190,18 +5195,18 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>46</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>60</v>
@@ -5236,7 +5241,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5245,7 +5250,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5254,7 +5259,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5265,7 +5270,7 @@
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5278,7 +5283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5291,7 +5296,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5304,533 +5309,555 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="W9">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="Y9" s="5"/>
+      <c r="AJ9" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>312</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="U10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="V10" s="6" t="s">
+      <c r="Y10" s="5"/>
+      <c r="AJ10" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V11" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="W10">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="W11">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="U12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+        <v>28</v>
+      </c>
       <c r="U13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V13" s="5" t="s">
-        <v>54</v>
+        <v>70</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="W13">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="U15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="W15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" t="s">
         <v>47</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>48</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K17" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N17" t="s">
         <v>56</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O17" t="s">
         <v>57</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P17" t="s">
         <v>52</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q17" t="s">
         <v>58</v>
       </c>
-      <c r="R15" s="5" t="s">
+      <c r="R17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="S15">
+      <c r="S17">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>146</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>47</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N18" t="s">
         <v>150</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O18" t="s">
         <v>149</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P18" t="s">
         <v>52</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q18" t="s">
         <v>147</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="R18" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="S16">
+      <c r="S18">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>62</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I19" t="s">
         <v>63</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J19" t="s">
         <v>64</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
-      <c r="X18" s="5" t="s">
+      <c r="X20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Y18" s="5" t="s">
+      <c r="Y20" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>72</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>48</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N21" t="s">
         <v>73</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O21" t="s">
         <v>74</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P21" t="s">
         <v>52</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q21" t="s">
         <v>75</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="R21" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="S19">
+      <c r="S21">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F22" t="s">
         <v>78</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G22" t="s">
         <v>79</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N22" t="s">
         <v>80</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O22" t="s">
         <v>81</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P22" t="s">
         <v>52</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q22" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="5" t="s">
+      <c r="R22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="S20">
+      <c r="S22">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="7" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="7"/>
-      <c r="K21" s="2" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="K23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M23" t="s">
         <v>291</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N23" t="s">
         <v>260</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O23" t="s">
         <v>261</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P23" t="s">
         <v>263</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q23" t="s">
         <v>262</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R23" t="s">
         <v>264</v>
       </c>
-      <c r="S21" s="9">
+      <c r="S23" s="9">
         <v>9898989898</v>
       </c>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="2"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="2"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>290</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="7"/>
-      <c r="K22" s="2"/>
-      <c r="M22" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="7"/>
+      <c r="K24" s="2"/>
+      <c r="M24" t="s">
         <v>291</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N24" t="s">
         <v>289</v>
       </c>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="2"/>
-      <c r="AD22" s="5"/>
-      <c r="AE22" s="5"/>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="2"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>94</v>
       </c>
-      <c r="X23" t="s">
+      <c r="X25" t="s">
         <v>316</v>
       </c>
-      <c r="Y23" s="5" t="s">
+      <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="Z25" t="s">
         <v>317</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AA25" t="s">
         <v>319</v>
       </c>
-      <c r="AI23" t="s">
+      <c r="AI25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>98</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F26" t="s">
         <v>78</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>79</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K26" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N26" t="s">
         <v>99</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O26" t="s">
         <v>100</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P26" t="s">
         <v>52</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q26" t="s">
         <v>101</v>
       </c>
-      <c r="R24" s="11" t="s">
+      <c r="R26" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="S24" s="9">
+      <c r="S26" s="9">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>104</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M27" t="s">
         <v>103</v>
       </c>
-      <c r="R25" s="10"/>
-      <c r="S25" s="9"/>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="R27" s="10"/>
+      <c r="S27" s="9"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>105</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M28" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>109</v>
       </c>
-      <c r="U27" s="5" t="s">
+      <c r="U29" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="V27" s="5" t="s">
+      <c r="V29" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="W27" s="5" t="s">
+      <c r="W29" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>113</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AJ28" s="7"/>
-      <c r="AK28" s="7"/>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="AJ30" s="7"/>
+      <c r="AK30" s="7"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>145</v>
       </c>
-      <c r="AC29" t="s">
+      <c r="AC31" t="s">
         <v>144</v>
       </c>
-      <c r="AI29" t="s">
+      <c r="AI31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>158</v>
       </c>
-      <c r="AJ30" s="7" t="s">
+      <c r="AJ32" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AK30" s="7" t="s">
+      <c r="AK32" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>161</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M33" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>163</v>
       </c>
-      <c r="X32" t="s">
+      <c r="X34" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>172</v>
       </c>
-      <c r="X33" s="5" t="s">
+      <c r="X35" s="5" t="s">
         <v>315</v>
-      </c>
-      <c r="Y33" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>183</v>
-      </c>
-      <c r="F34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G34" t="s">
-        <v>79</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="N34" t="s">
-        <v>80</v>
-      </c>
-      <c r="O34" t="s">
-        <v>81</v>
-      </c>
-      <c r="P34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>82</v>
-      </c>
-      <c r="R34" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S34">
-        <v>9898989898</v>
-      </c>
-      <c r="T34">
-        <v>888888</v>
-      </c>
-      <c r="U34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V34" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W34" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>219</v>
-      </c>
-      <c r="X35" t="s">
-        <v>221</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" t="s">
+        <v>79</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N36" t="s">
+        <v>80</v>
+      </c>
+      <c r="O36" t="s">
+        <v>81</v>
+      </c>
+      <c r="P36" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>82</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S36">
+        <v>9898989898</v>
+      </c>
+      <c r="T36">
+        <v>888888</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>219</v>
+      </c>
+      <c r="X37" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>220</v>
       </c>
-      <c r="X36" t="s">
+      <c r="X38" t="s">
         <v>222</v>
       </c>
-      <c r="Y36" s="5" t="s">
+      <c r="Y38" s="5" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K15" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
     <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
     <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
     <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="K34" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="K21" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="K23" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="K26" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="K18" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="K36" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
65 Tetscase for drybar UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EC5636-942F-42C3-BE6C-0267D50A6C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,8 +21,8 @@
     <sheet name="Address Book" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="323">
   <si>
     <t>UserName</t>
   </si>
@@ -1009,11 +1008,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1421,21 +1420,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL33" sqref="AL33:AL34"/>
+    <sheetView topLeftCell="N7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14:W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1463,7 +1462,7 @@
     <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1661,7 +1660,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1712,7 +1711,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1730,7 +1729,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1775,7 +1774,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1825,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1860,7 +1859,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1871,7 +1870,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2060,7 +2059,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2092,7 +2091,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2223,7 +2222,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2234,7 +2233,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2264,7 +2263,7 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -2304,7 +2303,7 @@
       </c>
       <c r="AM34" s="7"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2315,7 +2314,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2401,7 +2400,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2435,7 +2434,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2482,7 +2481,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:40">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:40">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2623,7 +2622,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:41">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2658,7 +2657,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:41">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:41">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:41">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:41">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2724,40 +2723,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B43" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D43" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C43" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K19" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="K22" r:id="rId7"/>
+    <hyperlink ref="K24" r:id="rId8"/>
+    <hyperlink ref="K26" r:id="rId9"/>
+    <hyperlink ref="B37" r:id="rId10"/>
+    <hyperlink ref="D37" r:id="rId11"/>
+    <hyperlink ref="E37" r:id="rId12"/>
+    <hyperlink ref="K37" r:id="rId13"/>
+    <hyperlink ref="K42" r:id="rId14"/>
+    <hyperlink ref="B43" r:id="rId15"/>
+    <hyperlink ref="D43" r:id="rId16"/>
+    <hyperlink ref="E43" r:id="rId17"/>
+    <hyperlink ref="C43" r:id="rId18"/>
+    <hyperlink ref="F9" r:id="rId19"/>
+    <hyperlink ref="D9" r:id="rId20"/>
+    <hyperlink ref="E9" r:id="rId21"/>
+    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123"/>
+    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123"/>
+    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com"/>
+    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123"/>
+    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234"/>
+    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com"/>
+    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com"/>
+    <hyperlink ref="K49" r:id="rId32"/>
+    <hyperlink ref="K50" r:id="rId33"/>
+    <hyperlink ref="B51" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -2765,20 +2764,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView topLeftCell="P2" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2855,7 +2854,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2924,11 +2923,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2936,14 +2935,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
@@ -2958,7 +2957,7 @@
     <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3092,7 +3091,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3126,26 +3125,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="AC4" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="AC4" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -3161,7 +3160,7 @@
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3229,7 +3228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3296,7 +3295,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3322,7 +3321,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -3348,7 +3347,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="187.2">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -3377,29 +3376,29 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
-    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:hydroflaskemea978+7@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:hydroflaskemea978+7@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" customWidth="1"/>
@@ -3408,7 +3407,7 @@
     <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3538,7 +3537,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3561,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3580,7 +3579,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3593,33 +3592,33 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Y4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N3" r:id="rId1" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="P3" r:id="rId4" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="R3" r:id="rId5" display="https://mcloud-na-stage3.drybar.com/gin-twist-curl-quenching-shampoo"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
@@ -3631,7 +3630,7 @@
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3686,7 +3685,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3698,7 +3697,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3714,7 +3713,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3743,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3754,7 +3753,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3778,31 +3777,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Testers@278"/>
+    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3933,7 +3932,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3979,7 +3978,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -4000,7 +3999,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -4014,7 +4013,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -4028,7 +4027,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4041,7 +4040,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4056,7 +4055,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4071,7 +4070,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4086,7 +4085,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4096,30 +4095,30 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -4128,7 +4127,7 @@
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4248,27 +4247,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4276,7 +4275,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4290,14 +4289,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
@@ -4318,7 +4317,7 @@
     <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4392,7 +4391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4443,7 +4442,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4495,7 +4494,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4549,7 +4548,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4576,7 +4575,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4591,7 +4590,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4604,38 +4603,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="C2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId12"/>
+    <hyperlink ref="C5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4742,7 +4741,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4790,7 +4789,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4799,7 +4798,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4810,7 +4809,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4831,14 +4830,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4858,7 +4857,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4887,7 +4886,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4919,7 +4918,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4940,7 +4939,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4980,7 +4979,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -5007,7 +5006,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -5021,7 +5020,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -5029,7 +5028,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -5037,7 +5036,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5045,33 +5044,33 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AK38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16"/>
+      <selection activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
@@ -5082,7 +5081,7 @@
     <col min="37" max="37" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5195,7 +5194,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5240,8 +5239,11 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5249,8 +5251,11 @@
       <c r="E3" s="2"/>
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5258,8 +5263,11 @@
       <c r="E4" s="2"/>
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5269,8 +5277,11 @@
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5282,8 +5293,11 @@
       <c r="Y6" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5295,8 +5309,11 @@
       <c r="Y7" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5306,32 +5323,38 @@
         <v>2</v>
       </c>
       <c r="AI8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>304</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="Y9" s="5"/>
+      <c r="AI9" t="s">
+        <v>259</v>
+      </c>
       <c r="AJ9" s="7" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>312</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="Y10" s="5"/>
+      <c r="AI10" t="s">
+        <v>259</v>
+      </c>
       <c r="AJ10" s="7" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5344,8 +5367,11 @@
       <c r="W11">
         <v>123</v>
       </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5360,8 +5386,11 @@
       <c r="W12">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5374,76 +5403,73 @@
       <c r="W13">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
+        <v>306</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="W14">
+        <v>123</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
-      <c r="U15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="W15">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="U16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="W16">
+        <v>123</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="AI17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" t="s">
         <v>55</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" t="s">
-        <v>56</v>
-      </c>
-      <c r="O17" t="s">
-        <v>57</v>
-      </c>
-      <c r="P17" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>58</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="S17">
-        <v>9898989898</v>
-      </c>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>146</v>
       </c>
       <c r="F18" t="s">
         <v>47</v>
@@ -5455,409 +5481,465 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
       <c r="O18" t="s">
-        <v>149</v>
+        <v>261</v>
       </c>
       <c r="P18" t="s">
-        <v>52</v>
+        <v>263</v>
       </c>
       <c r="Q18" t="s">
-        <v>147</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>148</v>
+        <v>262</v>
+      </c>
+      <c r="R18" t="s">
+        <v>264</v>
       </c>
       <c r="S18">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" t="s">
+        <v>150</v>
+      </c>
+      <c r="O19" t="s">
+        <v>149</v>
+      </c>
+      <c r="P19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>147</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="S19">
+        <v>9898989898</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" t="s">
         <v>62</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>62</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>63</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>64</v>
       </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="AI20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="X20" s="5" t="s">
+      <c r="X21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Y20" s="5" t="s">
+      <c r="Y21" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="AI21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" t="s">
         <v>72</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>48</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>77</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N22" t="s">
         <v>73</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>74</v>
-      </c>
-      <c r="P21" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>75</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S21">
-        <v>9898989898</v>
-      </c>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>79</v>
-      </c>
-      <c r="N22" t="s">
-        <v>80</v>
-      </c>
-      <c r="O22" t="s">
-        <v>81</v>
       </c>
       <c r="P22" t="s">
         <v>52</v>
       </c>
       <c r="Q22" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
+        <v>79</v>
+      </c>
+      <c r="N23" t="s">
+        <v>80</v>
+      </c>
+      <c r="O23" t="s">
+        <v>81</v>
+      </c>
+      <c r="P23" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>82</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S23">
+        <v>9898989898</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="7"/>
-      <c r="K23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M23" t="s">
-        <v>291</v>
-      </c>
-      <c r="N23" t="s">
-        <v>260</v>
-      </c>
-      <c r="O23" t="s">
-        <v>261</v>
-      </c>
-      <c r="P23" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>262</v>
-      </c>
-      <c r="R23" t="s">
-        <v>264</v>
-      </c>
-      <c r="S23" s="9">
-        <v>9898989898</v>
-      </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="2"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>290</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="7"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="7"/>
-      <c r="K24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="M24" t="s">
         <v>291</v>
       </c>
       <c r="N24" t="s">
-        <v>289</v>
-      </c>
-      <c r="S24" s="9"/>
+        <v>260</v>
+      </c>
+      <c r="O24" t="s">
+        <v>261</v>
+      </c>
+      <c r="P24" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>262</v>
+      </c>
+      <c r="R24" t="s">
+        <v>264</v>
+      </c>
+      <c r="S24" s="9">
+        <v>9898989898</v>
+      </c>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
       <c r="W24" s="2"/>
       <c r="AD24" s="5"/>
       <c r="AE24" s="5"/>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AI24" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="7"/>
+      <c r="K25" s="2"/>
+      <c r="M25" t="s">
+        <v>291</v>
+      </c>
+      <c r="N25" t="s">
+        <v>289</v>
+      </c>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="2"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AI25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" t="s">
         <v>94</v>
       </c>
-      <c r="X25" t="s">
+      <c r="X26" t="s">
         <v>316</v>
       </c>
-      <c r="Y25" s="5" t="s">
+      <c r="Y26" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="Z26" t="s">
         <v>317</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AA26" t="s">
         <v>319</v>
       </c>
-      <c r="AI25" t="s">
+      <c r="AI26" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>79</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O27" t="s">
+        <v>100</v>
+      </c>
+      <c r="P27" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>101</v>
+      </c>
+      <c r="R27" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="S27" s="9">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R28" s="10"/>
+      <c r="S28" s="9"/>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="M29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="V30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7"/>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI32" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" t="s">
+    <row r="33" spans="1:37">
+      <c r="A33" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ33" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AK33" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" t="s">
+        <v>161</v>
+      </c>
+      <c r="M34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
+      <c r="A35" t="s">
+        <v>163</v>
+      </c>
+      <c r="X35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" t="s">
+        <v>172</v>
+      </c>
+      <c r="X36" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" t="s">
+        <v>183</v>
+      </c>
+      <c r="F37" t="s">
         <v>78</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G37" t="s">
         <v>79</v>
       </c>
-      <c r="K26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N26" t="s">
-        <v>99</v>
-      </c>
-      <c r="O26" t="s">
-        <v>100</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="K37" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N37" t="s">
+        <v>80</v>
+      </c>
+      <c r="O37" t="s">
+        <v>81</v>
+      </c>
+      <c r="P37" t="s">
         <v>52</v>
       </c>
-      <c r="Q26" t="s">
-        <v>101</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="S26" s="9">
+      <c r="Q37" t="s">
+        <v>82</v>
+      </c>
+      <c r="R37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S37">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>104</v>
-      </c>
-      <c r="M27" t="s">
-        <v>103</v>
-      </c>
-      <c r="R27" s="10"/>
-      <c r="S27" s="9"/>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>105</v>
-      </c>
-      <c r="M28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>109</v>
-      </c>
-      <c r="U29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="V29" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>113</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ30" s="7"/>
-      <c r="AK30" s="7"/>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI31" t="s">
+      <c r="T37">
+        <v>888888</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V37" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="W37" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI37" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>158</v>
-      </c>
-      <c r="AJ32" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="AK32" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>161</v>
-      </c>
-      <c r="M33" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>163</v>
-      </c>
-      <c r="X34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>172</v>
-      </c>
-      <c r="X35" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="Y35" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>183</v>
-      </c>
-      <c r="F36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G36" t="s">
-        <v>79</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="N36" t="s">
-        <v>80</v>
-      </c>
-      <c r="O36" t="s">
-        <v>81</v>
-      </c>
-      <c r="P36" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>82</v>
-      </c>
-      <c r="R36" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S36">
-        <v>9898989898</v>
-      </c>
-      <c r="T36">
-        <v>888888</v>
-      </c>
-      <c r="U36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V36" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W36" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:37">
+      <c r="A38" t="s">
         <v>219</v>
       </c>
-      <c r="X37" t="s">
+      <c r="X38" t="s">
         <v>221</v>
-      </c>
-      <c r="Y37" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>220</v>
-      </c>
-      <c r="X38" t="s">
-        <v>222</v>
       </c>
       <c r="Y38" s="5" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="39" spans="1:37">
+      <c r="A39" t="s">
+        <v>220</v>
+      </c>
+      <c r="X39" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y39" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K17" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="K21" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="K23" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="K26" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="K18" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="K36" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="K22" r:id="rId6"/>
+    <hyperlink ref="K24" r:id="rId7"/>
+    <hyperlink ref="K27" r:id="rId8"/>
+    <hyperlink ref="K19" r:id="rId9"/>
+    <hyperlink ref="K37" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
84 testcase changes for drybar us
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView topLeftCell="N7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14:W14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4"/>
@@ -5066,8 +5066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AJ19" sqref="AJ19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5075,6 +5075,9 @@
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
@@ -5542,10 +5545,10 @@
         <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>311</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -5566,7 +5569,7 @@
         <v>65</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>66</v>
+        <v>309</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Dry Uk - Test cases 179,84,85
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FF09DE-B03C-4A3B-9364-ECF7C5E96CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF6B44-C26C-4F47-808F-90C9071BC6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="327">
   <si>
     <t>UserName</t>
   </si>
@@ -1010,6 +1010,12 @@
   </si>
   <si>
     <t>TEST_DRYBAR_PROMO_8878</t>
+  </si>
+  <si>
+    <t>Same SKU Product</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo Lush Scent Full Size</t>
   </si>
 </sst>
 </file>
@@ -1437,39 +1443,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:AL54"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="16" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.28515625" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.33203125" customWidth="1"/>
+    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1594,22 +1600,14 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>168</v>
-      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>48</v>
       </c>
@@ -1643,7 +1641,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1655,7 +1653,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1667,7 +1665,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1683,7 +1681,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1703,7 +1701,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1718,7 +1716,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1736,7 +1734,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1781,7 +1779,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1796,7 +1794,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1813,7 +1811,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1832,7 +1830,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1849,7 +1847,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -1866,7 +1864,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1877,7 +1875,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1887,7 +1885,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1910,7 +1908,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1945,7 +1943,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1955,9 +1953,7 @@
       <c r="G19" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="8" t="s">
-        <v>188</v>
-      </c>
+      <c r="K19" s="8"/>
       <c r="N19" t="s">
         <v>260</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2006,7 +2002,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2031,7 +2027,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2066,7 +2062,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2098,7 +2094,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2144,7 +2140,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2165,7 +2161,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2203,7 +2199,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2216,7 +2212,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -2229,7 +2225,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2240,7 +2236,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2257,7 +2253,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2270,7 +2266,7 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2284,7 +2280,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -2298,7 +2294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -2310,7 +2306,7 @@
       </c>
       <c r="AM34" s="7"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2321,7 +2317,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2337,7 +2333,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2363,7 +2359,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2382,7 +2378,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2407,7 +2403,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2424,7 +2420,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2441,7 +2437,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2488,16 +2484,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>187</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>188</v>
-      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="8" t="s">
         <v>168</v>
       </c>
@@ -2508,7 +2500,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2540,7 +2532,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2574,7 +2566,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2604,7 +2596,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2618,7 +2610,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2629,7 +2621,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2664,7 +2656,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2678,7 +2670,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>284</v>
       </c>
@@ -2692,7 +2684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
@@ -2703,7 +2695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -2728,7 +2720,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>323</v>
       </c>
@@ -2739,42 +2731,35 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="K24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="K26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="K37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="K42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B43" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D43" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C43" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B45" r:id="rId22" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C45" r:id="rId23" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D45" r:id="rId24" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E45" r:id="rId25" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K45" r:id="rId26" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B46" r:id="rId27" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D46" r:id="rId28" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E46" r:id="rId29" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K46" r:id="rId30" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L46" r:id="rId31" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="K50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="K22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B37" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D37" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E37" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K42" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E43" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B45" r:id="rId15" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C45" r:id="rId16" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D45" r:id="rId17" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E45" r:id="rId18" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K45" r:id="rId19" display="mailto:hydroflaskemea978+7@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B46" r:id="rId20" display="mailto:hydroflaskemea978+8@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D46" r:id="rId21" display="mailto:Lotus@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E46" r:id="rId22" display="mailto:Lotuswave@1234" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K46" r:id="rId23" display="mailto:avayugundla@helenoftroy.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L46" r:id="rId24" display="mailto:hydroflaskemea978+2@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K49" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K50" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B51" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId35"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -2786,13 +2771,13 @@
       <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2869,7 +2854,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2910,7 +2895,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2957,22 +2942,22 @@
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3061,7 +3046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3106,7 +3091,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3127,7 +3112,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3159,23 +3144,23 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3243,7 +3228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3284,7 +3269,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3310,7 +3295,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3336,7 +3321,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -3362,7 +3347,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -3391,7 +3376,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
@@ -3413,16 +3398,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" customWidth="1"/>
-    <col min="28" max="28" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3511,7 +3496,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3552,7 +3537,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3575,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3583,7 +3568,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3594,7 +3579,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3607,7 +3592,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3629,23 +3614,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3680,27 +3665,19 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>60</v>
-      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3712,7 +3689,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3728,7 +3705,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3746,7 +3723,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3757,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3768,7 +3745,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3782,7 +3759,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3793,10 +3770,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" display="Testers@278" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3806,17 +3779,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3947,22 +3920,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>48</v>
       </c>
@@ -3993,7 +3958,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -4014,7 +3979,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -4028,7 +3993,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -4042,7 +4007,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4055,7 +4020,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4070,7 +4035,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4085,7 +4050,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4100,7 +4065,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4110,17 +4075,11 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4133,16 +4092,16 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4246,7 +4205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4276,13 +4235,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4290,7 +4249,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4311,28 +4270,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4406,7 +4365,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4457,7 +4416,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4509,7 +4468,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4563,7 +4522,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4590,7 +4549,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4605,7 +4564,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4640,16 +4599,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4756,16 +4715,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
         <v>60</v>
       </c>
@@ -4778,9 +4733,7 @@
       <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
@@ -4804,7 +4757,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4813,7 +4766,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4824,7 +4777,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4837,7 +4790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4845,14 +4798,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4872,7 +4825,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4901,7 +4854,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4933,7 +4886,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4954,7 +4907,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4965,7 +4918,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4994,7 +4947,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -5021,7 +4974,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -5035,7 +4988,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -5043,7 +4996,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -5051,7 +5004,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5059,19 +5012,16 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K2" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="K14" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K10" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5079,27 +5029,27 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AK39"/>
+  <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="K29" workbookViewId="0">
+      <selection activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5212,7 +5162,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5261,7 +5211,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5273,7 +5223,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5285,7 +5235,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5299,7 +5249,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5315,7 +5265,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5331,7 +5281,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5344,7 +5294,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -5358,7 +5308,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>312</v>
       </c>
@@ -5372,7 +5322,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5389,7 +5339,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5408,7 +5358,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5425,7 +5375,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -5442,7 +5392,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5452,7 +5402,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5475,7 +5425,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5485,7 +5435,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5520,7 +5470,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -5555,7 +5505,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -5579,7 +5529,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -5593,7 +5543,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -5628,7 +5578,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -5660,7 +5610,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -5706,7 +5656,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>290</v>
       </c>
@@ -5734,7 +5684,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -5754,7 +5704,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -5786,7 +5736,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -5796,7 +5746,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -5804,7 +5754,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -5818,7 +5768,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -5828,7 +5778,7 @@
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -5839,7 +5789,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -5850,7 +5800,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -5858,7 +5808,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>163</v>
       </c>
@@ -5866,7 +5816,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -5877,7 +5827,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -5924,7 +5874,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>219</v>
       </c>
@@ -5935,7 +5885,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>220</v>
       </c>
@@ -5943,6 +5893,17 @@
         <v>222</v>
       </c>
       <c r="Y39" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>325</v>
+      </c>
+      <c r="X40" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="Y40" s="5" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel and helper changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF6B44-C26C-4F47-808F-90C9071BC6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7F1A11-C5C2-4116-83DB-8978A5749921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5655" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="326">
   <si>
     <t>UserName</t>
   </si>
@@ -877,9 +877,6 @@
   </si>
   <si>
     <t>good product</t>
-  </si>
-  <si>
-    <t>DRYQATEST20</t>
   </si>
   <si>
     <t>.</t>
@@ -1443,39 +1440,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="AJ16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM25" sqref="AM25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="16" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.33203125" customWidth="1"/>
-    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.28515625" customWidth="1"/>
+    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>258</v>
@@ -1600,7 +1597,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1641,7 +1638,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1653,7 +1650,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1665,7 +1662,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1701,14 +1698,14 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Y7" s="5">
         <v>2</v>
@@ -1716,14 +1713,14 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>160</v>
@@ -1734,7 +1731,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1779,7 +1776,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1794,7 +1791,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1811,7 +1808,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1830,7 +1827,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1847,12 +1844,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>305</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>307</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -1864,7 +1861,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1875,7 +1872,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1885,7 +1882,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1908,7 +1905,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1943,7 +1940,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1976,7 +1973,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1984,7 +1981,7 @@
         <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -2002,7 +1999,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2010,10 +2007,10 @@
         <v>240</v>
       </c>
       <c r="I21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -2024,10 +2021,10 @@
         <v>259</v>
       </c>
       <c r="AO21" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2094,7 +2091,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2110,7 +2107,7 @@
         <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N24" t="s">
         <v>260</v>
@@ -2140,28 +2137,28 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
       <c r="X25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AA25" s="5"/>
       <c r="AB25" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AK25" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2172,7 +2169,7 @@
         <v>79</v>
       </c>
       <c r="I26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>46</v>
@@ -2199,7 +2196,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2212,31 +2209,31 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>289</v>
+      </c>
+      <c r="M28" t="s">
         <v>290</v>
       </c>
-      <c r="M28" t="s">
-        <v>291</v>
-      </c>
       <c r="N28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
       <c r="M29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AK29" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2266,12 +2263,12 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
       <c r="AE32" t="s">
-        <v>282</v>
+        <v>144</v>
       </c>
       <c r="AF32" t="s">
         <v>144</v>
@@ -2280,33 +2277,33 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>303</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL33" s="7" t="s">
         <v>304</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>259</v>
-      </c>
-      <c r="AL33" s="7" t="s">
-        <v>305</v>
       </c>
       <c r="AM33" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>311</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL34" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="AK34" t="s">
-        <v>259</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>313</v>
-      </c>
       <c r="AM34" s="7"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2317,7 +2314,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2333,7 +2330,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2359,7 +2356,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2378,7 +2375,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2403,7 +2400,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2414,13 +2411,13 @@
         <v>259</v>
       </c>
       <c r="AL40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2437,7 +2434,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2500,7 +2497,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2532,7 +2529,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2566,7 +2563,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2596,7 +2593,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2610,7 +2607,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2621,7 +2618,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2656,7 +2653,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2670,34 +2667,34 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>181</v>
       </c>
       <c r="X51" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="X52" t="s">
         <v>286</v>
-      </c>
-      <c r="X52" t="s">
-        <v>287</v>
       </c>
       <c r="Y52">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H53" t="s">
         <v>62</v>
@@ -2706,7 +2703,7 @@
         <v>63</v>
       </c>
       <c r="X53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y53" s="5" t="s">
         <v>67</v>
@@ -2717,15 +2714,15 @@
         <v>259</v>
       </c>
       <c r="AO53" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>322</v>
+      </c>
+      <c r="AL54" t="s">
         <v>323</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2771,13 +2768,13 @@
       <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2854,7 +2851,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2895,7 +2892,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2903,16 +2900,16 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q3" t="s">
         <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -2942,22 +2939,22 @@
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3016,7 +3013,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>123</v>
@@ -3046,7 +3043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3091,7 +3088,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3103,24 +3100,24 @@
         <v>97</v>
       </c>
       <c r="V3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>276</v>
       </c>
       <c r="AB4" t="s">
+        <v>293</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>294</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3144,23 +3141,23 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3201,7 +3198,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>22</v>
@@ -3228,7 +3225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3266,10 +3263,10 @@
         <v>209</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3280,7 +3277,7 @@
         <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J3" t="s">
         <v>271</v>
@@ -3292,12 +3289,12 @@
         <v>273</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>213</v>
@@ -3321,9 +3318,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G5" t="s">
         <v>78</v>
@@ -3332,7 +3329,7 @@
         <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J5" t="s">
         <v>271</v>
@@ -3344,12 +3341,12 @@
         <v>273</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G6" t="s">
         <v>78</v>
@@ -3370,13 +3367,13 @@
         <v>209</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
@@ -3398,16 +3395,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="25" max="25" width="36.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" customWidth="1"/>
-    <col min="28" max="28" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="36.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3496,7 +3493,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3537,7 +3534,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3560,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3568,7 +3565,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3579,7 +3576,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3592,7 +3589,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3614,23 +3611,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3677,7 +3674,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3689,7 +3686,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3705,7 +3702,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3723,7 +3720,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3734,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3745,7 +3742,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3759,7 +3756,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3783,13 +3780,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3920,7 +3917,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3958,7 +3955,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3979,7 +3976,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -3993,7 +3990,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -4007,7 +4004,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4020,7 +4017,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4035,7 +4032,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4050,7 +4047,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4065,7 +4062,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4075,7 +4072,7 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
@@ -4092,16 +4089,16 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4205,7 +4202,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4235,13 +4232,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4249,7 +4246,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4270,28 +4267,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4365,7 +4362,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4416,7 +4413,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4468,7 +4465,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4522,7 +4519,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4549,7 +4546,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4564,7 +4561,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4603,12 +4600,12 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4715,7 +4712,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4757,7 +4754,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4766,7 +4763,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4777,7 +4774,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4790,7 +4787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4798,14 +4795,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4825,7 +4822,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4854,7 +4851,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4886,7 +4883,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4894,7 +4891,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
@@ -4907,7 +4904,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4918,7 +4915,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4947,7 +4944,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4974,12 +4971,12 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>67</v>
@@ -4988,7 +4985,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4996,7 +4993,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -5004,7 +5001,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5012,7 +5009,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
@@ -5035,21 +5032,21 @@
       <selection activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5129,7 +5126,7 @@
         <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5162,7 +5159,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5211,7 +5208,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5223,7 +5220,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5235,7 +5232,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5249,7 +5246,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5265,7 +5262,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5281,7 +5278,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5294,9 +5291,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -5305,12 +5302,12 @@
         <v>259</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -5319,10 +5316,10 @@
         <v>259</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5339,7 +5336,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5358,7 +5355,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5375,12 +5372,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>305</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>307</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -5392,7 +5389,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5402,7 +5399,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5425,7 +5422,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5435,7 +5432,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5470,7 +5467,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -5505,7 +5502,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -5513,7 +5510,7 @@
         <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -5529,12 +5526,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -5543,7 +5540,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -5578,7 +5575,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -5626,7 +5623,7 @@
         <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N24" t="s">
         <v>260</v>
@@ -5656,9 +5653,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="7"/>
@@ -5668,10 +5665,10 @@
       <c r="H25" s="7"/>
       <c r="K25" s="2"/>
       <c r="M25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
@@ -5684,27 +5681,27 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>94</v>
       </c>
       <c r="X26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Y26" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AA26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AI26" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -5736,7 +5733,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -5746,7 +5743,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -5754,7 +5751,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -5768,7 +5765,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -5778,7 +5775,7 @@
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -5789,7 +5786,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -5800,7 +5797,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -5808,7 +5805,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>163</v>
       </c>
@@ -5816,18 +5813,18 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -5874,7 +5871,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>219</v>
       </c>
@@ -5885,7 +5882,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>220</v>
       </c>
@@ -5896,12 +5893,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>324</v>
+      </c>
+      <c r="X40" s="24" t="s">
         <v>325</v>
-      </c>
-      <c r="X40" s="24" t="s">
-        <v>326</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Dry Uk 150 instock product
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA38B2B-58EF-41D9-AE72-F213C4EE5D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46125AE-AEA6-4FBC-B823-263106C38464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1443,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL55" sqref="AL55"/>
+    <sheetView topLeftCell="O3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4607,8 +4607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4920,7 +4920,7 @@
         <v>65</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
174 testcase change for drybar Uk
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46125AE-AEA6-4FBC-B823-263106C38464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A37938B-B8FE-4F92-9283-13E671367FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -939,83 +939,83 @@
     <t>New BillingAddress</t>
   </si>
   <si>
-    <t>QA TEST
+    <t>Partial GiftCode</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_7297</t>
+  </si>
+  <si>
+    <t>3d_Secure</t>
+  </si>
+  <si>
+    <t>4000000000003220</t>
+  </si>
+  <si>
+    <t>Product_2</t>
+  </si>
+  <si>
+    <t>Buttercup Blow-Dryer</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_5759</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All Hair Tools</t>
+  </si>
+  <si>
+    <t>Partial GiftCode1</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_3484</t>
+  </si>
+  <si>
+    <t>Double Pint Large Round Ceramic Brush</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo Bundle Test</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo</t>
+  </si>
+  <si>
+    <t>Travel Size: 40g/1.4 oz.</t>
+  </si>
+  <si>
+    <t>scent</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Big Swig Thickening Spray</t>
+  </si>
+  <si>
+    <t>Lush</t>
+  </si>
+  <si>
+    <t>Full Size: 100g/3.5 oz.</t>
+  </si>
+  <si>
+    <t>Partial GiftCode-2</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_8878</t>
+  </si>
+  <si>
+    <t>Same SKU Product</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo Lush Scent Full Size</t>
+  </si>
+  <si>
+    <t>GiftCode Partial Redeem</t>
+  </si>
+  <si>
+    <t>Qa Test
 93 York House
 Bradford, West Yorkshire, BD109ET
 United Kingdom
 T: 9999999999</t>
-  </si>
-  <si>
-    <t>Partial GiftCode</t>
-  </si>
-  <si>
-    <t>TEST_DRYBAR_PROMO_7297</t>
-  </si>
-  <si>
-    <t>3d_Secure</t>
-  </si>
-  <si>
-    <t>4000000000003220</t>
-  </si>
-  <si>
-    <t>Product_2</t>
-  </si>
-  <si>
-    <t>Buttercup Blow-Dryer</t>
-  </si>
-  <si>
-    <t>TEST_DRYBAR_PROMO_5759</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> All Hair Tools</t>
-  </si>
-  <si>
-    <t>Partial GiftCode1</t>
-  </si>
-  <si>
-    <t>TEST_DRYBAR_PROMO_3484</t>
-  </si>
-  <si>
-    <t>Double Pint Large Round Ceramic Brush</t>
-  </si>
-  <si>
-    <t>Detox Dry Shampoo Bundle Test</t>
-  </si>
-  <si>
-    <t>Detox Dry Shampoo</t>
-  </si>
-  <si>
-    <t>Travel Size: 40g/1.4 oz.</t>
-  </si>
-  <si>
-    <t>scent</t>
-  </si>
-  <si>
-    <t>Original</t>
-  </si>
-  <si>
-    <t>Big Swig Thickening Spray</t>
-  </si>
-  <si>
-    <t>Lush</t>
-  </si>
-  <si>
-    <t>Full Size: 100g/3.5 oz.</t>
-  </si>
-  <si>
-    <t>Partial GiftCode-2</t>
-  </si>
-  <si>
-    <t>TEST_DRYBAR_PROMO_8878</t>
-  </si>
-  <si>
-    <t>Same SKU Product</t>
-  </si>
-  <si>
-    <t>Detox Dry Shampoo Lush Scent Full Size</t>
-  </si>
-  <si>
-    <t>GiftCode Partial Redeem</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1552,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>258</v>
@@ -1703,12 +1703,12 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y7" s="5">
         <v>2</v>
@@ -1723,7 +1723,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>160</v>
@@ -1849,10 +1849,10 @@
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>304</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -1984,7 +1984,7 @@
         <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -2010,10 +2010,10 @@
         <v>240</v>
       </c>
       <c r="I21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -2145,17 +2145,17 @@
         <v>94</v>
       </c>
       <c r="X25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AA25" s="5"/>
       <c r="AB25" s="25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AK25" t="s">
         <v>259</v>
@@ -2282,13 +2282,13 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>302</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL33" s="7" t="s">
         <v>303</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>259</v>
-      </c>
-      <c r="AL33" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="AM33" s="7" t="s">
         <v>157</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>310</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL34" s="7" t="s">
         <v>311</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>259</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>312</v>
       </c>
       <c r="AM34" s="7"/>
     </row>
@@ -2414,7 +2414,7 @@
         <v>259</v>
       </c>
       <c r="AL40" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>157</v>
@@ -2722,18 +2722,18 @@
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>321</v>
+      </c>
+      <c r="AL54" t="s">
         <v>322</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL55" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2911,16 +2911,16 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q3" t="s">
         <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -3148,8 +3148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,7 +3381,7 @@
         <v>297</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>302</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
@@ -4902,7 +4902,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
@@ -4920,7 +4920,7 @@
         <v>65</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>67</v>
@@ -4987,7 +4987,7 @@
         <v>94</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>67</v>
@@ -5137,7 +5137,7 @@
         <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5304,7 +5304,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -5313,12 +5313,12 @@
         <v>259</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -5327,7 +5327,7 @@
         <v>259</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -5385,10 +5385,10 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>304</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -5521,7 +5521,7 @@
         <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -5542,7 +5542,7 @@
         <v>65</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -5697,16 +5697,16 @@
         <v>94</v>
       </c>
       <c r="X26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y26" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AI26" t="s">
         <v>259</v>
@@ -5829,7 +5829,7 @@
         <v>172</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>67</v>
@@ -5906,10 +5906,10 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>323</v>
+      </c>
+      <c r="X40" s="24" t="s">
         <v>324</v>
-      </c>
-      <c r="X40" s="24" t="s">
-        <v>325</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
165 testcase for drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38F425B-0365-494E-888E-215123D063B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0A205B-6493-4A1F-B678-938997621E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="328">
   <si>
     <t>UserName</t>
   </si>
@@ -1102,7 +1102,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF17C6A3"/>
+      <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -1446,39 +1446,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE27" sqref="AE27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="16" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.33203125" customWidth="1"/>
-    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.28515625" customWidth="1"/>
+    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>306</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>304</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>289</v>
       </c>
@@ -2228,7 +2228,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>302</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>310</v>
       </c>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="AM34" s="7"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>166</v>
       </c>
@@ -2565,11 +2565,29 @@
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
+      <c r="N45" t="s">
+        <v>260</v>
+      </c>
+      <c r="O45" t="s">
+        <v>261</v>
+      </c>
+      <c r="P45" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>262</v>
+      </c>
+      <c r="R45" t="s">
+        <v>264</v>
+      </c>
+      <c r="S45">
+        <v>9898989898</v>
+      </c>
       <c r="AK45" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>215</v>
       </c>
@@ -2599,7 +2617,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -2613,7 +2631,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>255</v>
       </c>
@@ -2624,7 +2642,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2659,7 +2677,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>279</v>
       </c>
@@ -2673,7 +2691,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>283</v>
       </c>
@@ -2687,7 +2705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>285</v>
       </c>
@@ -2698,7 +2716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>295</v>
       </c>
@@ -2723,7 +2741,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>321</v>
       </c>
@@ -2731,7 +2749,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>325</v>
       </c>
@@ -2782,13 +2800,13 @@
       <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2865,7 +2883,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2906,7 +2924,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -2953,22 +2971,22 @@
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3057,7 +3075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3102,7 +3120,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3123,7 +3141,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3155,23 +3173,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3239,7 +3257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -3280,7 +3298,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3306,7 +3324,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -3332,7 +3350,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>300</v>
       </c>
@@ -3358,7 +3376,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>301</v>
       </c>
@@ -3387,7 +3405,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
@@ -3409,16 +3427,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="25" max="25" width="36.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" customWidth="1"/>
-    <col min="28" max="28" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="36.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3507,7 +3525,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3548,7 +3566,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -3571,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3579,7 +3597,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3590,7 +3608,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3603,7 +3621,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3629,19 +3647,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3676,7 +3694,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>274</v>
       </c>
@@ -3688,7 +3706,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>275</v>
       </c>
@@ -3700,7 +3718,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3716,7 +3734,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>276</v>
       </c>
@@ -3734,7 +3752,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3745,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>276</v>
       </c>
@@ -3756,7 +3774,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3770,7 +3788,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -3794,13 +3812,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3931,7 +3949,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3969,7 +3987,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3990,7 +4008,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -4004,7 +4022,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -4018,7 +4036,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4031,7 +4049,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4046,7 +4064,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4061,7 +4079,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4076,7 +4094,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4086,7 +4104,7 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
@@ -4103,16 +4121,16 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4216,7 +4234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4246,13 +4264,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4260,7 +4278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4281,28 +4299,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4376,7 +4394,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4427,7 +4445,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4479,7 +4497,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4533,7 +4551,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4560,7 +4578,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4575,7 +4593,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4614,12 +4632,12 @@
       <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4726,7 +4744,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4768,7 +4786,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4777,7 +4795,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4788,7 +4806,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4801,7 +4819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4809,14 +4827,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4836,7 +4854,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4865,7 +4883,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4897,7 +4915,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -4918,7 +4936,7 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4929,7 +4947,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4958,7 +4976,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4985,7 +5003,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4999,7 +5017,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -5007,7 +5025,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -5015,7 +5033,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -5023,7 +5041,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
@@ -5046,21 +5064,21 @@
       <selection activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5173,7 +5191,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5222,7 +5240,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5234,7 +5252,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5246,7 +5264,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5260,7 +5278,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5276,7 +5294,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -5292,7 +5310,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5305,7 +5323,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>302</v>
       </c>
@@ -5319,7 +5337,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>310</v>
       </c>
@@ -5333,7 +5351,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5350,7 +5368,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5369,7 +5387,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5386,7 +5404,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>304</v>
       </c>
@@ -5403,7 +5421,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5413,7 +5431,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5436,7 +5454,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5446,7 +5464,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5481,7 +5499,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -5516,7 +5534,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -5540,7 +5558,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -5554,7 +5572,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -5589,7 +5607,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -5621,7 +5639,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -5667,7 +5685,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>289</v>
       </c>
@@ -5695,7 +5713,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -5715,7 +5733,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -5747,7 +5765,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -5757,7 +5775,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -5765,7 +5783,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -5779,7 +5797,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -5789,7 +5807,7 @@
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -5800,7 +5818,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -5811,7 +5829,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -5819,7 +5837,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>163</v>
       </c>
@@ -5827,7 +5845,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -5838,7 +5856,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -5885,7 +5903,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>219</v>
       </c>
@@ -5896,7 +5914,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>220</v>
       </c>
@@ -5907,7 +5925,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>323</v>
       </c>

</xml_diff>

<commit_message>
116 Testcase changes for drybar UK Express Paypal related
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_UK/GoldDrybarUKTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699C27BA-8525-412B-B599-6F9A88A9811C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE21B638-FDD3-4507-9A6B-C0C3A9B4611C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="328">
   <si>
     <t>UserName</t>
   </si>
@@ -889,9 +889,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Blow-Dryers</t>
-  </si>
-  <si>
-    <t>Test Qa - 84/4 Great King Street, Edinburgh, MIDLOTHIAN, EH36QU</t>
   </si>
   <si>
     <t>Express Paypal</t>
@@ -1449,39 +1446,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="16" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.28515625" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.33203125" customWidth="1"/>
+    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>256</v>
@@ -1606,7 +1603,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1655,7 +1652,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1667,7 +1664,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1679,7 +1676,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1695,7 +1692,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1715,14 +1712,14 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y7" s="5">
         <v>2</v>
@@ -1730,14 +1727,14 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>157</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>158</v>
@@ -1748,7 +1745,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1793,7 +1790,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1808,12 +1805,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>53</v>
@@ -1825,7 +1822,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1841,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1861,12 +1858,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>301</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>303</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>69</v>
@@ -1878,7 +1875,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1889,7 +1886,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1899,7 +1896,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1910,7 +1907,7 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="U17" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V17" s="5" t="s">
         <v>53</v>
@@ -1922,7 +1919,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1957,7 +1954,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1990,7 +1987,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1998,7 +1995,7 @@
         <v>238</v>
       </c>
       <c r="I20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J20" t="s">
         <v>63</v>
@@ -2016,7 +2013,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -2024,10 +2021,10 @@
         <v>238</v>
       </c>
       <c r="I21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>66</v>
@@ -2041,7 +2038,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2076,7 +2073,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2108,7 +2105,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -2124,7 +2121,7 @@
         <v>83</v>
       </c>
       <c r="M24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N24" t="s">
         <v>258</v>
@@ -2154,28 +2151,28 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>92</v>
       </c>
       <c r="X25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>66</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AA25" s="5"/>
       <c r="AB25" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AK25" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2213,7 +2210,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -2226,31 +2223,31 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>286</v>
+      </c>
+      <c r="M28" t="s">
         <v>287</v>
       </c>
-      <c r="M28" t="s">
-        <v>288</v>
-      </c>
       <c r="N28" t="s">
-        <v>286</v>
+        <v>327</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>103</v>
       </c>
       <c r="M29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AK29" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -2267,7 +2264,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2280,47 +2277,47 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>143</v>
       </c>
       <c r="AE32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AF32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AK32" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>257</v>
+      </c>
+      <c r="AL33" s="7" t="s">
         <v>300</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>257</v>
-      </c>
-      <c r="AL33" s="7" t="s">
-        <v>301</v>
       </c>
       <c r="AM33" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>307</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>257</v>
+      </c>
+      <c r="AL34" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="AK34" t="s">
-        <v>257</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>309</v>
-      </c>
       <c r="AM34" s="7"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -2331,7 +2328,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -2347,7 +2344,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>164</v>
       </c>
@@ -2373,7 +2370,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>171</v>
       </c>
@@ -2392,7 +2389,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>172</v>
       </c>
@@ -2417,7 +2414,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>177</v>
       </c>
@@ -2428,13 +2425,13 @@
         <v>257</v>
       </c>
       <c r="AL40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -2451,7 +2448,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>181</v>
       </c>
@@ -2486,7 +2483,7 @@
         <v>888888</v>
       </c>
       <c r="U42" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V42" s="5" t="s">
         <v>183</v>
@@ -2498,7 +2495,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -2514,7 +2511,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>187</v>
       </c>
@@ -2546,7 +2543,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>164</v>
       </c>
@@ -2598,7 +2595,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>213</v>
       </c>
@@ -2628,7 +2625,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>221</v>
       </c>
@@ -2642,7 +2639,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>253</v>
       </c>
@@ -2653,7 +2650,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -2688,7 +2685,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>277</v>
       </c>
@@ -2702,7 +2699,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>281</v>
       </c>
@@ -2716,7 +2713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>283</v>
       </c>
@@ -2727,9 +2724,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H53" t="s">
         <v>61</v>
@@ -2752,20 +2749,20 @@
         <v>285</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>318</v>
+      </c>
+      <c r="AL54" t="s">
         <v>319</v>
       </c>
-      <c r="AL54" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AL55" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2815,13 +2812,13 @@
       <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2898,7 +2895,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2939,7 +2936,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -2947,16 +2944,16 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q3" t="s">
         <v>95</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -2986,22 +2983,22 @@
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3060,7 +3057,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>121</v>
@@ -3090,7 +3087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3135,7 +3132,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3147,24 +3144,24 @@
         <v>95</v>
       </c>
       <c r="V3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>66</v>
       </c>
       <c r="AB3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>274</v>
       </c>
       <c r="AB4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3188,23 +3185,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3245,7 +3242,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>22</v>
@@ -3272,7 +3269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>272</v>
       </c>
@@ -3310,10 +3307,10 @@
         <v>207</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3324,7 +3321,7 @@
         <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J3" t="s">
         <v>269</v>
@@ -3336,12 +3333,12 @@
         <v>271</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>211</v>
@@ -3365,9 +3362,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G5" t="s">
         <v>76</v>
@@ -3376,7 +3373,7 @@
         <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J5" t="s">
         <v>269</v>
@@ -3388,12 +3385,12 @@
         <v>271</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G6" t="s">
         <v>76</v>
@@ -3414,13 +3411,13 @@
         <v>207</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="24"/>
     </row>
   </sheetData>
@@ -3442,16 +3439,16 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" customWidth="1"/>
-    <col min="28" max="28" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3540,7 +3537,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3581,7 +3578,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -3604,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -3612,7 +3609,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>228</v>
       </c>
@@ -3623,7 +3620,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>230</v>
       </c>
@@ -3636,7 +3633,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3662,19 +3659,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -3709,7 +3706,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>272</v>
       </c>
@@ -3721,7 +3718,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>273</v>
       </c>
@@ -3733,7 +3730,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -3749,7 +3746,7 @@
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>274</v>
       </c>
@@ -3767,7 +3764,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>230</v>
       </c>
@@ -3778,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>274</v>
       </c>
@@ -3789,7 +3786,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -3803,7 +3800,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>64</v>
       </c>
@@ -3827,13 +3824,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3964,7 +3961,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4002,7 +3999,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -4023,7 +4020,7 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -4037,7 +4034,7 @@
       <c r="AG4" s="4"/>
       <c r="AM4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -4051,7 +4048,7 @@
       <c r="AG5" s="4"/>
       <c r="AM5" s="5"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -4064,7 +4061,7 @@
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -4079,7 +4076,7 @@
       <c r="Z7" s="2"/>
       <c r="AM7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>248</v>
       </c>
@@ -4094,7 +4091,7 @@
       <c r="Z8" s="2"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>250</v>
       </c>
@@ -4109,7 +4106,7 @@
       <c r="Z9" s="2"/>
       <c r="AM9" s="5"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E10" s="16"/>
       <c r="G10" s="16"/>
       <c r="P10" s="7"/>
@@ -4119,7 +4116,7 @@
       <c r="Z10" s="2"/>
       <c r="AU10" s="8"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="P11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
@@ -4136,16 +4133,16 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4249,7 +4246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -4279,13 +4276,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4293,7 +4290,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -4314,28 +4311,28 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4409,7 +4406,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -4460,7 +4457,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -4512,7 +4509,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -4566,7 +4563,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -4593,7 +4590,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4608,7 +4605,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4647,14 +4644,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4761,7 +4758,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4801,7 +4798,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4810,7 +4807,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4821,7 +4818,7 @@
       <c r="S4" s="4"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4834,7 +4831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4842,14 +4839,14 @@
       <c r="L6" s="2"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4860,7 +4857,7 @@
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="U8" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V8" s="5" t="s">
         <v>53</v>
@@ -4869,7 +4866,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4898,7 +4895,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -4930,7 +4927,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -4938,7 +4935,7 @@
         <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J11" t="s">
         <v>63</v>
@@ -4951,18 +4948,18 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>64</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -4991,7 +4988,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -5018,12 +5015,12 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>92</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>66</v>
@@ -5032,7 +5029,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -5040,7 +5037,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>193</v>
       </c>
@@ -5048,7 +5045,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>195</v>
       </c>
@@ -5056,7 +5053,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
     </row>
@@ -5074,25 +5071,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5172,7 +5169,7 @@
         <v>94</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5205,7 +5202,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5254,7 +5251,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5266,7 +5263,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5278,7 +5275,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5292,7 +5289,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5308,7 +5305,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -5324,7 +5321,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5337,9 +5334,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -5348,12 +5345,12 @@
         <v>257</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -5362,15 +5359,15 @@
         <v>257</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>53</v>
@@ -5382,7 +5379,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5401,7 +5398,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5418,12 +5415,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>301</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>303</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>69</v>
@@ -5435,7 +5432,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5445,7 +5442,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5456,7 +5453,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="U16" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>53</v>
@@ -5468,7 +5465,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5478,7 +5475,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -5513,7 +5510,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>144</v>
       </c>
@@ -5548,7 +5545,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -5556,7 +5553,7 @@
         <v>238</v>
       </c>
       <c r="I20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J20" t="s">
         <v>63</v>
@@ -5572,12 +5569,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>64</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>66</v>
@@ -5586,7 +5583,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -5621,7 +5618,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -5653,7 +5650,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -5669,7 +5666,7 @@
         <v>83</v>
       </c>
       <c r="M24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N24" t="s">
         <v>258</v>
@@ -5699,9 +5696,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="7"/>
@@ -5711,10 +5708,10 @@
       <c r="H25" s="7"/>
       <c r="K25" s="2"/>
       <c r="M25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
@@ -5727,27 +5724,27 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>92</v>
       </c>
       <c r="X26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y26" s="5" t="s">
         <v>66</v>
       </c>
       <c r="Z26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AA26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AI26" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -5779,7 +5776,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -5789,7 +5786,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -5797,7 +5794,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -5811,7 +5808,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -5821,7 +5818,7 @@
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -5832,7 +5829,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>156</v>
       </c>
@@ -5843,7 +5840,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>159</v>
       </c>
@@ -5851,7 +5848,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -5859,18 +5856,18 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>170</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -5905,7 +5902,7 @@
         <v>888888</v>
       </c>
       <c r="U37" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V37" s="5" t="s">
         <v>183</v>
@@ -5917,7 +5914,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>217</v>
       </c>
@@ -5928,7 +5925,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>218</v>
       </c>
@@ -5939,12 +5936,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>320</v>
+      </c>
+      <c r="X40" s="24" t="s">
         <v>321</v>
-      </c>
-      <c r="X40" s="24" t="s">
-        <v>322</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>66</v>

</xml_diff>